<commit_message>
updated nz-au comparisons to 8 November
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C439CBC4-0447-AE4F-B66A-DF2E4C137020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E03A6-5CF6-2445-B18F-D9FC2F5DBB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{CC76B4D3-A05A-1747-A415-7F1BF9F8BF56}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{CC76B4D3-A05A-1747-A415-7F1BF9F8BF56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>date</t>
+    <t>second doses</t>
   </si>
   <si>
-    <t>second doses</t>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F03638-8190-9B46-9C3E-CA99D8A5449E}">
-  <dimension ref="A1:B227"/>
+  <dimension ref="A1:B232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,1801 +420,1844 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44503</v>
+        <v>44508</v>
       </c>
       <c r="B2" s="2">
-        <v>6077355</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44502</v>
+        <v>44507</v>
       </c>
       <c r="B3" s="2">
-        <v>6046074</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44501</v>
+        <v>44506</v>
       </c>
       <c r="B4" s="2">
-        <v>6009574</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44500</v>
+        <v>44505</v>
       </c>
       <c r="B5" s="2">
-        <v>5999926</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44499</v>
+        <v>44504</v>
       </c>
       <c r="B6" s="2">
-        <v>5977973</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44498</v>
+        <v>44503</v>
       </c>
       <c r="B7" s="2">
-        <v>5938861</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44497</v>
+        <v>44502</v>
       </c>
       <c r="B8" s="2">
-        <v>5898147</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44496</v>
+        <v>44501</v>
       </c>
       <c r="B9" s="2">
-        <v>5858123</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44495</v>
+        <v>44500</v>
       </c>
       <c r="B10" s="2">
-        <v>5818705</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44494</v>
+        <v>44499</v>
       </c>
       <c r="B11" s="2">
-        <v>5780737</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44493</v>
+        <v>44498</v>
       </c>
       <c r="B12" s="2">
-        <v>5766748</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44492</v>
+        <v>44497</v>
       </c>
       <c r="B13" s="2">
-        <v>5732872</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44491</v>
+        <v>44496</v>
       </c>
       <c r="B14" s="2">
-        <v>5677232</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>44490</v>
+        <v>44495</v>
       </c>
       <c r="B15" s="2">
-        <v>5621660</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44489</v>
+        <v>44494</v>
       </c>
       <c r="B16" s="2">
-        <v>5565441</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>44488</v>
+        <v>44493</v>
       </c>
       <c r="B17" s="2">
-        <v>5506563</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>44487</v>
+        <v>44492</v>
       </c>
       <c r="B18" s="2">
-        <v>5440365</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>44486</v>
+        <v>44491</v>
       </c>
       <c r="B19" s="2">
-        <v>5405628</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>44485</v>
+        <v>44490</v>
       </c>
       <c r="B20" s="2">
-        <v>5364911</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>44484</v>
+        <v>44489</v>
       </c>
       <c r="B21" s="2">
-        <v>5288225</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>44483</v>
+        <v>44488</v>
       </c>
       <c r="B22" s="2">
-        <v>5207377</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>44482</v>
+        <v>44487</v>
       </c>
       <c r="B23" s="2">
-        <v>5116994</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>44481</v>
+        <v>44486</v>
       </c>
       <c r="B24" s="2">
-        <v>5018535</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>44480</v>
+        <v>44485</v>
       </c>
       <c r="B25" s="2">
-        <v>4925635</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>44479</v>
+        <v>44484</v>
       </c>
       <c r="B26" s="2">
-        <v>4890800</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>44478</v>
+        <v>44483</v>
       </c>
       <c r="B27" s="2">
-        <v>4831173</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>44477</v>
+        <v>44482</v>
       </c>
       <c r="B28" s="2">
-        <v>4738793</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>44476</v>
+        <v>44481</v>
       </c>
       <c r="B29" s="2">
-        <v>4653723</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>44475</v>
+        <v>44480</v>
       </c>
       <c r="B30" s="2">
-        <v>4567214</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>44474</v>
+        <v>44479</v>
       </c>
       <c r="B31" s="2">
-        <v>4465060</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>44473</v>
+        <v>44478</v>
       </c>
       <c r="B32" s="2">
-        <v>4449546</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>44472</v>
+        <v>44477</v>
       </c>
       <c r="B33" s="2">
-        <v>4428121</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>44471</v>
+        <v>44476</v>
       </c>
       <c r="B34" s="2">
-        <v>4384051</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>44470</v>
+        <v>44475</v>
       </c>
       <c r="B35" s="2">
-        <v>4297900</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>44469</v>
+        <v>44474</v>
       </c>
       <c r="B36" s="2">
-        <v>4218516</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>44468</v>
+        <v>44473</v>
       </c>
       <c r="B37" s="2">
-        <v>4145673</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>44467</v>
+        <v>44472</v>
       </c>
       <c r="B38" s="2">
-        <v>4060612</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>44466</v>
+        <v>44471</v>
       </c>
       <c r="B39" s="2">
-        <v>3979094</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>44465</v>
+        <v>44470</v>
       </c>
       <c r="B40" s="2">
-        <v>3953132</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>44464</v>
+        <v>44469</v>
       </c>
       <c r="B41" s="2">
-        <v>3898564</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>44463</v>
+        <v>44468</v>
       </c>
       <c r="B42" s="2">
-        <v>3804258</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>44462</v>
+        <v>44467</v>
       </c>
       <c r="B43" s="2">
-        <v>3724979</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>44461</v>
+        <v>44466</v>
       </c>
       <c r="B44" s="2">
-        <v>3646849</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>44460</v>
+        <v>44465</v>
       </c>
       <c r="B45" s="2">
-        <v>3563962</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>44459</v>
+        <v>44464</v>
       </c>
       <c r="B46" s="2">
-        <v>3487539</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>44458</v>
+        <v>44463</v>
       </c>
       <c r="B47" s="2">
-        <v>3461082</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>44457</v>
+        <v>44462</v>
       </c>
       <c r="B48" s="2">
-        <v>3412016</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>44456</v>
+        <v>44461</v>
       </c>
       <c r="B49" s="2">
-        <v>3323936</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>44455</v>
+        <v>44460</v>
       </c>
       <c r="B50" s="2">
-        <v>3259323</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>44454</v>
+        <v>44459</v>
       </c>
       <c r="B51" s="2">
-        <v>3189070</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>44453</v>
+        <v>44458</v>
       </c>
       <c r="B52" s="2">
-        <v>3123699</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>44452</v>
+        <v>44457</v>
       </c>
       <c r="B53" s="2">
-        <v>3051925</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>44451</v>
+        <v>44456</v>
       </c>
       <c r="B54" s="2">
-        <v>3031072</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>44450</v>
+        <v>44455</v>
       </c>
       <c r="B55" s="2">
-        <v>2992899</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>44449</v>
+        <v>44454</v>
       </c>
       <c r="B56" s="2">
-        <v>2924263</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>44448</v>
+        <v>44453</v>
       </c>
       <c r="B57" s="2">
-        <v>2860253</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>44447</v>
+        <v>44452</v>
       </c>
       <c r="B58" s="2">
-        <v>2802011</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>44446</v>
+        <v>44451</v>
       </c>
       <c r="B59" s="2">
-        <v>2743498</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>44445</v>
+        <v>44450</v>
       </c>
       <c r="B60" s="2">
-        <v>2692904</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>44444</v>
+        <v>44449</v>
       </c>
       <c r="B61" s="2">
-        <v>2678906</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>44443</v>
+        <v>44448</v>
       </c>
       <c r="B62" s="2">
-        <v>2644865</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>44442</v>
+        <v>44447</v>
       </c>
       <c r="B63" s="2">
-        <v>2590966</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>44441</v>
+        <v>44446</v>
       </c>
       <c r="B64" s="2">
-        <v>2539287</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>44440</v>
+        <v>44445</v>
       </c>
       <c r="B65" s="2">
-        <v>2484199</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>44439</v>
+        <v>44444</v>
       </c>
       <c r="B66" s="2">
-        <v>2433592</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>44438</v>
+        <v>44443</v>
       </c>
       <c r="B67" s="2">
-        <v>2372417</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>44437</v>
+        <v>44442</v>
       </c>
       <c r="B68" s="2">
-        <v>2353563</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>44436</v>
+        <v>44441</v>
       </c>
       <c r="B69" s="2">
-        <v>2326130</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>44435</v>
+        <v>44440</v>
       </c>
       <c r="B70" s="2">
-        <v>2273984</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>44434</v>
+        <v>44439</v>
       </c>
       <c r="B71" s="2">
-        <v>2218458</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>44433</v>
+        <v>44438</v>
       </c>
       <c r="B72" s="2">
-        <v>2163192</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>44432</v>
+        <v>44437</v>
       </c>
       <c r="B73" s="2">
-        <v>2112611</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>44431</v>
+        <v>44436</v>
       </c>
       <c r="B74" s="2">
-        <v>2066915</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>44430</v>
+        <v>44435</v>
       </c>
       <c r="B75" s="2">
-        <v>2052364</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>44429</v>
+        <v>44434</v>
       </c>
       <c r="B76" s="2">
-        <v>2022928</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>44428</v>
+        <v>44433</v>
       </c>
       <c r="B77" s="2">
-        <v>1973224</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>44427</v>
+        <v>44432</v>
       </c>
       <c r="B78" s="2">
-        <v>1924839</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>44426</v>
+        <v>44431</v>
       </c>
       <c r="B79" s="2">
-        <v>1871458</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>44425</v>
+        <v>44430</v>
       </c>
       <c r="B80" s="2">
-        <v>1826165</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>44424</v>
+        <v>44429</v>
       </c>
       <c r="B81" s="2">
-        <v>1781578</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>44423</v>
+        <v>44428</v>
       </c>
       <c r="B82" s="2">
-        <v>1767176</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>44422</v>
+        <v>44427</v>
       </c>
       <c r="B83" s="2">
-        <v>1742669</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>44421</v>
+        <v>44426</v>
       </c>
       <c r="B84" s="2">
-        <v>1693577</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>44420</v>
+        <v>44425</v>
       </c>
       <c r="B85" s="2">
-        <v>1645077</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>44419</v>
+        <v>44424</v>
       </c>
       <c r="B86" s="2">
-        <v>1599438</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>44418</v>
+        <v>44423</v>
       </c>
       <c r="B87" s="2">
-        <v>1548545</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>44417</v>
+        <v>44422</v>
       </c>
       <c r="B88" s="2">
-        <v>1510648</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>44416</v>
+        <v>44421</v>
       </c>
       <c r="B89" s="2">
-        <v>1501249</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>44415</v>
+        <v>44420</v>
       </c>
       <c r="B90" s="2">
-        <v>1463495</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>44414</v>
+        <v>44419</v>
       </c>
       <c r="B91" s="2">
-        <v>1423185</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>44413</v>
+        <v>44418</v>
       </c>
       <c r="B92" s="2">
-        <v>1381481</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>44412</v>
+        <v>44417</v>
       </c>
       <c r="B93" s="2">
-        <v>1342211</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>44411</v>
+        <v>44416</v>
       </c>
       <c r="B94" s="2">
-        <v>1300394</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>44410</v>
+        <v>44415</v>
       </c>
       <c r="B95" s="2">
-        <v>1265839</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>44409</v>
+        <v>44414</v>
       </c>
       <c r="B96" s="2">
-        <v>1252304</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>44408</v>
+        <v>44413</v>
       </c>
       <c r="B97" s="2">
-        <v>1228845</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>44407</v>
+        <v>44412</v>
       </c>
       <c r="B98" s="2">
-        <v>1190942</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>44406</v>
+        <v>44411</v>
       </c>
       <c r="B99" s="2">
-        <v>1156321</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>44405</v>
+        <v>44410</v>
       </c>
       <c r="B100" s="2">
-        <v>1108405</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>44404</v>
+        <v>44409</v>
       </c>
       <c r="B101" s="2">
-        <v>1071895</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>44403</v>
+        <v>44408</v>
       </c>
       <c r="B102" s="2">
-        <v>1045515</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>44402</v>
+        <v>44407</v>
       </c>
       <c r="B103" s="2">
-        <v>1034280</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>44401</v>
+        <v>44406</v>
       </c>
       <c r="B104" s="2">
-        <v>1012939</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>44400</v>
+        <v>44405</v>
       </c>
       <c r="B105" s="2">
-        <v>982170</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>44399</v>
+        <v>44404</v>
       </c>
       <c r="B106" s="2">
-        <v>948667</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>44398</v>
+        <v>44403</v>
       </c>
       <c r="B107" s="2">
-        <v>912940</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>44397</v>
+        <v>44402</v>
       </c>
       <c r="B108" s="2">
-        <v>882844</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>44396</v>
+        <v>44401</v>
       </c>
       <c r="B109" s="2">
-        <v>854625</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>44395</v>
+        <v>44400</v>
       </c>
       <c r="B110" s="2">
-        <v>846261</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>44394</v>
+        <v>44399</v>
       </c>
       <c r="B111" s="2">
-        <v>830856</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>44393</v>
+        <v>44398</v>
       </c>
       <c r="B112" s="2">
-        <v>801520</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>44392</v>
+        <v>44397</v>
       </c>
       <c r="B113" s="2">
-        <v>769552</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>44391</v>
+        <v>44396</v>
       </c>
       <c r="B114" s="2">
-        <v>741075</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>44390</v>
+        <v>44395</v>
       </c>
       <c r="B115" s="2">
-        <v>710714</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>44389</v>
+        <v>44394</v>
       </c>
       <c r="B116" s="2">
-        <v>686408</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>44388</v>
+        <v>44393</v>
       </c>
       <c r="B117" s="2">
-        <v>683667</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>44387</v>
+        <v>44392</v>
       </c>
       <c r="B118" s="2">
-        <v>671858</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>44386</v>
+        <v>44391</v>
       </c>
       <c r="B119" s="2">
-        <v>651446</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>44385</v>
+        <v>44390</v>
       </c>
       <c r="B120" s="2">
-        <v>629961</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>44384</v>
+        <v>44389</v>
       </c>
       <c r="B121" s="2">
-        <v>609108</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>44383</v>
+        <v>44388</v>
       </c>
       <c r="B122" s="2">
-        <v>586674</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>44382</v>
+        <v>44387</v>
       </c>
       <c r="B123" s="2">
-        <v>567316</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>44381</v>
+        <v>44386</v>
       </c>
       <c r="B124" s="2">
-        <v>564930</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>44380</v>
+        <v>44385</v>
       </c>
       <c r="B125" s="2">
-        <v>554057</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>44379</v>
+        <v>44384</v>
       </c>
       <c r="B126" s="2">
-        <v>534493</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>44378</v>
+        <v>44383</v>
       </c>
       <c r="B127" s="2">
-        <v>471176</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>44377</v>
+        <v>44382</v>
       </c>
       <c r="B128" s="2">
-        <v>471176</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>44376</v>
+        <v>44381</v>
       </c>
       <c r="B129" s="2">
-        <v>463624</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>44375</v>
+        <v>44380</v>
       </c>
       <c r="B130" s="2">
-        <v>396652</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>44374</v>
+        <v>44379</v>
       </c>
       <c r="B131" s="2">
-        <v>396246</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>44373</v>
+        <v>44378</v>
       </c>
       <c r="B132" s="2">
-        <v>392527</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>44372</v>
+        <v>44377</v>
       </c>
       <c r="B133" s="2">
-        <v>385092</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>44371</v>
+        <v>44376</v>
       </c>
       <c r="B134" s="2">
-        <v>376276</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>44370</v>
+        <v>44375</v>
       </c>
       <c r="B135" s="2">
-        <v>366660</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>44369</v>
+        <v>44374</v>
       </c>
       <c r="B136" s="2">
-        <v>357767</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>44368</v>
+        <v>44373</v>
       </c>
       <c r="B137" s="2">
-        <v>294981</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>44367</v>
+        <v>44372</v>
       </c>
       <c r="B138" s="2">
-        <v>294965</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>44366</v>
+        <v>44371</v>
       </c>
       <c r="B139" s="2">
-        <v>289941</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>44365</v>
+        <v>44370</v>
       </c>
       <c r="B140" s="2">
-        <v>279418</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>44364</v>
+        <v>44369</v>
       </c>
       <c r="B141" s="2">
-        <v>269824</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>44363</v>
+        <v>44368</v>
       </c>
       <c r="B142" s="2">
-        <v>259437</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>44362</v>
+        <v>44367</v>
       </c>
       <c r="B143" s="2">
-        <v>237250</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>44361</v>
+        <v>44366</v>
       </c>
       <c r="B144" s="2">
-        <v>237250</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>44360</v>
+        <v>44365</v>
       </c>
       <c r="B145" s="2">
-        <v>237250</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>44359</v>
+        <v>44364</v>
       </c>
       <c r="B146" s="2">
-        <v>232335</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>44358</v>
+        <v>44363</v>
       </c>
       <c r="B147" s="2">
-        <v>222807</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>44357</v>
+        <v>44362</v>
       </c>
       <c r="B148" s="2">
-        <v>213686</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>44356</v>
+        <v>44361</v>
       </c>
       <c r="B149" s="2">
-        <v>213686</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>44355</v>
+        <v>44360</v>
       </c>
       <c r="B150" s="2">
-        <v>204595</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>44354</v>
+        <v>44359</v>
       </c>
       <c r="B151" s="2">
-        <v>180397</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>44353</v>
+        <v>44358</v>
       </c>
       <c r="B152" s="2">
-        <v>180397</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>44352</v>
+        <v>44357</v>
       </c>
       <c r="B153" s="2">
-        <v>179477</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>44351</v>
+        <v>44356</v>
       </c>
       <c r="B154" s="2">
-        <v>175030</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>44350</v>
+        <v>44355</v>
       </c>
       <c r="B155" s="2">
-        <v>170669</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>44349</v>
+        <v>44354</v>
       </c>
       <c r="B156" s="2">
-        <v>167075</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>44348</v>
+        <v>44353</v>
       </c>
       <c r="B157" s="2">
-        <v>156333</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>44347</v>
+        <v>44352</v>
       </c>
       <c r="B158" s="2">
-        <v>153886</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>44346</v>
+        <v>44351</v>
       </c>
       <c r="B159" s="2">
-        <v>153886</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>44345</v>
+        <v>44350</v>
       </c>
       <c r="B160" s="2">
-        <v>153886</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>44344</v>
+        <v>44349</v>
       </c>
       <c r="B161" s="2">
-        <v>153886</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>44343</v>
+        <v>44348</v>
       </c>
       <c r="B162" s="2">
-        <v>150552</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>44342</v>
+        <v>44347</v>
       </c>
       <c r="B163" s="2">
-        <v>145341</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>44341</v>
+        <v>44346</v>
       </c>
       <c r="B164" s="2">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>44340</v>
+        <v>44345</v>
       </c>
       <c r="B165" s="2">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>44339</v>
+        <v>44344</v>
       </c>
       <c r="B166" s="2">
-        <v>96745</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>44338</v>
+        <v>44343</v>
       </c>
       <c r="B167" s="2">
-        <v>96266</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>44337</v>
+        <v>44342</v>
       </c>
       <c r="B168" s="2">
-        <v>93860</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>44336</v>
+        <v>44341</v>
       </c>
       <c r="B169" s="2">
-        <v>91297</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>44335</v>
+        <v>44340</v>
       </c>
       <c r="B170" s="2">
-        <v>89049</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>44334</v>
+        <v>44339</v>
       </c>
       <c r="B171" s="2">
-        <v>87045</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>44333</v>
+        <v>44338</v>
       </c>
       <c r="B172" s="2">
-        <v>84963</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>44332</v>
+        <v>44337</v>
       </c>
       <c r="B173" s="2">
-        <v>84963</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>44331</v>
+        <v>44336</v>
       </c>
       <c r="B174" s="2">
-        <v>84474</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>44330</v>
+        <v>44335</v>
       </c>
       <c r="B175" s="2">
-        <v>82774</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>44329</v>
+        <v>44334</v>
       </c>
       <c r="B176" s="2">
-        <v>81457</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>44328</v>
+        <v>44333</v>
       </c>
       <c r="B177" s="2">
-        <v>80082</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>44327</v>
+        <v>44332</v>
       </c>
       <c r="B178" s="2">
-        <v>78744</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>44326</v>
+        <v>44331</v>
       </c>
       <c r="B179" s="2">
-        <v>77392</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>44325</v>
+        <v>44330</v>
       </c>
       <c r="B180" s="2">
-        <v>77392</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>44324</v>
+        <v>44329</v>
       </c>
       <c r="B181" s="2">
-        <v>76908</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>44323</v>
+        <v>44328</v>
       </c>
       <c r="B182" s="2">
-        <v>75187</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>44322</v>
+        <v>44327</v>
       </c>
       <c r="B183" s="2">
-        <v>73270</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>44321</v>
+        <v>44326</v>
       </c>
       <c r="B184" s="2">
-        <v>71767</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>44320</v>
+        <v>44325</v>
       </c>
       <c r="B185" s="2">
-        <v>70039</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>44319</v>
+        <v>44324</v>
       </c>
       <c r="B186" s="2">
-        <v>68656</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>44318</v>
+        <v>44323</v>
       </c>
       <c r="B187" s="2">
-        <v>68656</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>44317</v>
+        <v>44322</v>
       </c>
       <c r="B188" s="2">
-        <v>68472</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B189" s="2">
-        <v>67149</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>44315</v>
+        <v>44320</v>
       </c>
       <c r="B190" s="2">
-        <v>65948</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>44314</v>
+        <v>44319</v>
       </c>
       <c r="B191" s="2">
-        <v>64910</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>44313</v>
+        <v>44318</v>
       </c>
       <c r="B192" s="2">
-        <v>63944</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>44312</v>
+        <v>44317</v>
       </c>
       <c r="B193" s="2">
-        <v>63537</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>44311</v>
+        <v>44316</v>
       </c>
       <c r="B194" s="2">
-        <v>63537</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>44310</v>
+        <v>44315</v>
       </c>
       <c r="B195" s="2">
-        <v>63317</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>44309</v>
+        <v>44314</v>
       </c>
       <c r="B196" s="2">
-        <v>62491</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>44308</v>
+        <v>44313</v>
       </c>
       <c r="B197" s="2">
-        <v>60582</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>44307</v>
+        <v>44312</v>
       </c>
       <c r="B198" s="2">
-        <v>58662</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>44306</v>
+        <v>44311</v>
       </c>
       <c r="B199" s="2">
-        <v>54736</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>44305</v>
+        <v>44310</v>
       </c>
       <c r="B200" s="2">
-        <v>54668</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>44304</v>
+        <v>44309</v>
       </c>
       <c r="B201" s="2">
-        <v>54668</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>44303</v>
+        <v>44308</v>
       </c>
       <c r="B202" s="2">
-        <v>54555</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>44302</v>
+        <v>44307</v>
       </c>
       <c r="B203" s="2">
-        <v>52537</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>44301</v>
+        <v>44306</v>
       </c>
       <c r="B204" s="2">
-        <v>50388</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>44300</v>
+        <v>44305</v>
       </c>
       <c r="B205" s="2">
-        <v>48482</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>44299</v>
+        <v>44304</v>
       </c>
       <c r="B206" s="2">
-        <v>46400</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>44298</v>
+        <v>44303</v>
       </c>
       <c r="B207" s="2">
-        <v>44208</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>44297</v>
+        <v>44302</v>
       </c>
       <c r="B208" s="2">
-        <v>44208</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>44296</v>
+        <v>44301</v>
       </c>
       <c r="B209" s="2">
-        <v>44016</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>44295</v>
+        <v>44300</v>
       </c>
       <c r="B210" s="2">
-        <v>41376</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>44294</v>
+        <v>44299</v>
       </c>
       <c r="B211" s="2">
-        <v>38445</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>44293</v>
+        <v>44298</v>
       </c>
       <c r="B212" s="2">
-        <v>35475</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>44292</v>
+        <v>44297</v>
       </c>
       <c r="B213" s="2">
-        <v>31795</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>44291</v>
+        <v>44296</v>
       </c>
       <c r="B214" s="2">
-        <v>31212</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>44290</v>
+        <v>44295</v>
       </c>
       <c r="B215" s="2">
-        <v>31212</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>44289</v>
+        <v>44294</v>
       </c>
       <c r="B216" s="2">
-        <v>30383</v>
+        <v>38445</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>44288</v>
+        <v>44293</v>
       </c>
       <c r="B217" s="2">
-        <v>29796</v>
+        <v>35475</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>44287</v>
-      </c>
-      <c r="B218" s="3"/>
+        <v>44292</v>
+      </c>
+      <c r="B218" s="2">
+        <v>31795</v>
+      </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>44286</v>
-      </c>
-      <c r="B219" s="3"/>
+        <v>44291</v>
+      </c>
+      <c r="B219" s="2">
+        <v>31212</v>
+      </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>44285</v>
-      </c>
-      <c r="B220" s="3"/>
+        <v>44290</v>
+      </c>
+      <c r="B220" s="2">
+        <v>31212</v>
+      </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>44284</v>
-      </c>
-      <c r="B221" s="3"/>
+        <v>44289</v>
+      </c>
+      <c r="B221" s="2">
+        <v>30383</v>
+      </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>44283</v>
-      </c>
-      <c r="B222" s="3"/>
+        <v>44288</v>
+      </c>
+      <c r="B222" s="2">
+        <v>29796</v>
+      </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>44282</v>
+        <v>44287</v>
       </c>
       <c r="B223" s="3"/>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>44281</v>
+        <v>44286</v>
       </c>
       <c r="B224" s="3"/>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>44280</v>
+        <v>44285</v>
       </c>
       <c r="B225" s="3"/>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>44279</v>
+        <v>44284</v>
       </c>
       <c r="B226" s="3"/>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
+        <v>44283</v>
+      </c>
+      <c r="B227" s="3"/>
+    </row>
+    <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>44282</v>
+      </c>
+      <c r="B228" s="3"/>
+    </row>
+    <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>44281</v>
+      </c>
+      <c r="B229" s="3"/>
+    </row>
+    <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>44280</v>
+      </c>
+      <c r="B230" s="3"/>
+    </row>
+    <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>44279</v>
+      </c>
+      <c r="B231" s="3"/>
+    </row>
+    <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
         <v>44278</v>
       </c>
-      <c r="B227" s="3"/>
+      <c r="B232" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{11F02C1F-9B72-5E45-857D-BA94EFE24064}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated NZ vs NSW/VIC comparisons to 16 November
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588E03A6-5CF6-2445-B18F-D9FC2F5DBB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A36CFE52-2052-AC47-9E18-07E917223C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{CC76B4D3-A05A-1747-A415-7F1BF9F8BF56}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{10D8DC41-9BF2-5648-B173-A5B29921ADE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>second doses</t>
+    <t>DATE</t>
   </si>
   <si>
-    <t>DATE</t>
+    <t>Second Doses</t>
   </si>
 </sst>
 </file>
@@ -405,11 +405,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F03638-8190-9B46-9C3E-CA99D8A5449E}">
-  <dimension ref="A1:B232"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE69A6C-8A50-8D49-89FB-0214725D1725}">
+  <dimension ref="A1:B239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,1843 +420,1899 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44508</v>
+        <v>44515</v>
       </c>
       <c r="B2" s="2">
-        <v>6172372</v>
+        <v>6268391</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44507</v>
+        <v>44514</v>
       </c>
       <c r="B3" s="2">
-        <v>6168060</v>
+        <v>6265758</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44506</v>
+        <v>44513</v>
       </c>
       <c r="B4" s="2">
-        <v>6156414</v>
+        <v>6259089</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44505</v>
+        <v>44512</v>
       </c>
       <c r="B5" s="2">
-        <v>6130474</v>
+        <v>6243318</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44504</v>
+        <v>44511</v>
       </c>
       <c r="B6" s="2">
-        <v>6105744</v>
+        <v>6226830</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>44503</v>
+        <v>44510</v>
       </c>
       <c r="B7" s="2">
-        <v>6077355</v>
+        <v>6210103</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>44502</v>
+        <v>44509</v>
       </c>
       <c r="B8" s="2">
-        <v>6046074</v>
+        <v>6192099</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>44501</v>
+        <v>44508</v>
       </c>
       <c r="B9" s="2">
-        <v>6009574</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>44500</v>
+        <v>44507</v>
       </c>
       <c r="B10" s="2">
-        <v>5999926</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>44499</v>
+        <v>44506</v>
       </c>
       <c r="B11" s="2">
-        <v>5977973</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>44498</v>
+        <v>44505</v>
       </c>
       <c r="B12" s="2">
-        <v>5938861</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>44497</v>
+        <v>44504</v>
       </c>
       <c r="B13" s="2">
-        <v>5898147</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>44496</v>
+        <v>44503</v>
       </c>
       <c r="B14" s="2">
-        <v>5858123</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>44495</v>
+        <v>44502</v>
       </c>
       <c r="B15" s="2">
-        <v>5818705</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>44494</v>
+        <v>44501</v>
       </c>
       <c r="B16" s="2">
-        <v>5780737</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>44493</v>
+        <v>44500</v>
       </c>
       <c r="B17" s="2">
-        <v>5766748</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>44492</v>
+        <v>44499</v>
       </c>
       <c r="B18" s="2">
-        <v>5732872</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>44491</v>
+        <v>44498</v>
       </c>
       <c r="B19" s="2">
-        <v>5677232</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>44490</v>
+        <v>44497</v>
       </c>
       <c r="B20" s="2">
-        <v>5621660</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="B21" s="2">
-        <v>5565441</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>44488</v>
+        <v>44495</v>
       </c>
       <c r="B22" s="2">
-        <v>5506563</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>44487</v>
+        <v>44494</v>
       </c>
       <c r="B23" s="2">
-        <v>5440365</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>44486</v>
+        <v>44493</v>
       </c>
       <c r="B24" s="2">
-        <v>5405628</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B25" s="2">
-        <v>5364911</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>44484</v>
+        <v>44491</v>
       </c>
       <c r="B26" s="2">
-        <v>5288225</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>44483</v>
+        <v>44490</v>
       </c>
       <c r="B27" s="2">
-        <v>5207377</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>44482</v>
+        <v>44489</v>
       </c>
       <c r="B28" s="2">
-        <v>5116994</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>44481</v>
+        <v>44488</v>
       </c>
       <c r="B29" s="2">
-        <v>5018535</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>44480</v>
+        <v>44487</v>
       </c>
       <c r="B30" s="2">
-        <v>4925635</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>44479</v>
+        <v>44486</v>
       </c>
       <c r="B31" s="2">
-        <v>4890800</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B32" s="2">
-        <v>4831173</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>44477</v>
+        <v>44484</v>
       </c>
       <c r="B33" s="2">
-        <v>4738793</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>44476</v>
+        <v>44483</v>
       </c>
       <c r="B34" s="2">
-        <v>4653723</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>44475</v>
+        <v>44482</v>
       </c>
       <c r="B35" s="2">
-        <v>4567214</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>44474</v>
+        <v>44481</v>
       </c>
       <c r="B36" s="2">
-        <v>4465060</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>44473</v>
+        <v>44480</v>
       </c>
       <c r="B37" s="2">
-        <v>4449546</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>44472</v>
+        <v>44479</v>
       </c>
       <c r="B38" s="2">
-        <v>4428121</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>44471</v>
+        <v>44478</v>
       </c>
       <c r="B39" s="2">
-        <v>4384051</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>44470</v>
+        <v>44477</v>
       </c>
       <c r="B40" s="2">
-        <v>4297900</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>44469</v>
+        <v>44476</v>
       </c>
       <c r="B41" s="2">
-        <v>4218516</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>44468</v>
+        <v>44475</v>
       </c>
       <c r="B42" s="2">
-        <v>4145673</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>44467</v>
+        <v>44474</v>
       </c>
       <c r="B43" s="2">
-        <v>4060612</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>44466</v>
+        <v>44473</v>
       </c>
       <c r="B44" s="2">
-        <v>3979094</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>44465</v>
+        <v>44472</v>
       </c>
       <c r="B45" s="2">
-        <v>3953132</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B46" s="2">
-        <v>3898564</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>44463</v>
+        <v>44470</v>
       </c>
       <c r="B47" s="2">
-        <v>3804258</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>44462</v>
+        <v>44469</v>
       </c>
       <c r="B48" s="2">
-        <v>3724979</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>44461</v>
+        <v>44468</v>
       </c>
       <c r="B49" s="2">
-        <v>3646849</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>44460</v>
+        <v>44467</v>
       </c>
       <c r="B50" s="2">
-        <v>3563962</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>44459</v>
+        <v>44466</v>
       </c>
       <c r="B51" s="2">
-        <v>3487539</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>44458</v>
+        <v>44465</v>
       </c>
       <c r="B52" s="2">
-        <v>3461082</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B53" s="2">
-        <v>3412016</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>44456</v>
+        <v>44463</v>
       </c>
       <c r="B54" s="2">
-        <v>3323936</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>44455</v>
+        <v>44462</v>
       </c>
       <c r="B55" s="2">
-        <v>3259323</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B56" s="2">
-        <v>3189070</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>44453</v>
+        <v>44460</v>
       </c>
       <c r="B57" s="2">
-        <v>3123699</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>44452</v>
+        <v>44459</v>
       </c>
       <c r="B58" s="2">
-        <v>3051925</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>44451</v>
+        <v>44458</v>
       </c>
       <c r="B59" s="2">
-        <v>3031072</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B60" s="2">
-        <v>2992899</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>44449</v>
+        <v>44456</v>
       </c>
       <c r="B61" s="2">
-        <v>2924263</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>44448</v>
+        <v>44455</v>
       </c>
       <c r="B62" s="2">
-        <v>2860253</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>44447</v>
+        <v>44454</v>
       </c>
       <c r="B63" s="2">
-        <v>2802011</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>44446</v>
+        <v>44453</v>
       </c>
       <c r="B64" s="2">
-        <v>2743498</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>44445</v>
+        <v>44452</v>
       </c>
       <c r="B65" s="2">
-        <v>2692904</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>44444</v>
+        <v>44451</v>
       </c>
       <c r="B66" s="2">
-        <v>2678906</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>44443</v>
+        <v>44450</v>
       </c>
       <c r="B67" s="2">
-        <v>2644865</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>44442</v>
+        <v>44449</v>
       </c>
       <c r="B68" s="2">
-        <v>2590966</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>44441</v>
+        <v>44448</v>
       </c>
       <c r="B69" s="2">
-        <v>2539287</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>44440</v>
+        <v>44447</v>
       </c>
       <c r="B70" s="2">
-        <v>2484199</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>44439</v>
+        <v>44446</v>
       </c>
       <c r="B71" s="2">
-        <v>2433592</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>44438</v>
+        <v>44445</v>
       </c>
       <c r="B72" s="2">
-        <v>2372417</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>44437</v>
+        <v>44444</v>
       </c>
       <c r="B73" s="2">
-        <v>2353563</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>44436</v>
+        <v>44443</v>
       </c>
       <c r="B74" s="2">
-        <v>2326130</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>44435</v>
+        <v>44442</v>
       </c>
       <c r="B75" s="2">
-        <v>2273984</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>44434</v>
+        <v>44441</v>
       </c>
       <c r="B76" s="2">
-        <v>2218458</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>44433</v>
+        <v>44440</v>
       </c>
       <c r="B77" s="2">
-        <v>2163192</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>44432</v>
+        <v>44439</v>
       </c>
       <c r="B78" s="2">
-        <v>2112611</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>44431</v>
+        <v>44438</v>
       </c>
       <c r="B79" s="2">
-        <v>2066915</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>44430</v>
+        <v>44437</v>
       </c>
       <c r="B80" s="2">
-        <v>2052364</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>44429</v>
+        <v>44436</v>
       </c>
       <c r="B81" s="2">
-        <v>2022928</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>44428</v>
+        <v>44435</v>
       </c>
       <c r="B82" s="2">
-        <v>1973224</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>44427</v>
+        <v>44434</v>
       </c>
       <c r="B83" s="2">
-        <v>1924839</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>44426</v>
+        <v>44433</v>
       </c>
       <c r="B84" s="2">
-        <v>1871458</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>44425</v>
+        <v>44432</v>
       </c>
       <c r="B85" s="2">
-        <v>1826165</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>44424</v>
+        <v>44431</v>
       </c>
       <c r="B86" s="2">
-        <v>1781578</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>44423</v>
+        <v>44430</v>
       </c>
       <c r="B87" s="2">
-        <v>1767176</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="B88" s="2">
-        <v>1742669</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>44421</v>
+        <v>44428</v>
       </c>
       <c r="B89" s="2">
-        <v>1693577</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>44420</v>
+        <v>44427</v>
       </c>
       <c r="B90" s="2">
-        <v>1645077</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="B91" s="2">
-        <v>1599438</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>44418</v>
+        <v>44425</v>
       </c>
       <c r="B92" s="2">
-        <v>1548545</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>44417</v>
+        <v>44424</v>
       </c>
       <c r="B93" s="2">
-        <v>1510648</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>44416</v>
+        <v>44423</v>
       </c>
       <c r="B94" s="2">
-        <v>1501249</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>44415</v>
+        <v>44422</v>
       </c>
       <c r="B95" s="2">
-        <v>1463495</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>44414</v>
+        <v>44421</v>
       </c>
       <c r="B96" s="2">
-        <v>1423185</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>44413</v>
+        <v>44420</v>
       </c>
       <c r="B97" s="2">
-        <v>1381481</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>44412</v>
+        <v>44419</v>
       </c>
       <c r="B98" s="2">
-        <v>1342211</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>44411</v>
+        <v>44418</v>
       </c>
       <c r="B99" s="2">
-        <v>1300394</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>44410</v>
+        <v>44417</v>
       </c>
       <c r="B100" s="2">
-        <v>1265839</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>44409</v>
+        <v>44416</v>
       </c>
       <c r="B101" s="2">
-        <v>1252304</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>44408</v>
+        <v>44415</v>
       </c>
       <c r="B102" s="2">
-        <v>1228845</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>44407</v>
+        <v>44414</v>
       </c>
       <c r="B103" s="2">
-        <v>1190942</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>44406</v>
+        <v>44413</v>
       </c>
       <c r="B104" s="2">
-        <v>1156321</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>44405</v>
+        <v>44412</v>
       </c>
       <c r="B105" s="2">
-        <v>1108405</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>44404</v>
+        <v>44411</v>
       </c>
       <c r="B106" s="2">
-        <v>1071895</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>44403</v>
+        <v>44410</v>
       </c>
       <c r="B107" s="2">
-        <v>1045515</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>44402</v>
+        <v>44409</v>
       </c>
       <c r="B108" s="2">
-        <v>1034280</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>44401</v>
+        <v>44408</v>
       </c>
       <c r="B109" s="2">
-        <v>1012939</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>44400</v>
+        <v>44407</v>
       </c>
       <c r="B110" s="2">
-        <v>982170</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>44399</v>
+        <v>44406</v>
       </c>
       <c r="B111" s="2">
-        <v>948667</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>44398</v>
+        <v>44405</v>
       </c>
       <c r="B112" s="2">
-        <v>912940</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>44397</v>
+        <v>44404</v>
       </c>
       <c r="B113" s="2">
-        <v>882844</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>44396</v>
+        <v>44403</v>
       </c>
       <c r="B114" s="2">
-        <v>854625</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>44395</v>
+        <v>44402</v>
       </c>
       <c r="B115" s="2">
-        <v>846261</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>44394</v>
+        <v>44401</v>
       </c>
       <c r="B116" s="2">
-        <v>830856</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="B117" s="2">
-        <v>801520</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>44392</v>
+        <v>44399</v>
       </c>
       <c r="B118" s="2">
-        <v>769552</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>44391</v>
+        <v>44398</v>
       </c>
       <c r="B119" s="2">
-        <v>741075</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>44390</v>
+        <v>44397</v>
       </c>
       <c r="B120" s="2">
-        <v>710714</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>44389</v>
+        <v>44396</v>
       </c>
       <c r="B121" s="2">
-        <v>686408</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>44388</v>
+        <v>44395</v>
       </c>
       <c r="B122" s="2">
-        <v>683667</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>44387</v>
+        <v>44394</v>
       </c>
       <c r="B123" s="2">
-        <v>671858</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>44386</v>
+        <v>44393</v>
       </c>
       <c r="B124" s="2">
-        <v>651446</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>44385</v>
+        <v>44392</v>
       </c>
       <c r="B125" s="2">
-        <v>629961</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>44384</v>
+        <v>44391</v>
       </c>
       <c r="B126" s="2">
-        <v>609108</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>44383</v>
+        <v>44390</v>
       </c>
       <c r="B127" s="2">
-        <v>586674</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>44382</v>
+        <v>44389</v>
       </c>
       <c r="B128" s="2">
-        <v>567316</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>44381</v>
+        <v>44388</v>
       </c>
       <c r="B129" s="2">
-        <v>564930</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>44380</v>
+        <v>44387</v>
       </c>
       <c r="B130" s="2">
-        <v>554057</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>44379</v>
+        <v>44386</v>
       </c>
       <c r="B131" s="2">
-        <v>534493</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>44378</v>
+        <v>44385</v>
       </c>
       <c r="B132" s="2">
-        <v>471176</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>44377</v>
+        <v>44384</v>
       </c>
       <c r="B133" s="2">
-        <v>471176</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>44376</v>
+        <v>44383</v>
       </c>
       <c r="B134" s="2">
-        <v>463624</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>44375</v>
+        <v>44382</v>
       </c>
       <c r="B135" s="2">
-        <v>396652</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>44374</v>
+        <v>44381</v>
       </c>
       <c r="B136" s="2">
-        <v>396246</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>44373</v>
+        <v>44380</v>
       </c>
       <c r="B137" s="2">
-        <v>392527</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>44372</v>
+        <v>44379</v>
       </c>
       <c r="B138" s="2">
-        <v>385092</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>44371</v>
+        <v>44378</v>
       </c>
       <c r="B139" s="2">
-        <v>376276</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>44370</v>
+        <v>44377</v>
       </c>
       <c r="B140" s="2">
-        <v>366660</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>44369</v>
+        <v>44376</v>
       </c>
       <c r="B141" s="2">
-        <v>357767</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="B142" s="2">
-        <v>294981</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>44367</v>
+        <v>44374</v>
       </c>
       <c r="B143" s="2">
-        <v>294965</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>44366</v>
+        <v>44373</v>
       </c>
       <c r="B144" s="2">
-        <v>289941</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>44365</v>
+        <v>44372</v>
       </c>
       <c r="B145" s="2">
-        <v>279418</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>44364</v>
+        <v>44371</v>
       </c>
       <c r="B146" s="2">
-        <v>269824</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>44363</v>
+        <v>44370</v>
       </c>
       <c r="B147" s="2">
-        <v>259437</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>44362</v>
+        <v>44369</v>
       </c>
       <c r="B148" s="2">
-        <v>237250</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>44361</v>
+        <v>44368</v>
       </c>
       <c r="B149" s="2">
-        <v>237250</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>44360</v>
+        <v>44367</v>
       </c>
       <c r="B150" s="2">
-        <v>237250</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>44359</v>
+        <v>44366</v>
       </c>
       <c r="B151" s="2">
-        <v>232335</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>44358</v>
+        <v>44365</v>
       </c>
       <c r="B152" s="2">
-        <v>222807</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>44357</v>
+        <v>44364</v>
       </c>
       <c r="B153" s="2">
-        <v>213686</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>44356</v>
+        <v>44363</v>
       </c>
       <c r="B154" s="2">
-        <v>213686</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>44355</v>
+        <v>44362</v>
       </c>
       <c r="B155" s="2">
-        <v>204595</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>44354</v>
+        <v>44361</v>
       </c>
       <c r="B156" s="2">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>44353</v>
+        <v>44360</v>
       </c>
       <c r="B157" s="2">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>44352</v>
+        <v>44359</v>
       </c>
       <c r="B158" s="2">
-        <v>179477</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>44351</v>
+        <v>44358</v>
       </c>
       <c r="B159" s="2">
-        <v>175030</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>44350</v>
+        <v>44357</v>
       </c>
       <c r="B160" s="2">
-        <v>170669</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>44349</v>
+        <v>44356</v>
       </c>
       <c r="B161" s="2">
-        <v>167075</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>44348</v>
+        <v>44355</v>
       </c>
       <c r="B162" s="2">
-        <v>156333</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>44347</v>
+        <v>44354</v>
       </c>
       <c r="B163" s="2">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>44346</v>
+        <v>44353</v>
       </c>
       <c r="B164" s="2">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B165" s="2">
-        <v>153886</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B166" s="2">
-        <v>153886</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B167" s="2">
-        <v>150552</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B168" s="2">
-        <v>145341</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B169" s="2">
-        <v>125810</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B170" s="2">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>44339</v>
+        <v>44346</v>
       </c>
       <c r="B171" s="2">
-        <v>96745</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>44338</v>
+        <v>44345</v>
       </c>
       <c r="B172" s="2">
-        <v>96266</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>44337</v>
+        <v>44344</v>
       </c>
       <c r="B173" s="2">
-        <v>93860</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>44336</v>
+        <v>44343</v>
       </c>
       <c r="B174" s="2">
-        <v>91297</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>44335</v>
+        <v>44342</v>
       </c>
       <c r="B175" s="2">
-        <v>89049</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>44334</v>
+        <v>44341</v>
       </c>
       <c r="B176" s="2">
-        <v>87045</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>44333</v>
+        <v>44340</v>
       </c>
       <c r="B177" s="2">
-        <v>84963</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>44332</v>
+        <v>44339</v>
       </c>
       <c r="B178" s="2">
-        <v>84963</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>44331</v>
+        <v>44338</v>
       </c>
       <c r="B179" s="2">
-        <v>84474</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>44330</v>
+        <v>44337</v>
       </c>
       <c r="B180" s="2">
-        <v>82774</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>44329</v>
+        <v>44336</v>
       </c>
       <c r="B181" s="2">
-        <v>81457</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>44328</v>
+        <v>44335</v>
       </c>
       <c r="B182" s="2">
-        <v>80082</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>44327</v>
+        <v>44334</v>
       </c>
       <c r="B183" s="2">
-        <v>78744</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>44326</v>
+        <v>44333</v>
       </c>
       <c r="B184" s="2">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>44325</v>
+        <v>44332</v>
       </c>
       <c r="B185" s="2">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B186" s="2">
-        <v>76908</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B187" s="2">
-        <v>75187</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>44322</v>
+        <v>44329</v>
       </c>
       <c r="B188" s="2">
-        <v>73270</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B189" s="2">
-        <v>71767</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B190" s="2">
-        <v>70039</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B191" s="2">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>44318</v>
+        <v>44325</v>
       </c>
       <c r="B192" s="2">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>44317</v>
+        <v>44324</v>
       </c>
       <c r="B193" s="2">
-        <v>68472</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="B194" s="2">
-        <v>67149</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>44315</v>
+        <v>44322</v>
       </c>
       <c r="B195" s="2">
-        <v>65948</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>44314</v>
+        <v>44321</v>
       </c>
       <c r="B196" s="2">
-        <v>64910</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>44313</v>
+        <v>44320</v>
       </c>
       <c r="B197" s="2">
-        <v>63944</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>44312</v>
+        <v>44319</v>
       </c>
       <c r="B198" s="2">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>44311</v>
+        <v>44318</v>
       </c>
       <c r="B199" s="2">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>44310</v>
+        <v>44317</v>
       </c>
       <c r="B200" s="2">
-        <v>63317</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>44309</v>
+        <v>44316</v>
       </c>
       <c r="B201" s="2">
-        <v>62491</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>44308</v>
+        <v>44315</v>
       </c>
       <c r="B202" s="2">
-        <v>60582</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>44307</v>
+        <v>44314</v>
       </c>
       <c r="B203" s="2">
-        <v>58662</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>44306</v>
+        <v>44313</v>
       </c>
       <c r="B204" s="2">
-        <v>54736</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="B205" s="2">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>44304</v>
+        <v>44311</v>
       </c>
       <c r="B206" s="2">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>44303</v>
+        <v>44310</v>
       </c>
       <c r="B207" s="2">
-        <v>54555</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>44302</v>
+        <v>44309</v>
       </c>
       <c r="B208" s="2">
-        <v>52537</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="B209" s="2">
-        <v>50388</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>44300</v>
+        <v>44307</v>
       </c>
       <c r="B210" s="2">
-        <v>48482</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>44299</v>
+        <v>44306</v>
       </c>
       <c r="B211" s="2">
-        <v>46400</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>44298</v>
+        <v>44305</v>
       </c>
       <c r="B212" s="2">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>44297</v>
+        <v>44304</v>
       </c>
       <c r="B213" s="2">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>44296</v>
+        <v>44303</v>
       </c>
       <c r="B214" s="2">
-        <v>44016</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>44295</v>
+        <v>44302</v>
       </c>
       <c r="B215" s="2">
-        <v>41376</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>44294</v>
+        <v>44301</v>
       </c>
       <c r="B216" s="2">
-        <v>38445</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>44293</v>
+        <v>44300</v>
       </c>
       <c r="B217" s="2">
-        <v>35475</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>44292</v>
+        <v>44299</v>
       </c>
       <c r="B218" s="2">
-        <v>31795</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>44291</v>
+        <v>44298</v>
       </c>
       <c r="B219" s="2">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>44290</v>
+        <v>44297</v>
       </c>
       <c r="B220" s="2">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>44289</v>
+        <v>44296</v>
       </c>
       <c r="B221" s="2">
-        <v>30383</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>44288</v>
+        <v>44295</v>
       </c>
       <c r="B222" s="2">
-        <v>29796</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>44287</v>
-      </c>
-      <c r="B223" s="3"/>
+        <v>44294</v>
+      </c>
+      <c r="B223" s="2">
+        <v>38445</v>
+      </c>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>44286</v>
-      </c>
-      <c r="B224" s="3"/>
+        <v>44293</v>
+      </c>
+      <c r="B224" s="2">
+        <v>35475</v>
+      </c>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>44285</v>
-      </c>
-      <c r="B225" s="3"/>
+        <v>44292</v>
+      </c>
+      <c r="B225" s="2">
+        <v>31795</v>
+      </c>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>44284</v>
-      </c>
-      <c r="B226" s="3"/>
+        <v>44291</v>
+      </c>
+      <c r="B226" s="2">
+        <v>31212</v>
+      </c>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
-        <v>44283</v>
-      </c>
-      <c r="B227" s="3"/>
+        <v>44290</v>
+      </c>
+      <c r="B227" s="2">
+        <v>31212</v>
+      </c>
     </row>
     <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
-        <v>44282</v>
-      </c>
-      <c r="B228" s="3"/>
+        <v>44289</v>
+      </c>
+      <c r="B228" s="2">
+        <v>30383</v>
+      </c>
     </row>
     <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
-        <v>44281</v>
-      </c>
-      <c r="B229" s="3"/>
+        <v>44288</v>
+      </c>
+      <c r="B229" s="2">
+        <v>29796</v>
+      </c>
     </row>
     <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
-        <v>44280</v>
+        <v>44287</v>
       </c>
       <c r="B230" s="3"/>
     </row>
     <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
-        <v>44279</v>
+        <v>44286</v>
       </c>
       <c r="B231" s="3"/>
     </row>
     <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
+        <v>44285</v>
+      </c>
+      <c r="B232" s="3"/>
+    </row>
+    <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>44284</v>
+      </c>
+      <c r="B233" s="3"/>
+    </row>
+    <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>44283</v>
+      </c>
+      <c r="B234" s="3"/>
+    </row>
+    <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A235" s="1">
+        <v>44282</v>
+      </c>
+      <c r="B235" s="3"/>
+    </row>
+    <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>44281</v>
+      </c>
+      <c r="B236" s="3"/>
+    </row>
+    <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>44280</v>
+      </c>
+      <c r="B237" s="3"/>
+    </row>
+    <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>44279</v>
+      </c>
+      <c r="B238" s="3"/>
+    </row>
+    <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
         <v>44278</v>
       </c>
-      <c r="B232" s="3"/>
+      <c r="B239" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{11F02C1F-9B72-5E45-857D-BA94EFE24064}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{23B490A8-2899-3544-8AAF-209C836DA81E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated NZ-AU comparison to 23 November
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A36CFE52-2052-AC47-9E18-07E917223C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44C96804-F63E-D847-BBB1-A4510560FE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{10D8DC41-9BF2-5648-B173-A5B29921ADE1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8009A520-03D6-BF45-99E7-24F606287CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,14 +39,14 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>Second Doses</t>
+    <t>second doses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -63,6 +63,20 @@
     <font>
       <sz val="14.4"/>
       <color rgb="FF779DB4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -84,16 +98,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,11 +423,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE69A6C-8A50-8D49-89FB-0214725D1725}">
-  <dimension ref="A1:B239"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CC4C5E-AB23-574B-B919-1D3C72CAF21C}">
+  <dimension ref="A1:B246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -419,1900 +437,1956 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
+        <v>44522</v>
+      </c>
+      <c r="B2" s="3">
+        <v>6325341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>44521</v>
+      </c>
+      <c r="B3" s="3">
+        <v>6324333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44520</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6320582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44519</v>
+      </c>
+      <c r="B5" s="3">
+        <v>6311361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44518</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6301870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>44517</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6291057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>44516</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6279967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>44515</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B9" s="3">
         <v>6268391</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>44514</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B10" s="3">
         <v>6265758</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
         <v>44513</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B11" s="3">
         <v>6259089</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>44512</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B12" s="3">
         <v>6243318</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>44511</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B13" s="3">
         <v>6226830</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
         <v>44510</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B14" s="3">
         <v>6210103</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>44509</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B15" s="3">
         <v>6192099</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>44508</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B16" s="3">
         <v>6172372</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>44507</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B17" s="3">
         <v>6168060</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>44506</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B18" s="3">
         <v>6156414</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>44505</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B19" s="3">
         <v>6130474</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>44504</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B20" s="3">
         <v>6105744</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>44503</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B21" s="3">
         <v>6077355</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>44502</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B22" s="3">
         <v>6046074</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>44501</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B23" s="3">
         <v>6009574</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>44500</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B24" s="3">
         <v>5999926</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>44499</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B25" s="3">
         <v>5977973</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>44498</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B26" s="3">
         <v>5938861</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>44497</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B27" s="3">
         <v>5898147</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>44496</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B28" s="3">
         <v>5858123</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>44495</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B29" s="3">
         <v>5818705</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+    <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>44494</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B30" s="3">
         <v>5780737</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+    <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
         <v>44493</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B31" s="3">
         <v>5766748</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+    <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>44492</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B32" s="3">
         <v>5732872</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>44491</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B33" s="3">
         <v>5677232</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+    <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>44490</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B34" s="3">
         <v>5621660</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>44489</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B35" s="3">
         <v>5565441</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>44488</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B36" s="3">
         <v>5506563</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
         <v>44487</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B37" s="3">
         <v>5440365</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
         <v>44486</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B38" s="3">
         <v>5405628</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>44485</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B39" s="3">
         <v>5364911</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>44484</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B40" s="3">
         <v>5288225</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>44483</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B41" s="3">
         <v>5207377</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>44482</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B42" s="3">
         <v>5116994</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>44481</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B43" s="3">
         <v>5018535</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <v>44480</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B44" s="3">
         <v>4925635</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>44479</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B45" s="3">
         <v>4890800</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <v>44478</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B46" s="3">
         <v>4831173</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+    <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
         <v>44477</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B47" s="3">
         <v>4738793</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
         <v>44476</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B48" s="3">
         <v>4653723</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
+    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
         <v>44475</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B49" s="3">
         <v>4567214</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
+    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
         <v>44474</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B50" s="3">
         <v>4465060</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
         <v>44473</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B51" s="3">
         <v>4449546</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
         <v>44472</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B52" s="3">
         <v>4428121</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
         <v>44471</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B53" s="3">
         <v>4384051</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
         <v>44470</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B54" s="3">
         <v>4297900</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
         <v>44469</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B55" s="3">
         <v>4218516</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
         <v>44468</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B56" s="3">
         <v>4145673</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
         <v>44467</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B57" s="3">
         <v>4060612</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
         <v>44466</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B58" s="3">
         <v>3979094</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
         <v>44465</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B59" s="3">
         <v>3953132</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
         <v>44464</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B60" s="3">
         <v>3898564</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
         <v>44463</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B61" s="3">
         <v>3804258</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
         <v>44462</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B62" s="3">
         <v>3724979</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
         <v>44461</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B63" s="3">
         <v>3646849</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
         <v>44460</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B64" s="3">
         <v>3563962</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
         <v>44459</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B65" s="3">
         <v>3487539</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
+    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
         <v>44458</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B66" s="3">
         <v>3461082</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
+    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
         <v>44457</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B67" s="3">
         <v>3412016</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
+    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
         <v>44456</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B68" s="3">
         <v>3323936</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
+    <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
         <v>44455</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B69" s="3">
         <v>3259323</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
+    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="2">
         <v>44454</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B70" s="3">
         <v>3189070</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
+    <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
         <v>44453</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B71" s="3">
         <v>3123699</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
+    <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
         <v>44452</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B72" s="3">
         <v>3051925</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="2">
         <v>44451</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B73" s="3">
         <v>3031072</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="2">
         <v>44450</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B74" s="3">
         <v>2992899</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="2">
         <v>44449</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B75" s="3">
         <v>2924263</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="2">
         <v>44448</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B76" s="3">
         <v>2860253</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
+    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="2">
         <v>44447</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B77" s="3">
         <v>2802011</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
+    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="2">
         <v>44446</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B78" s="3">
         <v>2743498</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
+    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="2">
         <v>44445</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B79" s="3">
         <v>2692904</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
+    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="2">
         <v>44444</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B80" s="3">
         <v>2678906</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
+    <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
         <v>44443</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B81" s="3">
         <v>2644865</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
+    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
         <v>44442</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B82" s="3">
         <v>2590966</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
+    <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="2">
         <v>44441</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B83" s="3">
         <v>2539287</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
+    <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
         <v>44440</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B84" s="3">
         <v>2484199</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
+    <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="2">
         <v>44439</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B85" s="3">
         <v>2433592</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
+    <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
         <v>44438</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B86" s="3">
         <v>2372417</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
+    <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
         <v>44437</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B87" s="3">
         <v>2353563</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
+    <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
         <v>44436</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B88" s="3">
         <v>2326130</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
+    <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
         <v>44435</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B89" s="3">
         <v>2273984</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A83" s="1">
+    <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
         <v>44434</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B90" s="3">
         <v>2218458</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A84" s="1">
+    <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
         <v>44433</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B91" s="3">
         <v>2163192</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A85" s="1">
+    <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
         <v>44432</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B92" s="3">
         <v>2112611</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A86" s="1">
+    <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
         <v>44431</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B93" s="3">
         <v>2066915</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A87" s="1">
+    <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
         <v>44430</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B94" s="3">
         <v>2052364</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A88" s="1">
+    <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
         <v>44429</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B95" s="3">
         <v>2022928</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A89" s="1">
+    <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
         <v>44428</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B96" s="3">
         <v>1973224</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A90" s="1">
+    <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
         <v>44427</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B97" s="3">
         <v>1924839</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A91" s="1">
+    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
         <v>44426</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B98" s="3">
         <v>1871458</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
+    <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
         <v>44425</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B99" s="3">
         <v>1826165</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A93" s="1">
+    <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
         <v>44424</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B100" s="3">
         <v>1781578</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A94" s="1">
+    <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
         <v>44423</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B101" s="3">
         <v>1767176</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A95" s="1">
+    <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
         <v>44422</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B102" s="3">
         <v>1742669</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
+    <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
         <v>44421</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B103" s="3">
         <v>1693577</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A97" s="1">
+    <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
         <v>44420</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B104" s="3">
         <v>1645077</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A98" s="1">
+    <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
         <v>44419</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B105" s="3">
         <v>1599438</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
+    <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
         <v>44418</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B106" s="3">
         <v>1548545</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A100" s="1">
+    <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
         <v>44417</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B107" s="3">
         <v>1510648</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A101" s="1">
+    <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
         <v>44416</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B108" s="3">
         <v>1501249</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A102" s="1">
+    <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
         <v>44415</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B109" s="3">
         <v>1463495</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A103" s="1">
+    <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
         <v>44414</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B110" s="3">
         <v>1423185</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A104" s="1">
+    <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
         <v>44413</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B111" s="3">
         <v>1381481</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A105" s="1">
+    <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
         <v>44412</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B112" s="3">
         <v>1342211</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A106" s="1">
+    <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
         <v>44411</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B113" s="3">
         <v>1300394</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A107" s="1">
+    <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
         <v>44410</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B114" s="3">
         <v>1265839</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A108" s="1">
+    <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
         <v>44409</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B115" s="3">
         <v>1252304</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A109" s="1">
+    <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
         <v>44408</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B116" s="3">
         <v>1228845</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A110" s="1">
+    <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
         <v>44407</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B117" s="3">
         <v>1190942</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A111" s="1">
+    <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
         <v>44406</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B118" s="3">
         <v>1156321</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A112" s="1">
+    <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
         <v>44405</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B119" s="3">
         <v>1108405</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A113" s="1">
+    <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
         <v>44404</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B120" s="3">
         <v>1071895</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A114" s="1">
+    <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
         <v>44403</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B121" s="3">
         <v>1045515</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A115" s="1">
+    <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
         <v>44402</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B122" s="3">
         <v>1034280</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A116" s="1">
+    <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
         <v>44401</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B123" s="3">
         <v>1012939</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A117" s="1">
+    <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
         <v>44400</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B124" s="3">
         <v>982170</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A118" s="1">
+    <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
         <v>44399</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B125" s="3">
         <v>948667</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A119" s="1">
+    <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
         <v>44398</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B126" s="3">
         <v>912940</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A120" s="1">
+    <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A127" s="2">
         <v>44397</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B127" s="3">
         <v>882844</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A121" s="1">
+    <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A128" s="2">
         <v>44396</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B128" s="3">
         <v>854625</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A122" s="1">
+    <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A129" s="2">
         <v>44395</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B129" s="3">
         <v>846261</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A123" s="1">
+    <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
         <v>44394</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B130" s="3">
         <v>830856</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A124" s="1">
+    <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A131" s="2">
         <v>44393</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B131" s="3">
         <v>801520</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A125" s="1">
+    <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A132" s="2">
         <v>44392</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B132" s="3">
         <v>769552</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A126" s="1">
+    <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A133" s="2">
         <v>44391</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B133" s="3">
         <v>741075</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A127" s="1">
+    <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A134" s="2">
         <v>44390</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B134" s="3">
         <v>710714</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A128" s="1">
+    <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A135" s="2">
         <v>44389</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B135" s="3">
         <v>686408</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A129" s="1">
+    <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A136" s="2">
         <v>44388</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B136" s="3">
         <v>683667</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A130" s="1">
+    <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
         <v>44387</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B137" s="3">
         <v>671858</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A131" s="1">
+    <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A138" s="2">
         <v>44386</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B138" s="3">
         <v>651446</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A132" s="1">
+    <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A139" s="2">
         <v>44385</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B139" s="3">
         <v>629961</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A133" s="1">
+    <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A140" s="2">
         <v>44384</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B140" s="3">
         <v>609108</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A134" s="1">
+    <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A141" s="2">
         <v>44383</v>
       </c>
-      <c r="B134" s="2">
+      <c r="B141" s="3">
         <v>586674</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A135" s="1">
+    <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A142" s="2">
         <v>44382</v>
       </c>
-      <c r="B135" s="2">
+      <c r="B142" s="3">
         <v>567316</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A136" s="1">
+    <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A143" s="2">
         <v>44381</v>
       </c>
-      <c r="B136" s="2">
+      <c r="B143" s="3">
         <v>564930</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A137" s="1">
+    <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A144" s="2">
         <v>44380</v>
       </c>
-      <c r="B137" s="2">
+      <c r="B144" s="3">
         <v>554057</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A138" s="1">
+    <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A145" s="2">
         <v>44379</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B145" s="3">
         <v>534493</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A139" s="1">
+    <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A146" s="2">
         <v>44378</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B146" s="3">
         <v>471176</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A140" s="1">
+    <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A147" s="2">
         <v>44377</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B147" s="3">
         <v>471176</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A141" s="1">
+    <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A148" s="2">
         <v>44376</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B148" s="3">
         <v>463624</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A142" s="1">
+    <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A149" s="2">
         <v>44375</v>
       </c>
-      <c r="B142" s="2">
+      <c r="B149" s="3">
         <v>396652</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A143" s="1">
+    <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A150" s="2">
         <v>44374</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B150" s="3">
         <v>396246</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A144" s="1">
+    <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
         <v>44373</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B151" s="3">
         <v>392527</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A145" s="1">
+    <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A152" s="2">
         <v>44372</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B152" s="3">
         <v>385092</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A146" s="1">
+    <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A153" s="2">
         <v>44371</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B153" s="3">
         <v>376276</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A147" s="1">
+    <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A154" s="2">
         <v>44370</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B154" s="3">
         <v>366660</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A148" s="1">
+    <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A155" s="2">
         <v>44369</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B155" s="3">
         <v>357767</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A149" s="1">
+    <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A156" s="2">
         <v>44368</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B156" s="3">
         <v>294981</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A150" s="1">
+    <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A157" s="2">
         <v>44367</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B157" s="3">
         <v>294965</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A151" s="1">
+    <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A158" s="2">
         <v>44366</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B158" s="3">
         <v>289941</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A152" s="1">
+    <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A159" s="2">
         <v>44365</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B159" s="3">
         <v>279418</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A153" s="1">
+    <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A160" s="2">
         <v>44364</v>
       </c>
-      <c r="B153" s="2">
+      <c r="B160" s="3">
         <v>269824</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A154" s="1">
+    <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A161" s="2">
         <v>44363</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B161" s="3">
         <v>259437</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A155" s="1">
+    <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A162" s="2">
         <v>44362</v>
       </c>
-      <c r="B155" s="2">
+      <c r="B162" s="3">
         <v>237250</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A156" s="1">
+    <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A163" s="2">
         <v>44361</v>
       </c>
-      <c r="B156" s="2">
+      <c r="B163" s="3">
         <v>237250</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A157" s="1">
+    <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A164" s="2">
         <v>44360</v>
       </c>
-      <c r="B157" s="2">
+      <c r="B164" s="3">
         <v>237250</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A158" s="1">
+    <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
         <v>44359</v>
       </c>
-      <c r="B158" s="2">
+      <c r="B165" s="3">
         <v>232335</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A159" s="1">
+    <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
         <v>44358</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B166" s="3">
         <v>222807</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A160" s="1">
+    <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
         <v>44357</v>
       </c>
-      <c r="B160" s="2">
+      <c r="B167" s="3">
         <v>213686</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A161" s="1">
+    <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
         <v>44356</v>
       </c>
-      <c r="B161" s="2">
+      <c r="B168" s="3">
         <v>213686</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A162" s="1">
+    <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
         <v>44355</v>
       </c>
-      <c r="B162" s="2">
+      <c r="B169" s="3">
         <v>204595</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A163" s="1">
+    <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
         <v>44354</v>
       </c>
-      <c r="B163" s="2">
+      <c r="B170" s="3">
         <v>180397</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A164" s="1">
+    <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
         <v>44353</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B171" s="3">
         <v>180397</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A165" s="1">
+    <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
         <v>44352</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B172" s="3">
         <v>179477</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A166" s="1">
+    <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
         <v>44351</v>
       </c>
-      <c r="B166" s="2">
+      <c r="B173" s="3">
         <v>175030</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A167" s="1">
+    <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
         <v>44350</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B174" s="3">
         <v>170669</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A168" s="1">
+    <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
         <v>44349</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B175" s="3">
         <v>167075</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A169" s="1">
+    <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
         <v>44348</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B176" s="3">
         <v>156333</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A170" s="1">
+    <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
         <v>44347</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B177" s="3">
         <v>153886</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A171" s="1">
+    <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
         <v>44346</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B178" s="3">
         <v>153886</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A172" s="1">
+    <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
         <v>44345</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B179" s="3">
         <v>153886</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A173" s="1">
+    <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
         <v>44344</v>
       </c>
-      <c r="B173" s="2">
+      <c r="B180" s="3">
         <v>153886</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A174" s="1">
+    <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
         <v>44343</v>
       </c>
-      <c r="B174" s="2">
+      <c r="B181" s="3">
         <v>150552</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A175" s="1">
+    <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
         <v>44342</v>
       </c>
-      <c r="B175" s="2">
+      <c r="B182" s="3">
         <v>145341</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A176" s="1">
+    <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
         <v>44341</v>
       </c>
-      <c r="B176" s="2">
+      <c r="B183" s="3">
         <v>125810</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A177" s="1">
+    <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
         <v>44340</v>
       </c>
-      <c r="B177" s="2">
+      <c r="B184" s="3">
         <v>125810</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A178" s="1">
+    <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
         <v>44339</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B185" s="3">
         <v>96745</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A179" s="1">
+    <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
         <v>44338</v>
       </c>
-      <c r="B179" s="2">
+      <c r="B186" s="3">
         <v>96266</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A180" s="1">
+    <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
         <v>44337</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B187" s="3">
         <v>93860</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A181" s="1">
+    <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
         <v>44336</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B188" s="3">
         <v>91297</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A182" s="1">
+    <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
         <v>44335</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B189" s="3">
         <v>89049</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A183" s="1">
+    <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
         <v>44334</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B190" s="3">
         <v>87045</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A184" s="1">
+    <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
         <v>44333</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B191" s="3">
         <v>84963</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A185" s="1">
+    <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
         <v>44332</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B192" s="3">
         <v>84963</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A186" s="1">
+    <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A193" s="2">
         <v>44331</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B193" s="3">
         <v>84474</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A187" s="1">
+    <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A194" s="2">
         <v>44330</v>
       </c>
-      <c r="B187" s="2">
+      <c r="B194" s="3">
         <v>82774</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A188" s="1">
+    <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A195" s="2">
         <v>44329</v>
       </c>
-      <c r="B188" s="2">
+      <c r="B195" s="3">
         <v>81457</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A189" s="1">
+    <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A196" s="2">
         <v>44328</v>
       </c>
-      <c r="B189" s="2">
+      <c r="B196" s="3">
         <v>80082</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A190" s="1">
+    <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A197" s="2">
         <v>44327</v>
       </c>
-      <c r="B190" s="2">
+      <c r="B197" s="3">
         <v>78744</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A191" s="1">
+    <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A198" s="2">
         <v>44326</v>
       </c>
-      <c r="B191" s="2">
+      <c r="B198" s="3">
         <v>77392</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A192" s="1">
+    <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A199" s="2">
         <v>44325</v>
       </c>
-      <c r="B192" s="2">
+      <c r="B199" s="3">
         <v>77392</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A193" s="1">
+    <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A200" s="2">
         <v>44324</v>
       </c>
-      <c r="B193" s="2">
+      <c r="B200" s="3">
         <v>76908</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A194" s="1">
+    <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A201" s="2">
         <v>44323</v>
       </c>
-      <c r="B194" s="2">
+      <c r="B201" s="3">
         <v>75187</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A195" s="1">
+    <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A202" s="2">
         <v>44322</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B202" s="3">
         <v>73270</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A196" s="1">
+    <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A203" s="2">
         <v>44321</v>
       </c>
-      <c r="B196" s="2">
+      <c r="B203" s="3">
         <v>71767</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A197" s="1">
+    <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A204" s="2">
         <v>44320</v>
       </c>
-      <c r="B197" s="2">
+      <c r="B204" s="3">
         <v>70039</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A198" s="1">
+    <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A205" s="2">
         <v>44319</v>
       </c>
-      <c r="B198" s="2">
+      <c r="B205" s="3">
         <v>68656</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A199" s="1">
+    <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A206" s="2">
         <v>44318</v>
       </c>
-      <c r="B199" s="2">
+      <c r="B206" s="3">
         <v>68656</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A200" s="1">
+    <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A207" s="2">
         <v>44317</v>
       </c>
-      <c r="B200" s="2">
+      <c r="B207" s="3">
         <v>68472</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A201" s="1">
+    <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A208" s="2">
         <v>44316</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B208" s="3">
         <v>67149</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A202" s="1">
+    <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A209" s="2">
         <v>44315</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B209" s="3">
         <v>65948</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A203" s="1">
+    <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A210" s="2">
         <v>44314</v>
       </c>
-      <c r="B203" s="2">
+      <c r="B210" s="3">
         <v>64910</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A204" s="1">
+    <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
         <v>44313</v>
       </c>
-      <c r="B204" s="2">
+      <c r="B211" s="3">
         <v>63944</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A205" s="1">
+    <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A212" s="2">
         <v>44312</v>
       </c>
-      <c r="B205" s="2">
+      <c r="B212" s="3">
         <v>63537</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A206" s="1">
+    <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A213" s="2">
         <v>44311</v>
       </c>
-      <c r="B206" s="2">
+      <c r="B213" s="3">
         <v>63537</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A207" s="1">
+    <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A214" s="2">
         <v>44310</v>
       </c>
-      <c r="B207" s="2">
+      <c r="B214" s="3">
         <v>63317</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A208" s="1">
+    <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A215" s="2">
         <v>44309</v>
       </c>
-      <c r="B208" s="2">
+      <c r="B215" s="3">
         <v>62491</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A209" s="1">
+    <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A216" s="2">
         <v>44308</v>
       </c>
-      <c r="B209" s="2">
+      <c r="B216" s="3">
         <v>60582</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A210" s="1">
+    <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A217" s="2">
         <v>44307</v>
       </c>
-      <c r="B210" s="2">
+      <c r="B217" s="3">
         <v>58662</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A211" s="1">
+    <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A218" s="2">
         <v>44306</v>
       </c>
-      <c r="B211" s="2">
+      <c r="B218" s="3">
         <v>54736</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A212" s="1">
+    <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A219" s="2">
         <v>44305</v>
       </c>
-      <c r="B212" s="2">
+      <c r="B219" s="3">
         <v>54668</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A213" s="1">
+    <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
         <v>44304</v>
       </c>
-      <c r="B213" s="2">
+      <c r="B220" s="3">
         <v>54668</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A214" s="1">
+    <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
         <v>44303</v>
       </c>
-      <c r="B214" s="2">
+      <c r="B221" s="3">
         <v>54555</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A215" s="1">
+    <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
         <v>44302</v>
       </c>
-      <c r="B215" s="2">
+      <c r="B222" s="3">
         <v>52537</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A216" s="1">
+    <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
         <v>44301</v>
       </c>
-      <c r="B216" s="2">
+      <c r="B223" s="3">
         <v>50388</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A217" s="1">
+    <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
         <v>44300</v>
       </c>
-      <c r="B217" s="2">
+      <c r="B224" s="3">
         <v>48482</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A218" s="1">
+    <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
         <v>44299</v>
       </c>
-      <c r="B218" s="2">
+      <c r="B225" s="3">
         <v>46400</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A219" s="1">
+    <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
         <v>44298</v>
       </c>
-      <c r="B219" s="2">
+      <c r="B226" s="3">
         <v>44208</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A220" s="1">
+    <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
         <v>44297</v>
       </c>
-      <c r="B220" s="2">
+      <c r="B227" s="3">
         <v>44208</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A221" s="1">
+    <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A228" s="2">
         <v>44296</v>
       </c>
-      <c r="B221" s="2">
+      <c r="B228" s="3">
         <v>44016</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A222" s="1">
+    <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A229" s="2">
         <v>44295</v>
       </c>
-      <c r="B222" s="2">
+      <c r="B229" s="3">
         <v>41376</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A223" s="1">
+    <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A230" s="2">
         <v>44294</v>
       </c>
-      <c r="B223" s="2">
+      <c r="B230" s="3">
         <v>38445</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A224" s="1">
+    <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A231" s="2">
         <v>44293</v>
       </c>
-      <c r="B224" s="2">
+      <c r="B231" s="3">
         <v>35475</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A225" s="1">
+    <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A232" s="2">
         <v>44292</v>
       </c>
-      <c r="B225" s="2">
+      <c r="B232" s="3">
         <v>31795</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A226" s="1">
+    <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A233" s="2">
         <v>44291</v>
       </c>
-      <c r="B226" s="2">
+      <c r="B233" s="3">
         <v>31212</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A227" s="1">
+    <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A234" s="2">
         <v>44290</v>
       </c>
-      <c r="B227" s="2">
+      <c r="B234" s="3">
         <v>31212</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A228" s="1">
+    <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A235" s="2">
         <v>44289</v>
       </c>
-      <c r="B228" s="2">
+      <c r="B235" s="3">
         <v>30383</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A229" s="1">
+    <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A236" s="2">
         <v>44288</v>
       </c>
-      <c r="B229" s="2">
+      <c r="B236" s="3">
         <v>29796</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A230" s="1">
+    <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A237" s="2">
         <v>44287</v>
       </c>
-      <c r="B230" s="3"/>
-    </row>
-    <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A231" s="1">
+      <c r="B237" s="4"/>
+    </row>
+    <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A238" s="2">
         <v>44286</v>
       </c>
-      <c r="B231" s="3"/>
-    </row>
-    <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A232" s="1">
+      <c r="B238" s="4"/>
+    </row>
+    <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A239" s="2">
         <v>44285</v>
       </c>
-      <c r="B232" s="3"/>
-    </row>
-    <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A233" s="1">
+      <c r="B239" s="4"/>
+    </row>
+    <row r="240" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A240" s="2">
         <v>44284</v>
       </c>
-      <c r="B233" s="3"/>
-    </row>
-    <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A234" s="1">
+      <c r="B240" s="4"/>
+    </row>
+    <row r="241" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A241" s="2">
         <v>44283</v>
       </c>
-      <c r="B234" s="3"/>
-    </row>
-    <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A235" s="1">
+      <c r="B241" s="4"/>
+    </row>
+    <row r="242" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A242" s="2">
         <v>44282</v>
       </c>
-      <c r="B235" s="3"/>
-    </row>
-    <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A236" s="1">
+      <c r="B242" s="4"/>
+    </row>
+    <row r="243" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
         <v>44281</v>
       </c>
-      <c r="B236" s="3"/>
-    </row>
-    <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A237" s="1">
+      <c r="B243" s="4"/>
+    </row>
+    <row r="244" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A244" s="2">
         <v>44280</v>
       </c>
-      <c r="B237" s="3"/>
-    </row>
-    <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A238" s="1">
+      <c r="B244" s="4"/>
+    </row>
+    <row r="245" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A245" s="2">
         <v>44279</v>
       </c>
-      <c r="B238" s="3"/>
-    </row>
-    <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A239" s="1">
+      <c r="B245" s="4"/>
+    </row>
+    <row r="246" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A246" s="2">
         <v>44278</v>
       </c>
-      <c r="B239" s="3"/>
+      <c r="B246" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{23B490A8-2899-3544-8AAF-209C836DA81E}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{A7F15A82-DD8F-4D4A-B31F-57C09B82F350}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Trans-Tasman charts updated to 29 November
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44C96804-F63E-D847-BBB1-A4510560FE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82E83EA0-9021-8D46-8512-8321939065CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8009A520-03D6-BF45-99E7-24F606287CED}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,6 +77,7 @@
     <font>
       <b/>
       <sz val="9.6"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -423,11 +424,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CC4C5E-AB23-574B-B919-1D3C72CAF21C}">
-  <dimension ref="A1:B246"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BAE720-0FFD-AC44-A3E0-A012DA41F8A8}">
+  <dimension ref="A1:B253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,1947 +447,2003 @@
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44522</v>
+        <v>44529</v>
       </c>
       <c r="B2" s="3">
-        <v>6325341</v>
+        <v>6366060</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44521</v>
+        <v>44528</v>
       </c>
       <c r="B3" s="3">
-        <v>6324333</v>
+        <v>6365073</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44520</v>
+        <v>44527</v>
       </c>
       <c r="B4" s="3">
-        <v>6320582</v>
+        <v>6362348</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44519</v>
+        <v>44526</v>
       </c>
       <c r="B5" s="3">
-        <v>6311361</v>
+        <v>6355156</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44518</v>
+        <v>44525</v>
       </c>
       <c r="B6" s="3">
-        <v>6301870</v>
+        <v>6348980</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44517</v>
+        <v>44524</v>
       </c>
       <c r="B7" s="3">
-        <v>6291057</v>
+        <v>6341726</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44516</v>
+        <v>44523</v>
       </c>
       <c r="B8" s="3">
-        <v>6279967</v>
+        <v>6334061</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44515</v>
+        <v>44522</v>
       </c>
       <c r="B9" s="3">
-        <v>6268391</v>
+        <v>6325341</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44514</v>
+        <v>44521</v>
       </c>
       <c r="B10" s="3">
-        <v>6265758</v>
+        <v>6324333</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44513</v>
+        <v>44520</v>
       </c>
       <c r="B11" s="3">
-        <v>6259089</v>
+        <v>6320582</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44512</v>
+        <v>44519</v>
       </c>
       <c r="B12" s="3">
-        <v>6243318</v>
+        <v>6311361</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44511</v>
+        <v>44518</v>
       </c>
       <c r="B13" s="3">
-        <v>6226830</v>
+        <v>6301870</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="B14" s="3">
-        <v>6210103</v>
+        <v>6291057</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44509</v>
+        <v>44516</v>
       </c>
       <c r="B15" s="3">
-        <v>6192099</v>
+        <v>6279967</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44508</v>
+        <v>44515</v>
       </c>
       <c r="B16" s="3">
-        <v>6172372</v>
+        <v>6268391</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44507</v>
+        <v>44514</v>
       </c>
       <c r="B17" s="3">
-        <v>6168060</v>
+        <v>6265758</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44506</v>
+        <v>44513</v>
       </c>
       <c r="B18" s="3">
-        <v>6156414</v>
+        <v>6259089</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44505</v>
+        <v>44512</v>
       </c>
       <c r="B19" s="3">
-        <v>6130474</v>
+        <v>6243318</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>44504</v>
+        <v>44511</v>
       </c>
       <c r="B20" s="3">
-        <v>6105744</v>
+        <v>6226830</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44503</v>
+        <v>44510</v>
       </c>
       <c r="B21" s="3">
-        <v>6077355</v>
+        <v>6210103</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44502</v>
+        <v>44509</v>
       </c>
       <c r="B22" s="3">
-        <v>6046074</v>
+        <v>6192099</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44501</v>
+        <v>44508</v>
       </c>
       <c r="B23" s="3">
-        <v>6009574</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44500</v>
+        <v>44507</v>
       </c>
       <c r="B24" s="3">
-        <v>5999926</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44499</v>
+        <v>44506</v>
       </c>
       <c r="B25" s="3">
-        <v>5977973</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44498</v>
+        <v>44505</v>
       </c>
       <c r="B26" s="3">
-        <v>5938861</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44497</v>
+        <v>44504</v>
       </c>
       <c r="B27" s="3">
-        <v>5898147</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44496</v>
+        <v>44503</v>
       </c>
       <c r="B28" s="3">
-        <v>5858123</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44495</v>
+        <v>44502</v>
       </c>
       <c r="B29" s="3">
-        <v>5818705</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44494</v>
+        <v>44501</v>
       </c>
       <c r="B30" s="3">
-        <v>5780737</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44493</v>
+        <v>44500</v>
       </c>
       <c r="B31" s="3">
-        <v>5766748</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44492</v>
+        <v>44499</v>
       </c>
       <c r="B32" s="3">
-        <v>5732872</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44491</v>
+        <v>44498</v>
       </c>
       <c r="B33" s="3">
-        <v>5677232</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44490</v>
+        <v>44497</v>
       </c>
       <c r="B34" s="3">
-        <v>5621660</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="B35" s="3">
-        <v>5565441</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44488</v>
+        <v>44495</v>
       </c>
       <c r="B36" s="3">
-        <v>5506563</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44487</v>
+        <v>44494</v>
       </c>
       <c r="B37" s="3">
-        <v>5440365</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44486</v>
+        <v>44493</v>
       </c>
       <c r="B38" s="3">
-        <v>5405628</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B39" s="3">
-        <v>5364911</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44484</v>
+        <v>44491</v>
       </c>
       <c r="B40" s="3">
-        <v>5288225</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44483</v>
+        <v>44490</v>
       </c>
       <c r="B41" s="3">
-        <v>5207377</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44482</v>
+        <v>44489</v>
       </c>
       <c r="B42" s="3">
-        <v>5116994</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44481</v>
+        <v>44488</v>
       </c>
       <c r="B43" s="3">
-        <v>5018535</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44480</v>
+        <v>44487</v>
       </c>
       <c r="B44" s="3">
-        <v>4925635</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44479</v>
+        <v>44486</v>
       </c>
       <c r="B45" s="3">
-        <v>4890800</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B46" s="3">
-        <v>4831173</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44477</v>
+        <v>44484</v>
       </c>
       <c r="B47" s="3">
-        <v>4738793</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44476</v>
+        <v>44483</v>
       </c>
       <c r="B48" s="3">
-        <v>4653723</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44475</v>
+        <v>44482</v>
       </c>
       <c r="B49" s="3">
-        <v>4567214</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44474</v>
+        <v>44481</v>
       </c>
       <c r="B50" s="3">
-        <v>4465060</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44473</v>
+        <v>44480</v>
       </c>
       <c r="B51" s="3">
-        <v>4449546</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>44472</v>
+        <v>44479</v>
       </c>
       <c r="B52" s="3">
-        <v>4428121</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44471</v>
+        <v>44478</v>
       </c>
       <c r="B53" s="3">
-        <v>4384051</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>44470</v>
+        <v>44477</v>
       </c>
       <c r="B54" s="3">
-        <v>4297900</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44469</v>
+        <v>44476</v>
       </c>
       <c r="B55" s="3">
-        <v>4218516</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44468</v>
+        <v>44475</v>
       </c>
       <c r="B56" s="3">
-        <v>4145673</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>44467</v>
+        <v>44474</v>
       </c>
       <c r="B57" s="3">
-        <v>4060612</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>44466</v>
+        <v>44473</v>
       </c>
       <c r="B58" s="3">
-        <v>3979094</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44465</v>
+        <v>44472</v>
       </c>
       <c r="B59" s="3">
-        <v>3953132</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B60" s="3">
-        <v>3898564</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44463</v>
+        <v>44470</v>
       </c>
       <c r="B61" s="3">
-        <v>3804258</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>44462</v>
+        <v>44469</v>
       </c>
       <c r="B62" s="3">
-        <v>3724979</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>44461</v>
+        <v>44468</v>
       </c>
       <c r="B63" s="3">
-        <v>3646849</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>44460</v>
+        <v>44467</v>
       </c>
       <c r="B64" s="3">
-        <v>3563962</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>44459</v>
+        <v>44466</v>
       </c>
       <c r="B65" s="3">
-        <v>3487539</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44458</v>
+        <v>44465</v>
       </c>
       <c r="B66" s="3">
-        <v>3461082</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B67" s="3">
-        <v>3412016</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>44456</v>
+        <v>44463</v>
       </c>
       <c r="B68" s="3">
-        <v>3323936</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>44455</v>
+        <v>44462</v>
       </c>
       <c r="B69" s="3">
-        <v>3259323</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B70" s="3">
-        <v>3189070</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>44453</v>
+        <v>44460</v>
       </c>
       <c r="B71" s="3">
-        <v>3123699</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>44452</v>
+        <v>44459</v>
       </c>
       <c r="B72" s="3">
-        <v>3051925</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>44451</v>
+        <v>44458</v>
       </c>
       <c r="B73" s="3">
-        <v>3031072</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B74" s="3">
-        <v>2992899</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>44449</v>
+        <v>44456</v>
       </c>
       <c r="B75" s="3">
-        <v>2924263</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>44448</v>
+        <v>44455</v>
       </c>
       <c r="B76" s="3">
-        <v>2860253</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>44447</v>
+        <v>44454</v>
       </c>
       <c r="B77" s="3">
-        <v>2802011</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>44446</v>
+        <v>44453</v>
       </c>
       <c r="B78" s="3">
-        <v>2743498</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>44445</v>
+        <v>44452</v>
       </c>
       <c r="B79" s="3">
-        <v>2692904</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>44444</v>
+        <v>44451</v>
       </c>
       <c r="B80" s="3">
-        <v>2678906</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>44443</v>
+        <v>44450</v>
       </c>
       <c r="B81" s="3">
-        <v>2644865</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>44442</v>
+        <v>44449</v>
       </c>
       <c r="B82" s="3">
-        <v>2590966</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>44441</v>
+        <v>44448</v>
       </c>
       <c r="B83" s="3">
-        <v>2539287</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>44440</v>
+        <v>44447</v>
       </c>
       <c r="B84" s="3">
-        <v>2484199</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>44439</v>
+        <v>44446</v>
       </c>
       <c r="B85" s="3">
-        <v>2433592</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>44438</v>
+        <v>44445</v>
       </c>
       <c r="B86" s="3">
-        <v>2372417</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>44437</v>
+        <v>44444</v>
       </c>
       <c r="B87" s="3">
-        <v>2353563</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>44436</v>
+        <v>44443</v>
       </c>
       <c r="B88" s="3">
-        <v>2326130</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>44435</v>
+        <v>44442</v>
       </c>
       <c r="B89" s="3">
-        <v>2273984</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>44434</v>
+        <v>44441</v>
       </c>
       <c r="B90" s="3">
-        <v>2218458</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>44433</v>
+        <v>44440</v>
       </c>
       <c r="B91" s="3">
-        <v>2163192</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>44432</v>
+        <v>44439</v>
       </c>
       <c r="B92" s="3">
-        <v>2112611</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>44431</v>
+        <v>44438</v>
       </c>
       <c r="B93" s="3">
-        <v>2066915</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>44430</v>
+        <v>44437</v>
       </c>
       <c r="B94" s="3">
-        <v>2052364</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>44429</v>
+        <v>44436</v>
       </c>
       <c r="B95" s="3">
-        <v>2022928</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>44428</v>
+        <v>44435</v>
       </c>
       <c r="B96" s="3">
-        <v>1973224</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>44427</v>
+        <v>44434</v>
       </c>
       <c r="B97" s="3">
-        <v>1924839</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>44426</v>
+        <v>44433</v>
       </c>
       <c r="B98" s="3">
-        <v>1871458</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>44425</v>
+        <v>44432</v>
       </c>
       <c r="B99" s="3">
-        <v>1826165</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>44424</v>
+        <v>44431</v>
       </c>
       <c r="B100" s="3">
-        <v>1781578</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>44423</v>
+        <v>44430</v>
       </c>
       <c r="B101" s="3">
-        <v>1767176</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="B102" s="3">
-        <v>1742669</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>44421</v>
+        <v>44428</v>
       </c>
       <c r="B103" s="3">
-        <v>1693577</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>44420</v>
+        <v>44427</v>
       </c>
       <c r="B104" s="3">
-        <v>1645077</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="B105" s="3">
-        <v>1599438</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>44418</v>
+        <v>44425</v>
       </c>
       <c r="B106" s="3">
-        <v>1548545</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>44417</v>
+        <v>44424</v>
       </c>
       <c r="B107" s="3">
-        <v>1510648</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>44416</v>
+        <v>44423</v>
       </c>
       <c r="B108" s="3">
-        <v>1501249</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>44415</v>
+        <v>44422</v>
       </c>
       <c r="B109" s="3">
-        <v>1463495</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>44414</v>
+        <v>44421</v>
       </c>
       <c r="B110" s="3">
-        <v>1423185</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>44413</v>
+        <v>44420</v>
       </c>
       <c r="B111" s="3">
-        <v>1381481</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>44412</v>
+        <v>44419</v>
       </c>
       <c r="B112" s="3">
-        <v>1342211</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>44411</v>
+        <v>44418</v>
       </c>
       <c r="B113" s="3">
-        <v>1300394</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>44410</v>
+        <v>44417</v>
       </c>
       <c r="B114" s="3">
-        <v>1265839</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>44409</v>
+        <v>44416</v>
       </c>
       <c r="B115" s="3">
-        <v>1252304</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>44408</v>
+        <v>44415</v>
       </c>
       <c r="B116" s="3">
-        <v>1228845</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>44407</v>
+        <v>44414</v>
       </c>
       <c r="B117" s="3">
-        <v>1190942</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>44406</v>
+        <v>44413</v>
       </c>
       <c r="B118" s="3">
-        <v>1156321</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>44405</v>
+        <v>44412</v>
       </c>
       <c r="B119" s="3">
-        <v>1108405</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>44404</v>
+        <v>44411</v>
       </c>
       <c r="B120" s="3">
-        <v>1071895</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>44403</v>
+        <v>44410</v>
       </c>
       <c r="B121" s="3">
-        <v>1045515</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>44402</v>
+        <v>44409</v>
       </c>
       <c r="B122" s="3">
-        <v>1034280</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>44401</v>
+        <v>44408</v>
       </c>
       <c r="B123" s="3">
-        <v>1012939</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>44400</v>
+        <v>44407</v>
       </c>
       <c r="B124" s="3">
-        <v>982170</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>44399</v>
+        <v>44406</v>
       </c>
       <c r="B125" s="3">
-        <v>948667</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>44398</v>
+        <v>44405</v>
       </c>
       <c r="B126" s="3">
-        <v>912940</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>44397</v>
+        <v>44404</v>
       </c>
       <c r="B127" s="3">
-        <v>882844</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>44396</v>
+        <v>44403</v>
       </c>
       <c r="B128" s="3">
-        <v>854625</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>44395</v>
+        <v>44402</v>
       </c>
       <c r="B129" s="3">
-        <v>846261</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>44394</v>
+        <v>44401</v>
       </c>
       <c r="B130" s="3">
-        <v>830856</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="B131" s="3">
-        <v>801520</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>44392</v>
+        <v>44399</v>
       </c>
       <c r="B132" s="3">
-        <v>769552</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>44391</v>
+        <v>44398</v>
       </c>
       <c r="B133" s="3">
-        <v>741075</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>44390</v>
+        <v>44397</v>
       </c>
       <c r="B134" s="3">
-        <v>710714</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>44389</v>
+        <v>44396</v>
       </c>
       <c r="B135" s="3">
-        <v>686408</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>44388</v>
+        <v>44395</v>
       </c>
       <c r="B136" s="3">
-        <v>683667</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>44387</v>
+        <v>44394</v>
       </c>
       <c r="B137" s="3">
-        <v>671858</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>44386</v>
+        <v>44393</v>
       </c>
       <c r="B138" s="3">
-        <v>651446</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>44385</v>
+        <v>44392</v>
       </c>
       <c r="B139" s="3">
-        <v>629961</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>44384</v>
+        <v>44391</v>
       </c>
       <c r="B140" s="3">
-        <v>609108</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>44383</v>
+        <v>44390</v>
       </c>
       <c r="B141" s="3">
-        <v>586674</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>44382</v>
+        <v>44389</v>
       </c>
       <c r="B142" s="3">
-        <v>567316</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>44381</v>
+        <v>44388</v>
       </c>
       <c r="B143" s="3">
-        <v>564930</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>44380</v>
+        <v>44387</v>
       </c>
       <c r="B144" s="3">
-        <v>554057</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>44379</v>
+        <v>44386</v>
       </c>
       <c r="B145" s="3">
-        <v>534493</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
-        <v>44378</v>
+        <v>44385</v>
       </c>
       <c r="B146" s="3">
-        <v>471176</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>44377</v>
+        <v>44384</v>
       </c>
       <c r="B147" s="3">
-        <v>471176</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>44376</v>
+        <v>44383</v>
       </c>
       <c r="B148" s="3">
-        <v>463624</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>44375</v>
+        <v>44382</v>
       </c>
       <c r="B149" s="3">
-        <v>396652</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
-        <v>44374</v>
+        <v>44381</v>
       </c>
       <c r="B150" s="3">
-        <v>396246</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
-        <v>44373</v>
+        <v>44380</v>
       </c>
       <c r="B151" s="3">
-        <v>392527</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
-        <v>44372</v>
+        <v>44379</v>
       </c>
       <c r="B152" s="3">
-        <v>385092</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
-        <v>44371</v>
+        <v>44378</v>
       </c>
       <c r="B153" s="3">
-        <v>376276</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
-        <v>44370</v>
+        <v>44377</v>
       </c>
       <c r="B154" s="3">
-        <v>366660</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
-        <v>44369</v>
+        <v>44376</v>
       </c>
       <c r="B155" s="3">
-        <v>357767</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="B156" s="3">
-        <v>294981</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
-        <v>44367</v>
+        <v>44374</v>
       </c>
       <c r="B157" s="3">
-        <v>294965</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
-        <v>44366</v>
+        <v>44373</v>
       </c>
       <c r="B158" s="3">
-        <v>289941</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
-        <v>44365</v>
+        <v>44372</v>
       </c>
       <c r="B159" s="3">
-        <v>279418</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
-        <v>44364</v>
+        <v>44371</v>
       </c>
       <c r="B160" s="3">
-        <v>269824</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
-        <v>44363</v>
+        <v>44370</v>
       </c>
       <c r="B161" s="3">
-        <v>259437</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
-        <v>44362</v>
+        <v>44369</v>
       </c>
       <c r="B162" s="3">
-        <v>237250</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
-        <v>44361</v>
+        <v>44368</v>
       </c>
       <c r="B163" s="3">
-        <v>237250</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
-        <v>44360</v>
+        <v>44367</v>
       </c>
       <c r="B164" s="3">
-        <v>237250</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
-        <v>44359</v>
+        <v>44366</v>
       </c>
       <c r="B165" s="3">
-        <v>232335</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
-        <v>44358</v>
+        <v>44365</v>
       </c>
       <c r="B166" s="3">
-        <v>222807</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
-        <v>44357</v>
+        <v>44364</v>
       </c>
       <c r="B167" s="3">
-        <v>213686</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
-        <v>44356</v>
+        <v>44363</v>
       </c>
       <c r="B168" s="3">
-        <v>213686</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
-        <v>44355</v>
+        <v>44362</v>
       </c>
       <c r="B169" s="3">
-        <v>204595</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
-        <v>44354</v>
+        <v>44361</v>
       </c>
       <c r="B170" s="3">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
-        <v>44353</v>
+        <v>44360</v>
       </c>
       <c r="B171" s="3">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
-        <v>44352</v>
+        <v>44359</v>
       </c>
       <c r="B172" s="3">
-        <v>179477</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
-        <v>44351</v>
+        <v>44358</v>
       </c>
       <c r="B173" s="3">
-        <v>175030</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
-        <v>44350</v>
+        <v>44357</v>
       </c>
       <c r="B174" s="3">
-        <v>170669</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
-        <v>44349</v>
+        <v>44356</v>
       </c>
       <c r="B175" s="3">
-        <v>167075</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
-        <v>44348</v>
+        <v>44355</v>
       </c>
       <c r="B176" s="3">
-        <v>156333</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
-        <v>44347</v>
+        <v>44354</v>
       </c>
       <c r="B177" s="3">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
-        <v>44346</v>
+        <v>44353</v>
       </c>
       <c r="B178" s="3">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B179" s="3">
-        <v>153886</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B180" s="3">
-        <v>153886</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B181" s="3">
-        <v>150552</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B182" s="3">
-        <v>145341</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B183" s="3">
-        <v>125810</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B184" s="3">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
-        <v>44339</v>
+        <v>44346</v>
       </c>
       <c r="B185" s="3">
-        <v>96745</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
-        <v>44338</v>
+        <v>44345</v>
       </c>
       <c r="B186" s="3">
-        <v>96266</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
-        <v>44337</v>
+        <v>44344</v>
       </c>
       <c r="B187" s="3">
-        <v>93860</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
-        <v>44336</v>
+        <v>44343</v>
       </c>
       <c r="B188" s="3">
-        <v>91297</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
-        <v>44335</v>
+        <v>44342</v>
       </c>
       <c r="B189" s="3">
-        <v>89049</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
-        <v>44334</v>
+        <v>44341</v>
       </c>
       <c r="B190" s="3">
-        <v>87045</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
-        <v>44333</v>
+        <v>44340</v>
       </c>
       <c r="B191" s="3">
-        <v>84963</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
-        <v>44332</v>
+        <v>44339</v>
       </c>
       <c r="B192" s="3">
-        <v>84963</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
-        <v>44331</v>
+        <v>44338</v>
       </c>
       <c r="B193" s="3">
-        <v>84474</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
-        <v>44330</v>
+        <v>44337</v>
       </c>
       <c r="B194" s="3">
-        <v>82774</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
-        <v>44329</v>
+        <v>44336</v>
       </c>
       <c r="B195" s="3">
-        <v>81457</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
-        <v>44328</v>
+        <v>44335</v>
       </c>
       <c r="B196" s="3">
-        <v>80082</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
-        <v>44327</v>
+        <v>44334</v>
       </c>
       <c r="B197" s="3">
-        <v>78744</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
-        <v>44326</v>
+        <v>44333</v>
       </c>
       <c r="B198" s="3">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
-        <v>44325</v>
+        <v>44332</v>
       </c>
       <c r="B199" s="3">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B200" s="3">
-        <v>76908</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B201" s="3">
-        <v>75187</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
-        <v>44322</v>
+        <v>44329</v>
       </c>
       <c r="B202" s="3">
-        <v>73270</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B203" s="3">
-        <v>71767</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B204" s="3">
-        <v>70039</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B205" s="3">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
-        <v>44318</v>
+        <v>44325</v>
       </c>
       <c r="B206" s="3">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
-        <v>44317</v>
+        <v>44324</v>
       </c>
       <c r="B207" s="3">
-        <v>68472</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="B208" s="3">
-        <v>67149</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
-        <v>44315</v>
+        <v>44322</v>
       </c>
       <c r="B209" s="3">
-        <v>65948</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
-        <v>44314</v>
+        <v>44321</v>
       </c>
       <c r="B210" s="3">
-        <v>64910</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
-        <v>44313</v>
+        <v>44320</v>
       </c>
       <c r="B211" s="3">
-        <v>63944</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
-        <v>44312</v>
+        <v>44319</v>
       </c>
       <c r="B212" s="3">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
-        <v>44311</v>
+        <v>44318</v>
       </c>
       <c r="B213" s="3">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
-        <v>44310</v>
+        <v>44317</v>
       </c>
       <c r="B214" s="3">
-        <v>63317</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
-        <v>44309</v>
+        <v>44316</v>
       </c>
       <c r="B215" s="3">
-        <v>62491</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
-        <v>44308</v>
+        <v>44315</v>
       </c>
       <c r="B216" s="3">
-        <v>60582</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
-        <v>44307</v>
+        <v>44314</v>
       </c>
       <c r="B217" s="3">
-        <v>58662</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
-        <v>44306</v>
+        <v>44313</v>
       </c>
       <c r="B218" s="3">
-        <v>54736</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="B219" s="3">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
-        <v>44304</v>
+        <v>44311</v>
       </c>
       <c r="B220" s="3">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
-        <v>44303</v>
+        <v>44310</v>
       </c>
       <c r="B221" s="3">
-        <v>54555</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
-        <v>44302</v>
+        <v>44309</v>
       </c>
       <c r="B222" s="3">
-        <v>52537</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="B223" s="3">
-        <v>50388</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
-        <v>44300</v>
+        <v>44307</v>
       </c>
       <c r="B224" s="3">
-        <v>48482</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
-        <v>44299</v>
+        <v>44306</v>
       </c>
       <c r="B225" s="3">
-        <v>46400</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
-        <v>44298</v>
+        <v>44305</v>
       </c>
       <c r="B226" s="3">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
-        <v>44297</v>
+        <v>44304</v>
       </c>
       <c r="B227" s="3">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
-        <v>44296</v>
+        <v>44303</v>
       </c>
       <c r="B228" s="3">
-        <v>44016</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
-        <v>44295</v>
+        <v>44302</v>
       </c>
       <c r="B229" s="3">
-        <v>41376</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
-        <v>44294</v>
+        <v>44301</v>
       </c>
       <c r="B230" s="3">
-        <v>38445</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
-        <v>44293</v>
+        <v>44300</v>
       </c>
       <c r="B231" s="3">
-        <v>35475</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
-        <v>44292</v>
+        <v>44299</v>
       </c>
       <c r="B232" s="3">
-        <v>31795</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
-        <v>44291</v>
+        <v>44298</v>
       </c>
       <c r="B233" s="3">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
-        <v>44290</v>
+        <v>44297</v>
       </c>
       <c r="B234" s="3">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
-        <v>44289</v>
+        <v>44296</v>
       </c>
       <c r="B235" s="3">
-        <v>30383</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
-        <v>44288</v>
+        <v>44295</v>
       </c>
       <c r="B236" s="3">
-        <v>29796</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B237" s="4"/>
+        <v>44294</v>
+      </c>
+      <c r="B237" s="3">
+        <v>38445</v>
+      </c>
     </row>
     <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
-        <v>44286</v>
-      </c>
-      <c r="B238" s="4"/>
+        <v>44293</v>
+      </c>
+      <c r="B238" s="3">
+        <v>35475</v>
+      </c>
     </row>
     <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
-        <v>44285</v>
-      </c>
-      <c r="B239" s="4"/>
+        <v>44292</v>
+      </c>
+      <c r="B239" s="3">
+        <v>31795</v>
+      </c>
     </row>
     <row r="240" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
-        <v>44284</v>
-      </c>
-      <c r="B240" s="4"/>
+        <v>44291</v>
+      </c>
+      <c r="B240" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="241" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
-        <v>44283</v>
-      </c>
-      <c r="B241" s="4"/>
+        <v>44290</v>
+      </c>
+      <c r="B241" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="242" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
-        <v>44282</v>
-      </c>
-      <c r="B242" s="4"/>
+        <v>44289</v>
+      </c>
+      <c r="B242" s="3">
+        <v>30383</v>
+      </c>
     </row>
     <row r="243" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
-        <v>44281</v>
-      </c>
-      <c r="B243" s="4"/>
+        <v>44288</v>
+      </c>
+      <c r="B243" s="3">
+        <v>29796</v>
+      </c>
     </row>
     <row r="244" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
-        <v>44280</v>
+        <v>44287</v>
       </c>
       <c r="B244" s="4"/>
     </row>
     <row r="245" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
-        <v>44279</v>
+        <v>44286</v>
       </c>
       <c r="B245" s="4"/>
     </row>
     <row r="246" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
+        <v>44285</v>
+      </c>
+      <c r="B246" s="4"/>
+    </row>
+    <row r="247" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A247" s="2">
+        <v>44284</v>
+      </c>
+      <c r="B247" s="4"/>
+    </row>
+    <row r="248" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A248" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B248" s="4"/>
+    </row>
+    <row r="249" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A249" s="2">
+        <v>44282</v>
+      </c>
+      <c r="B249" s="4"/>
+    </row>
+    <row r="250" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A250" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B250" s="4"/>
+    </row>
+    <row r="251" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A251" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B251" s="4"/>
+    </row>
+    <row r="252" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A252" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B252" s="4"/>
+    </row>
+    <row r="253" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A253" s="2">
         <v>44278</v>
       </c>
-      <c r="B246" s="4"/>
+      <c r="B253" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{A7F15A82-DD8F-4D4A-B31F-57C09B82F350}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{0CFE7143-ADE8-A945-8A62-4628C14A0C5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated trans-Tasman comparison to 7 December
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82E83EA0-9021-8D46-8512-8321939065CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252EA913-AE7C-0E4C-9048-5518C819E9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
+    <workbookView xWindow="54400" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BAE720-0FFD-AC44-A3E0-A012DA41F8A8}">
-  <dimension ref="A1:B253"/>
+  <dimension ref="A1:B260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="B271" sqref="B271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,2003 +447,2059 @@
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44529</v>
+        <v>44536</v>
       </c>
       <c r="B2" s="3">
-        <v>6366060</v>
+        <v>6396368</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44528</v>
+        <v>44535</v>
       </c>
       <c r="B3" s="3">
-        <v>6365073</v>
+        <v>6395543</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44527</v>
+        <v>44534</v>
       </c>
       <c r="B4" s="3">
-        <v>6362348</v>
+        <v>6393476</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44526</v>
+        <v>44533</v>
       </c>
       <c r="B5" s="3">
-        <v>6355156</v>
+        <v>6387955</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44525</v>
+        <v>44532</v>
       </c>
       <c r="B6" s="3">
-        <v>6348980</v>
+        <v>6383068</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44524</v>
+        <v>44531</v>
       </c>
       <c r="B7" s="3">
-        <v>6341726</v>
+        <v>6378225</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44523</v>
+        <v>44530</v>
       </c>
       <c r="B8" s="3">
-        <v>6334061</v>
+        <v>6372197</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44522</v>
+        <v>44529</v>
       </c>
       <c r="B9" s="3">
-        <v>6325341</v>
+        <v>6366060</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44521</v>
+        <v>44528</v>
       </c>
       <c r="B10" s="3">
-        <v>6324333</v>
+        <v>6365073</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44520</v>
+        <v>44527</v>
       </c>
       <c r="B11" s="3">
-        <v>6320582</v>
+        <v>6362348</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44519</v>
+        <v>44526</v>
       </c>
       <c r="B12" s="3">
-        <v>6311361</v>
+        <v>6355156</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44518</v>
+        <v>44525</v>
       </c>
       <c r="B13" s="3">
-        <v>6301870</v>
+        <v>6348980</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44517</v>
+        <v>44524</v>
       </c>
       <c r="B14" s="3">
-        <v>6291057</v>
+        <v>6341726</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44516</v>
+        <v>44523</v>
       </c>
       <c r="B15" s="3">
-        <v>6279967</v>
+        <v>6334061</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44515</v>
+        <v>44522</v>
       </c>
       <c r="B16" s="3">
-        <v>6268391</v>
+        <v>6325341</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44514</v>
+        <v>44521</v>
       </c>
       <c r="B17" s="3">
-        <v>6265758</v>
+        <v>6324333</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44513</v>
+        <v>44520</v>
       </c>
       <c r="B18" s="3">
-        <v>6259089</v>
+        <v>6320582</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44512</v>
+        <v>44519</v>
       </c>
       <c r="B19" s="3">
-        <v>6243318</v>
+        <v>6311361</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>44511</v>
+        <v>44518</v>
       </c>
       <c r="B20" s="3">
-        <v>6226830</v>
+        <v>6301870</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="B21" s="3">
-        <v>6210103</v>
+        <v>6291057</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44509</v>
+        <v>44516</v>
       </c>
       <c r="B22" s="3">
-        <v>6192099</v>
+        <v>6279967</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44508</v>
+        <v>44515</v>
       </c>
       <c r="B23" s="3">
-        <v>6172372</v>
+        <v>6268391</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44507</v>
+        <v>44514</v>
       </c>
       <c r="B24" s="3">
-        <v>6168060</v>
+        <v>6265758</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44506</v>
+        <v>44513</v>
       </c>
       <c r="B25" s="3">
-        <v>6156414</v>
+        <v>6259089</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44505</v>
+        <v>44512</v>
       </c>
       <c r="B26" s="3">
-        <v>6130474</v>
+        <v>6243318</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44504</v>
+        <v>44511</v>
       </c>
       <c r="B27" s="3">
-        <v>6105744</v>
+        <v>6226830</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44503</v>
+        <v>44510</v>
       </c>
       <c r="B28" s="3">
-        <v>6077355</v>
+        <v>6210103</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44502</v>
+        <v>44509</v>
       </c>
       <c r="B29" s="3">
-        <v>6046074</v>
+        <v>6192099</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44501</v>
+        <v>44508</v>
       </c>
       <c r="B30" s="3">
-        <v>6009574</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44500</v>
+        <v>44507</v>
       </c>
       <c r="B31" s="3">
-        <v>5999926</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44499</v>
+        <v>44506</v>
       </c>
       <c r="B32" s="3">
-        <v>5977973</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44498</v>
+        <v>44505</v>
       </c>
       <c r="B33" s="3">
-        <v>5938861</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44497</v>
+        <v>44504</v>
       </c>
       <c r="B34" s="3">
-        <v>5898147</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44496</v>
+        <v>44503</v>
       </c>
       <c r="B35" s="3">
-        <v>5858123</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44495</v>
+        <v>44502</v>
       </c>
       <c r="B36" s="3">
-        <v>5818705</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44494</v>
+        <v>44501</v>
       </c>
       <c r="B37" s="3">
-        <v>5780737</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44493</v>
+        <v>44500</v>
       </c>
       <c r="B38" s="3">
-        <v>5766748</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44492</v>
+        <v>44499</v>
       </c>
       <c r="B39" s="3">
-        <v>5732872</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44491</v>
+        <v>44498</v>
       </c>
       <c r="B40" s="3">
-        <v>5677232</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44490</v>
+        <v>44497</v>
       </c>
       <c r="B41" s="3">
-        <v>5621660</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="B42" s="3">
-        <v>5565441</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44488</v>
+        <v>44495</v>
       </c>
       <c r="B43" s="3">
-        <v>5506563</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44487</v>
+        <v>44494</v>
       </c>
       <c r="B44" s="3">
-        <v>5440365</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44486</v>
+        <v>44493</v>
       </c>
       <c r="B45" s="3">
-        <v>5405628</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B46" s="3">
-        <v>5364911</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44484</v>
+        <v>44491</v>
       </c>
       <c r="B47" s="3">
-        <v>5288225</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44483</v>
+        <v>44490</v>
       </c>
       <c r="B48" s="3">
-        <v>5207377</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44482</v>
+        <v>44489</v>
       </c>
       <c r="B49" s="3">
-        <v>5116994</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44481</v>
+        <v>44488</v>
       </c>
       <c r="B50" s="3">
-        <v>5018535</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44480</v>
+        <v>44487</v>
       </c>
       <c r="B51" s="3">
-        <v>4925635</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>44479</v>
+        <v>44486</v>
       </c>
       <c r="B52" s="3">
-        <v>4890800</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B53" s="3">
-        <v>4831173</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>44477</v>
+        <v>44484</v>
       </c>
       <c r="B54" s="3">
-        <v>4738793</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44476</v>
+        <v>44483</v>
       </c>
       <c r="B55" s="3">
-        <v>4653723</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44475</v>
+        <v>44482</v>
       </c>
       <c r="B56" s="3">
-        <v>4567214</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>44474</v>
+        <v>44481</v>
       </c>
       <c r="B57" s="3">
-        <v>4465060</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>44473</v>
+        <v>44480</v>
       </c>
       <c r="B58" s="3">
-        <v>4449546</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44472</v>
+        <v>44479</v>
       </c>
       <c r="B59" s="3">
-        <v>4428121</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>44471</v>
+        <v>44478</v>
       </c>
       <c r="B60" s="3">
-        <v>4384051</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44470</v>
+        <v>44477</v>
       </c>
       <c r="B61" s="3">
-        <v>4297900</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>44469</v>
+        <v>44476</v>
       </c>
       <c r="B62" s="3">
-        <v>4218516</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>44468</v>
+        <v>44475</v>
       </c>
       <c r="B63" s="3">
-        <v>4145673</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>44467</v>
+        <v>44474</v>
       </c>
       <c r="B64" s="3">
-        <v>4060612</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>44466</v>
+        <v>44473</v>
       </c>
       <c r="B65" s="3">
-        <v>3979094</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44465</v>
+        <v>44472</v>
       </c>
       <c r="B66" s="3">
-        <v>3953132</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B67" s="3">
-        <v>3898564</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>44463</v>
+        <v>44470</v>
       </c>
       <c r="B68" s="3">
-        <v>3804258</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>44462</v>
+        <v>44469</v>
       </c>
       <c r="B69" s="3">
-        <v>3724979</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>44461</v>
+        <v>44468</v>
       </c>
       <c r="B70" s="3">
-        <v>3646849</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>44460</v>
+        <v>44467</v>
       </c>
       <c r="B71" s="3">
-        <v>3563962</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>44459</v>
+        <v>44466</v>
       </c>
       <c r="B72" s="3">
-        <v>3487539</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>44458</v>
+        <v>44465</v>
       </c>
       <c r="B73" s="3">
-        <v>3461082</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B74" s="3">
-        <v>3412016</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>44456</v>
+        <v>44463</v>
       </c>
       <c r="B75" s="3">
-        <v>3323936</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>44455</v>
+        <v>44462</v>
       </c>
       <c r="B76" s="3">
-        <v>3259323</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B77" s="3">
-        <v>3189070</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>44453</v>
+        <v>44460</v>
       </c>
       <c r="B78" s="3">
-        <v>3123699</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>44452</v>
+        <v>44459</v>
       </c>
       <c r="B79" s="3">
-        <v>3051925</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>44451</v>
+        <v>44458</v>
       </c>
       <c r="B80" s="3">
-        <v>3031072</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B81" s="3">
-        <v>2992899</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>44449</v>
+        <v>44456</v>
       </c>
       <c r="B82" s="3">
-        <v>2924263</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>44448</v>
+        <v>44455</v>
       </c>
       <c r="B83" s="3">
-        <v>2860253</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>44447</v>
+        <v>44454</v>
       </c>
       <c r="B84" s="3">
-        <v>2802011</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>44446</v>
+        <v>44453</v>
       </c>
       <c r="B85" s="3">
-        <v>2743498</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>44445</v>
+        <v>44452</v>
       </c>
       <c r="B86" s="3">
-        <v>2692904</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>44444</v>
+        <v>44451</v>
       </c>
       <c r="B87" s="3">
-        <v>2678906</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>44443</v>
+        <v>44450</v>
       </c>
       <c r="B88" s="3">
-        <v>2644865</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>44442</v>
+        <v>44449</v>
       </c>
       <c r="B89" s="3">
-        <v>2590966</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>44441</v>
+        <v>44448</v>
       </c>
       <c r="B90" s="3">
-        <v>2539287</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>44440</v>
+        <v>44447</v>
       </c>
       <c r="B91" s="3">
-        <v>2484199</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>44439</v>
+        <v>44446</v>
       </c>
       <c r="B92" s="3">
-        <v>2433592</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>44438</v>
+        <v>44445</v>
       </c>
       <c r="B93" s="3">
-        <v>2372417</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>44437</v>
+        <v>44444</v>
       </c>
       <c r="B94" s="3">
-        <v>2353563</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>44436</v>
+        <v>44443</v>
       </c>
       <c r="B95" s="3">
-        <v>2326130</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>44435</v>
+        <v>44442</v>
       </c>
       <c r="B96" s="3">
-        <v>2273984</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>44434</v>
+        <v>44441</v>
       </c>
       <c r="B97" s="3">
-        <v>2218458</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>44433</v>
+        <v>44440</v>
       </c>
       <c r="B98" s="3">
-        <v>2163192</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>44432</v>
+        <v>44439</v>
       </c>
       <c r="B99" s="3">
-        <v>2112611</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>44431</v>
+        <v>44438</v>
       </c>
       <c r="B100" s="3">
-        <v>2066915</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>44430</v>
+        <v>44437</v>
       </c>
       <c r="B101" s="3">
-        <v>2052364</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>44429</v>
+        <v>44436</v>
       </c>
       <c r="B102" s="3">
-        <v>2022928</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>44428</v>
+        <v>44435</v>
       </c>
       <c r="B103" s="3">
-        <v>1973224</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>44427</v>
+        <v>44434</v>
       </c>
       <c r="B104" s="3">
-        <v>1924839</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>44426</v>
+        <v>44433</v>
       </c>
       <c r="B105" s="3">
-        <v>1871458</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>44425</v>
+        <v>44432</v>
       </c>
       <c r="B106" s="3">
-        <v>1826165</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>44424</v>
+        <v>44431</v>
       </c>
       <c r="B107" s="3">
-        <v>1781578</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>44423</v>
+        <v>44430</v>
       </c>
       <c r="B108" s="3">
-        <v>1767176</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="B109" s="3">
-        <v>1742669</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>44421</v>
+        <v>44428</v>
       </c>
       <c r="B110" s="3">
-        <v>1693577</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>44420</v>
+        <v>44427</v>
       </c>
       <c r="B111" s="3">
-        <v>1645077</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="B112" s="3">
-        <v>1599438</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>44418</v>
+        <v>44425</v>
       </c>
       <c r="B113" s="3">
-        <v>1548545</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>44417</v>
+        <v>44424</v>
       </c>
       <c r="B114" s="3">
-        <v>1510648</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>44416</v>
+        <v>44423</v>
       </c>
       <c r="B115" s="3">
-        <v>1501249</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>44415</v>
+        <v>44422</v>
       </c>
       <c r="B116" s="3">
-        <v>1463495</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>44414</v>
+        <v>44421</v>
       </c>
       <c r="B117" s="3">
-        <v>1423185</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>44413</v>
+        <v>44420</v>
       </c>
       <c r="B118" s="3">
-        <v>1381481</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>44412</v>
+        <v>44419</v>
       </c>
       <c r="B119" s="3">
-        <v>1342211</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>44411</v>
+        <v>44418</v>
       </c>
       <c r="B120" s="3">
-        <v>1300394</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>44410</v>
+        <v>44417</v>
       </c>
       <c r="B121" s="3">
-        <v>1265839</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>44409</v>
+        <v>44416</v>
       </c>
       <c r="B122" s="3">
-        <v>1252304</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>44408</v>
+        <v>44415</v>
       </c>
       <c r="B123" s="3">
-        <v>1228845</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>44407</v>
+        <v>44414</v>
       </c>
       <c r="B124" s="3">
-        <v>1190942</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>44406</v>
+        <v>44413</v>
       </c>
       <c r="B125" s="3">
-        <v>1156321</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>44405</v>
+        <v>44412</v>
       </c>
       <c r="B126" s="3">
-        <v>1108405</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>44404</v>
+        <v>44411</v>
       </c>
       <c r="B127" s="3">
-        <v>1071895</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>44403</v>
+        <v>44410</v>
       </c>
       <c r="B128" s="3">
-        <v>1045515</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>44402</v>
+        <v>44409</v>
       </c>
       <c r="B129" s="3">
-        <v>1034280</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>44401</v>
+        <v>44408</v>
       </c>
       <c r="B130" s="3">
-        <v>1012939</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>44400</v>
+        <v>44407</v>
       </c>
       <c r="B131" s="3">
-        <v>982170</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>44399</v>
+        <v>44406</v>
       </c>
       <c r="B132" s="3">
-        <v>948667</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>44398</v>
+        <v>44405</v>
       </c>
       <c r="B133" s="3">
-        <v>912940</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>44397</v>
+        <v>44404</v>
       </c>
       <c r="B134" s="3">
-        <v>882844</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>44396</v>
+        <v>44403</v>
       </c>
       <c r="B135" s="3">
-        <v>854625</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>44395</v>
+        <v>44402</v>
       </c>
       <c r="B136" s="3">
-        <v>846261</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>44394</v>
+        <v>44401</v>
       </c>
       <c r="B137" s="3">
-        <v>830856</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="B138" s="3">
-        <v>801520</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>44392</v>
+        <v>44399</v>
       </c>
       <c r="B139" s="3">
-        <v>769552</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>44391</v>
+        <v>44398</v>
       </c>
       <c r="B140" s="3">
-        <v>741075</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>44390</v>
+        <v>44397</v>
       </c>
       <c r="B141" s="3">
-        <v>710714</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>44389</v>
+        <v>44396</v>
       </c>
       <c r="B142" s="3">
-        <v>686408</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>44388</v>
+        <v>44395</v>
       </c>
       <c r="B143" s="3">
-        <v>683667</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>44387</v>
+        <v>44394</v>
       </c>
       <c r="B144" s="3">
-        <v>671858</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>44386</v>
+        <v>44393</v>
       </c>
       <c r="B145" s="3">
-        <v>651446</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
-        <v>44385</v>
+        <v>44392</v>
       </c>
       <c r="B146" s="3">
-        <v>629961</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>44384</v>
+        <v>44391</v>
       </c>
       <c r="B147" s="3">
-        <v>609108</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>44383</v>
+        <v>44390</v>
       </c>
       <c r="B148" s="3">
-        <v>586674</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>44382</v>
+        <v>44389</v>
       </c>
       <c r="B149" s="3">
-        <v>567316</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
-        <v>44381</v>
+        <v>44388</v>
       </c>
       <c r="B150" s="3">
-        <v>564930</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
-        <v>44380</v>
+        <v>44387</v>
       </c>
       <c r="B151" s="3">
-        <v>554057</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
-        <v>44379</v>
+        <v>44386</v>
       </c>
       <c r="B152" s="3">
-        <v>534493</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
-        <v>44378</v>
+        <v>44385</v>
       </c>
       <c r="B153" s="3">
-        <v>471176</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
-        <v>44377</v>
+        <v>44384</v>
       </c>
       <c r="B154" s="3">
-        <v>471176</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
-        <v>44376</v>
+        <v>44383</v>
       </c>
       <c r="B155" s="3">
-        <v>463624</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
-        <v>44375</v>
+        <v>44382</v>
       </c>
       <c r="B156" s="3">
-        <v>396652</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
-        <v>44374</v>
+        <v>44381</v>
       </c>
       <c r="B157" s="3">
-        <v>396246</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
-        <v>44373</v>
+        <v>44380</v>
       </c>
       <c r="B158" s="3">
-        <v>392527</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
-        <v>44372</v>
+        <v>44379</v>
       </c>
       <c r="B159" s="3">
-        <v>385092</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
-        <v>44371</v>
+        <v>44378</v>
       </c>
       <c r="B160" s="3">
-        <v>376276</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
-        <v>44370</v>
+        <v>44377</v>
       </c>
       <c r="B161" s="3">
-        <v>366660</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
-        <v>44369</v>
+        <v>44376</v>
       </c>
       <c r="B162" s="3">
-        <v>357767</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="B163" s="3">
-        <v>294981</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
-        <v>44367</v>
+        <v>44374</v>
       </c>
       <c r="B164" s="3">
-        <v>294965</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
-        <v>44366</v>
+        <v>44373</v>
       </c>
       <c r="B165" s="3">
-        <v>289941</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
-        <v>44365</v>
+        <v>44372</v>
       </c>
       <c r="B166" s="3">
-        <v>279418</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
-        <v>44364</v>
+        <v>44371</v>
       </c>
       <c r="B167" s="3">
-        <v>269824</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
-        <v>44363</v>
+        <v>44370</v>
       </c>
       <c r="B168" s="3">
-        <v>259437</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
-        <v>44362</v>
+        <v>44369</v>
       </c>
       <c r="B169" s="3">
-        <v>237250</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
-        <v>44361</v>
+        <v>44368</v>
       </c>
       <c r="B170" s="3">
-        <v>237250</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
-        <v>44360</v>
+        <v>44367</v>
       </c>
       <c r="B171" s="3">
-        <v>237250</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
-        <v>44359</v>
+        <v>44366</v>
       </c>
       <c r="B172" s="3">
-        <v>232335</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
-        <v>44358</v>
+        <v>44365</v>
       </c>
       <c r="B173" s="3">
-        <v>222807</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
-        <v>44357</v>
+        <v>44364</v>
       </c>
       <c r="B174" s="3">
-        <v>213686</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
-        <v>44356</v>
+        <v>44363</v>
       </c>
       <c r="B175" s="3">
-        <v>213686</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
-        <v>44355</v>
+        <v>44362</v>
       </c>
       <c r="B176" s="3">
-        <v>204595</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
-        <v>44354</v>
+        <v>44361</v>
       </c>
       <c r="B177" s="3">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
-        <v>44353</v>
+        <v>44360</v>
       </c>
       <c r="B178" s="3">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
-        <v>44352</v>
+        <v>44359</v>
       </c>
       <c r="B179" s="3">
-        <v>179477</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
-        <v>44351</v>
+        <v>44358</v>
       </c>
       <c r="B180" s="3">
-        <v>175030</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
-        <v>44350</v>
+        <v>44357</v>
       </c>
       <c r="B181" s="3">
-        <v>170669</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
-        <v>44349</v>
+        <v>44356</v>
       </c>
       <c r="B182" s="3">
-        <v>167075</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
-        <v>44348</v>
+        <v>44355</v>
       </c>
       <c r="B183" s="3">
-        <v>156333</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
-        <v>44347</v>
+        <v>44354</v>
       </c>
       <c r="B184" s="3">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
-        <v>44346</v>
+        <v>44353</v>
       </c>
       <c r="B185" s="3">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B186" s="3">
-        <v>153886</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B187" s="3">
-        <v>153886</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B188" s="3">
-        <v>150552</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B189" s="3">
-        <v>145341</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B190" s="3">
-        <v>125810</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B191" s="3">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
-        <v>44339</v>
+        <v>44346</v>
       </c>
       <c r="B192" s="3">
-        <v>96745</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
-        <v>44338</v>
+        <v>44345</v>
       </c>
       <c r="B193" s="3">
-        <v>96266</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
-        <v>44337</v>
+        <v>44344</v>
       </c>
       <c r="B194" s="3">
-        <v>93860</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
-        <v>44336</v>
+        <v>44343</v>
       </c>
       <c r="B195" s="3">
-        <v>91297</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
-        <v>44335</v>
+        <v>44342</v>
       </c>
       <c r="B196" s="3">
-        <v>89049</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
-        <v>44334</v>
+        <v>44341</v>
       </c>
       <c r="B197" s="3">
-        <v>87045</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
-        <v>44333</v>
+        <v>44340</v>
       </c>
       <c r="B198" s="3">
-        <v>84963</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
-        <v>44332</v>
+        <v>44339</v>
       </c>
       <c r="B199" s="3">
-        <v>84963</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
-        <v>44331</v>
+        <v>44338</v>
       </c>
       <c r="B200" s="3">
-        <v>84474</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
-        <v>44330</v>
+        <v>44337</v>
       </c>
       <c r="B201" s="3">
-        <v>82774</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
-        <v>44329</v>
+        <v>44336</v>
       </c>
       <c r="B202" s="3">
-        <v>81457</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
-        <v>44328</v>
+        <v>44335</v>
       </c>
       <c r="B203" s="3">
-        <v>80082</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
-        <v>44327</v>
+        <v>44334</v>
       </c>
       <c r="B204" s="3">
-        <v>78744</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
-        <v>44326</v>
+        <v>44333</v>
       </c>
       <c r="B205" s="3">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
-        <v>44325</v>
+        <v>44332</v>
       </c>
       <c r="B206" s="3">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B207" s="3">
-        <v>76908</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B208" s="3">
-        <v>75187</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
-        <v>44322</v>
+        <v>44329</v>
       </c>
       <c r="B209" s="3">
-        <v>73270</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B210" s="3">
-        <v>71767</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B211" s="3">
-        <v>70039</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B212" s="3">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
-        <v>44318</v>
+        <v>44325</v>
       </c>
       <c r="B213" s="3">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
-        <v>44317</v>
+        <v>44324</v>
       </c>
       <c r="B214" s="3">
-        <v>68472</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="B215" s="3">
-        <v>67149</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
-        <v>44315</v>
+        <v>44322</v>
       </c>
       <c r="B216" s="3">
-        <v>65948</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
-        <v>44314</v>
+        <v>44321</v>
       </c>
       <c r="B217" s="3">
-        <v>64910</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
-        <v>44313</v>
+        <v>44320</v>
       </c>
       <c r="B218" s="3">
-        <v>63944</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
-        <v>44312</v>
+        <v>44319</v>
       </c>
       <c r="B219" s="3">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
-        <v>44311</v>
+        <v>44318</v>
       </c>
       <c r="B220" s="3">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
-        <v>44310</v>
+        <v>44317</v>
       </c>
       <c r="B221" s="3">
-        <v>63317</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
-        <v>44309</v>
+        <v>44316</v>
       </c>
       <c r="B222" s="3">
-        <v>62491</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
-        <v>44308</v>
+        <v>44315</v>
       </c>
       <c r="B223" s="3">
-        <v>60582</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
-        <v>44307</v>
+        <v>44314</v>
       </c>
       <c r="B224" s="3">
-        <v>58662</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
-        <v>44306</v>
+        <v>44313</v>
       </c>
       <c r="B225" s="3">
-        <v>54736</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="B226" s="3">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
-        <v>44304</v>
+        <v>44311</v>
       </c>
       <c r="B227" s="3">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
-        <v>44303</v>
+        <v>44310</v>
       </c>
       <c r="B228" s="3">
-        <v>54555</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
-        <v>44302</v>
+        <v>44309</v>
       </c>
       <c r="B229" s="3">
-        <v>52537</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="B230" s="3">
-        <v>50388</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
-        <v>44300</v>
+        <v>44307</v>
       </c>
       <c r="B231" s="3">
-        <v>48482</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
-        <v>44299</v>
+        <v>44306</v>
       </c>
       <c r="B232" s="3">
-        <v>46400</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
-        <v>44298</v>
+        <v>44305</v>
       </c>
       <c r="B233" s="3">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
-        <v>44297</v>
+        <v>44304</v>
       </c>
       <c r="B234" s="3">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
-        <v>44296</v>
+        <v>44303</v>
       </c>
       <c r="B235" s="3">
-        <v>44016</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
-        <v>44295</v>
+        <v>44302</v>
       </c>
       <c r="B236" s="3">
-        <v>41376</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
-        <v>44294</v>
+        <v>44301</v>
       </c>
       <c r="B237" s="3">
-        <v>38445</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
-        <v>44293</v>
+        <v>44300</v>
       </c>
       <c r="B238" s="3">
-        <v>35475</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
-        <v>44292</v>
+        <v>44299</v>
       </c>
       <c r="B239" s="3">
-        <v>31795</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
-        <v>44291</v>
+        <v>44298</v>
       </c>
       <c r="B240" s="3">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
-        <v>44290</v>
+        <v>44297</v>
       </c>
       <c r="B241" s="3">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
-        <v>44289</v>
+        <v>44296</v>
       </c>
       <c r="B242" s="3">
-        <v>30383</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
-        <v>44288</v>
+        <v>44295</v>
       </c>
       <c r="B243" s="3">
-        <v>29796</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B244" s="4"/>
+        <v>44294</v>
+      </c>
+      <c r="B244" s="3">
+        <v>38445</v>
+      </c>
     </row>
     <row r="245" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
-        <v>44286</v>
-      </c>
-      <c r="B245" s="4"/>
+        <v>44293</v>
+      </c>
+      <c r="B245" s="3">
+        <v>35475</v>
+      </c>
     </row>
     <row r="246" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
-        <v>44285</v>
-      </c>
-      <c r="B246" s="4"/>
+        <v>44292</v>
+      </c>
+      <c r="B246" s="3">
+        <v>31795</v>
+      </c>
     </row>
     <row r="247" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
-        <v>44284</v>
-      </c>
-      <c r="B247" s="4"/>
+        <v>44291</v>
+      </c>
+      <c r="B247" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="248" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
-        <v>44283</v>
-      </c>
-      <c r="B248" s="4"/>
+        <v>44290</v>
+      </c>
+      <c r="B248" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="249" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
-        <v>44282</v>
-      </c>
-      <c r="B249" s="4"/>
+        <v>44289</v>
+      </c>
+      <c r="B249" s="3">
+        <v>30383</v>
+      </c>
     </row>
     <row r="250" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
-        <v>44281</v>
-      </c>
-      <c r="B250" s="4"/>
+        <v>44288</v>
+      </c>
+      <c r="B250" s="3">
+        <v>29796</v>
+      </c>
     </row>
     <row r="251" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
-        <v>44280</v>
+        <v>44287</v>
       </c>
       <c r="B251" s="4"/>
     </row>
     <row r="252" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
-        <v>44279</v>
+        <v>44286</v>
       </c>
       <c r="B252" s="4"/>
     </row>
     <row r="253" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
+        <v>44285</v>
+      </c>
+      <c r="B253" s="4"/>
+    </row>
+    <row r="254" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A254" s="2">
+        <v>44284</v>
+      </c>
+      <c r="B254" s="4"/>
+    </row>
+    <row r="255" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A255" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B255" s="4"/>
+    </row>
+    <row r="256" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A256" s="2">
+        <v>44282</v>
+      </c>
+      <c r="B256" s="4"/>
+    </row>
+    <row r="257" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A257" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B257" s="4"/>
+    </row>
+    <row r="258" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A258" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B258" s="4"/>
+    </row>
+    <row r="259" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A259" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B259" s="4"/>
+    </row>
+    <row r="260" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A260" s="2">
         <v>44278</v>
       </c>
-      <c r="B253" s="4"/>
+      <c r="B260" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{0CFE7143-ADE8-A945-8A62-4628C14A0C5C}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{91D4ACBB-8FF7-E24F-9942-0CA78BD7EE64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated NZ-AU comparison charts to 14 December
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252EA913-AE7C-0E4C-9048-5518C819E9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B4F36-9055-9C4D-B4B3-ADF51E11E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54400" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
   </bookViews>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BAE720-0FFD-AC44-A3E0-A012DA41F8A8}">
-  <dimension ref="A1:B260"/>
+  <dimension ref="A1:B267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="B271" sqref="B271"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,2059 +447,2115 @@
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44536</v>
+        <v>44543</v>
       </c>
       <c r="B2" s="3">
-        <v>6396368</v>
+        <v>6419310</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44535</v>
+        <v>44542</v>
       </c>
       <c r="B3" s="3">
-        <v>6395543</v>
+        <v>6418911</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44534</v>
+        <v>44541</v>
       </c>
       <c r="B4" s="3">
-        <v>6393476</v>
+        <v>6417289</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44533</v>
+        <v>44540</v>
       </c>
       <c r="B5" s="3">
-        <v>6387955</v>
+        <v>6413287</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44532</v>
+        <v>44539</v>
       </c>
       <c r="B6" s="3">
-        <v>6383068</v>
+        <v>6409218</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44531</v>
+        <v>44538</v>
       </c>
       <c r="B7" s="3">
-        <v>6378225</v>
+        <v>6405004</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44530</v>
+        <v>44537</v>
       </c>
       <c r="B8" s="3">
-        <v>6372197</v>
+        <v>6400706</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44529</v>
+        <v>44536</v>
       </c>
       <c r="B9" s="3">
-        <v>6366060</v>
+        <v>6396368</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44528</v>
+        <v>44535</v>
       </c>
       <c r="B10" s="3">
-        <v>6365073</v>
+        <v>6395543</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44527</v>
+        <v>44534</v>
       </c>
       <c r="B11" s="3">
-        <v>6362348</v>
+        <v>6393476</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44526</v>
+        <v>44533</v>
       </c>
       <c r="B12" s="3">
-        <v>6355156</v>
+        <v>6387955</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44525</v>
+        <v>44532</v>
       </c>
       <c r="B13" s="3">
-        <v>6348980</v>
+        <v>6383068</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44524</v>
+        <v>44531</v>
       </c>
       <c r="B14" s="3">
-        <v>6341726</v>
+        <v>6378225</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44523</v>
+        <v>44530</v>
       </c>
       <c r="B15" s="3">
-        <v>6334061</v>
+        <v>6372197</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44522</v>
+        <v>44529</v>
       </c>
       <c r="B16" s="3">
-        <v>6325341</v>
+        <v>6366060</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44521</v>
+        <v>44528</v>
       </c>
       <c r="B17" s="3">
-        <v>6324333</v>
+        <v>6365073</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44520</v>
+        <v>44527</v>
       </c>
       <c r="B18" s="3">
-        <v>6320582</v>
+        <v>6362348</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44519</v>
+        <v>44526</v>
       </c>
       <c r="B19" s="3">
-        <v>6311361</v>
+        <v>6355156</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>44518</v>
+        <v>44525</v>
       </c>
       <c r="B20" s="3">
-        <v>6301870</v>
+        <v>6348980</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44517</v>
+        <v>44524</v>
       </c>
       <c r="B21" s="3">
-        <v>6291057</v>
+        <v>6341726</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44516</v>
+        <v>44523</v>
       </c>
       <c r="B22" s="3">
-        <v>6279967</v>
+        <v>6334061</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44515</v>
+        <v>44522</v>
       </c>
       <c r="B23" s="3">
-        <v>6268391</v>
+        <v>6325341</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44514</v>
+        <v>44521</v>
       </c>
       <c r="B24" s="3">
-        <v>6265758</v>
+        <v>6324333</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44513</v>
+        <v>44520</v>
       </c>
       <c r="B25" s="3">
-        <v>6259089</v>
+        <v>6320582</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44512</v>
+        <v>44519</v>
       </c>
       <c r="B26" s="3">
-        <v>6243318</v>
+        <v>6311361</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44511</v>
+        <v>44518</v>
       </c>
       <c r="B27" s="3">
-        <v>6226830</v>
+        <v>6301870</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="B28" s="3">
-        <v>6210103</v>
+        <v>6291057</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44509</v>
+        <v>44516</v>
       </c>
       <c r="B29" s="3">
-        <v>6192099</v>
+        <v>6279967</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44508</v>
+        <v>44515</v>
       </c>
       <c r="B30" s="3">
-        <v>6172372</v>
+        <v>6268391</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44507</v>
+        <v>44514</v>
       </c>
       <c r="B31" s="3">
-        <v>6168060</v>
+        <v>6265758</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44506</v>
+        <v>44513</v>
       </c>
       <c r="B32" s="3">
-        <v>6156414</v>
+        <v>6259089</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44505</v>
+        <v>44512</v>
       </c>
       <c r="B33" s="3">
-        <v>6130474</v>
+        <v>6243318</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44504</v>
+        <v>44511</v>
       </c>
       <c r="B34" s="3">
-        <v>6105744</v>
+        <v>6226830</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44503</v>
+        <v>44510</v>
       </c>
       <c r="B35" s="3">
-        <v>6077355</v>
+        <v>6210103</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44502</v>
+        <v>44509</v>
       </c>
       <c r="B36" s="3">
-        <v>6046074</v>
+        <v>6192099</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44501</v>
+        <v>44508</v>
       </c>
       <c r="B37" s="3">
-        <v>6009574</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44500</v>
+        <v>44507</v>
       </c>
       <c r="B38" s="3">
-        <v>5999926</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44499</v>
+        <v>44506</v>
       </c>
       <c r="B39" s="3">
-        <v>5977973</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44498</v>
+        <v>44505</v>
       </c>
       <c r="B40" s="3">
-        <v>5938861</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44497</v>
+        <v>44504</v>
       </c>
       <c r="B41" s="3">
-        <v>5898147</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44496</v>
+        <v>44503</v>
       </c>
       <c r="B42" s="3">
-        <v>5858123</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44495</v>
+        <v>44502</v>
       </c>
       <c r="B43" s="3">
-        <v>5818705</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44494</v>
+        <v>44501</v>
       </c>
       <c r="B44" s="3">
-        <v>5780737</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44493</v>
+        <v>44500</v>
       </c>
       <c r="B45" s="3">
-        <v>5766748</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44492</v>
+        <v>44499</v>
       </c>
       <c r="B46" s="3">
-        <v>5732872</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44491</v>
+        <v>44498</v>
       </c>
       <c r="B47" s="3">
-        <v>5677232</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44490</v>
+        <v>44497</v>
       </c>
       <c r="B48" s="3">
-        <v>5621660</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44489</v>
+        <v>44496</v>
       </c>
       <c r="B49" s="3">
-        <v>5565441</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44488</v>
+        <v>44495</v>
       </c>
       <c r="B50" s="3">
-        <v>5506563</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44487</v>
+        <v>44494</v>
       </c>
       <c r="B51" s="3">
-        <v>5440365</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>44486</v>
+        <v>44493</v>
       </c>
       <c r="B52" s="3">
-        <v>5405628</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B53" s="3">
-        <v>5364911</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>44484</v>
+        <v>44491</v>
       </c>
       <c r="B54" s="3">
-        <v>5288225</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44483</v>
+        <v>44490</v>
       </c>
       <c r="B55" s="3">
-        <v>5207377</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44482</v>
+        <v>44489</v>
       </c>
       <c r="B56" s="3">
-        <v>5116994</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>44481</v>
+        <v>44488</v>
       </c>
       <c r="B57" s="3">
-        <v>5018535</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>44480</v>
+        <v>44487</v>
       </c>
       <c r="B58" s="3">
-        <v>4925635</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44479</v>
+        <v>44486</v>
       </c>
       <c r="B59" s="3">
-        <v>4890800</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B60" s="3">
-        <v>4831173</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44477</v>
+        <v>44484</v>
       </c>
       <c r="B61" s="3">
-        <v>4738793</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>44476</v>
+        <v>44483</v>
       </c>
       <c r="B62" s="3">
-        <v>4653723</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>44475</v>
+        <v>44482</v>
       </c>
       <c r="B63" s="3">
-        <v>4567214</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>44474</v>
+        <v>44481</v>
       </c>
       <c r="B64" s="3">
-        <v>4465060</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>44473</v>
+        <v>44480</v>
       </c>
       <c r="B65" s="3">
-        <v>4449546</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44472</v>
+        <v>44479</v>
       </c>
       <c r="B66" s="3">
-        <v>4428121</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>44471</v>
+        <v>44478</v>
       </c>
       <c r="B67" s="3">
-        <v>4384051</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>44470</v>
+        <v>44477</v>
       </c>
       <c r="B68" s="3">
-        <v>4297900</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>44469</v>
+        <v>44476</v>
       </c>
       <c r="B69" s="3">
-        <v>4218516</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>44468</v>
+        <v>44475</v>
       </c>
       <c r="B70" s="3">
-        <v>4145673</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>44467</v>
+        <v>44474</v>
       </c>
       <c r="B71" s="3">
-        <v>4060612</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>44466</v>
+        <v>44473</v>
       </c>
       <c r="B72" s="3">
-        <v>3979094</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>44465</v>
+        <v>44472</v>
       </c>
       <c r="B73" s="3">
-        <v>3953132</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B74" s="3">
-        <v>3898564</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>44463</v>
+        <v>44470</v>
       </c>
       <c r="B75" s="3">
-        <v>3804258</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>44462</v>
+        <v>44469</v>
       </c>
       <c r="B76" s="3">
-        <v>3724979</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>44461</v>
+        <v>44468</v>
       </c>
       <c r="B77" s="3">
-        <v>3646849</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>44460</v>
+        <v>44467</v>
       </c>
       <c r="B78" s="3">
-        <v>3563962</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>44459</v>
+        <v>44466</v>
       </c>
       <c r="B79" s="3">
-        <v>3487539</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>44458</v>
+        <v>44465</v>
       </c>
       <c r="B80" s="3">
-        <v>3461082</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B81" s="3">
-        <v>3412016</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>44456</v>
+        <v>44463</v>
       </c>
       <c r="B82" s="3">
-        <v>3323936</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>44455</v>
+        <v>44462</v>
       </c>
       <c r="B83" s="3">
-        <v>3259323</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B84" s="3">
-        <v>3189070</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>44453</v>
+        <v>44460</v>
       </c>
       <c r="B85" s="3">
-        <v>3123699</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>44452</v>
+        <v>44459</v>
       </c>
       <c r="B86" s="3">
-        <v>3051925</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>44451</v>
+        <v>44458</v>
       </c>
       <c r="B87" s="3">
-        <v>3031072</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B88" s="3">
-        <v>2992899</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>44449</v>
+        <v>44456</v>
       </c>
       <c r="B89" s="3">
-        <v>2924263</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>44448</v>
+        <v>44455</v>
       </c>
       <c r="B90" s="3">
-        <v>2860253</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>44447</v>
+        <v>44454</v>
       </c>
       <c r="B91" s="3">
-        <v>2802011</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>44446</v>
+        <v>44453</v>
       </c>
       <c r="B92" s="3">
-        <v>2743498</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>44445</v>
+        <v>44452</v>
       </c>
       <c r="B93" s="3">
-        <v>2692904</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>44444</v>
+        <v>44451</v>
       </c>
       <c r="B94" s="3">
-        <v>2678906</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>44443</v>
+        <v>44450</v>
       </c>
       <c r="B95" s="3">
-        <v>2644865</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>44442</v>
+        <v>44449</v>
       </c>
       <c r="B96" s="3">
-        <v>2590966</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>44441</v>
+        <v>44448</v>
       </c>
       <c r="B97" s="3">
-        <v>2539287</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>44440</v>
+        <v>44447</v>
       </c>
       <c r="B98" s="3">
-        <v>2484199</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>44439</v>
+        <v>44446</v>
       </c>
       <c r="B99" s="3">
-        <v>2433592</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>44438</v>
+        <v>44445</v>
       </c>
       <c r="B100" s="3">
-        <v>2372417</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>44437</v>
+        <v>44444</v>
       </c>
       <c r="B101" s="3">
-        <v>2353563</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>44436</v>
+        <v>44443</v>
       </c>
       <c r="B102" s="3">
-        <v>2326130</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>44435</v>
+        <v>44442</v>
       </c>
       <c r="B103" s="3">
-        <v>2273984</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>44434</v>
+        <v>44441</v>
       </c>
       <c r="B104" s="3">
-        <v>2218458</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>44433</v>
+        <v>44440</v>
       </c>
       <c r="B105" s="3">
-        <v>2163192</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>44432</v>
+        <v>44439</v>
       </c>
       <c r="B106" s="3">
-        <v>2112611</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>44431</v>
+        <v>44438</v>
       </c>
       <c r="B107" s="3">
-        <v>2066915</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>44430</v>
+        <v>44437</v>
       </c>
       <c r="B108" s="3">
-        <v>2052364</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>44429</v>
+        <v>44436</v>
       </c>
       <c r="B109" s="3">
-        <v>2022928</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>44428</v>
+        <v>44435</v>
       </c>
       <c r="B110" s="3">
-        <v>1973224</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>44427</v>
+        <v>44434</v>
       </c>
       <c r="B111" s="3">
-        <v>1924839</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>44426</v>
+        <v>44433</v>
       </c>
       <c r="B112" s="3">
-        <v>1871458</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>44425</v>
+        <v>44432</v>
       </c>
       <c r="B113" s="3">
-        <v>1826165</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>44424</v>
+        <v>44431</v>
       </c>
       <c r="B114" s="3">
-        <v>1781578</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>44423</v>
+        <v>44430</v>
       </c>
       <c r="B115" s="3">
-        <v>1767176</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>44422</v>
+        <v>44429</v>
       </c>
       <c r="B116" s="3">
-        <v>1742669</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>44421</v>
+        <v>44428</v>
       </c>
       <c r="B117" s="3">
-        <v>1693577</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>44420</v>
+        <v>44427</v>
       </c>
       <c r="B118" s="3">
-        <v>1645077</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>44419</v>
+        <v>44426</v>
       </c>
       <c r="B119" s="3">
-        <v>1599438</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>44418</v>
+        <v>44425</v>
       </c>
       <c r="B120" s="3">
-        <v>1548545</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>44417</v>
+        <v>44424</v>
       </c>
       <c r="B121" s="3">
-        <v>1510648</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>44416</v>
+        <v>44423</v>
       </c>
       <c r="B122" s="3">
-        <v>1501249</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>44415</v>
+        <v>44422</v>
       </c>
       <c r="B123" s="3">
-        <v>1463495</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>44414</v>
+        <v>44421</v>
       </c>
       <c r="B124" s="3">
-        <v>1423185</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>44413</v>
+        <v>44420</v>
       </c>
       <c r="B125" s="3">
-        <v>1381481</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>44412</v>
+        <v>44419</v>
       </c>
       <c r="B126" s="3">
-        <v>1342211</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>44411</v>
+        <v>44418</v>
       </c>
       <c r="B127" s="3">
-        <v>1300394</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>44410</v>
+        <v>44417</v>
       </c>
       <c r="B128" s="3">
-        <v>1265839</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>44409</v>
+        <v>44416</v>
       </c>
       <c r="B129" s="3">
-        <v>1252304</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>44408</v>
+        <v>44415</v>
       </c>
       <c r="B130" s="3">
-        <v>1228845</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>44407</v>
+        <v>44414</v>
       </c>
       <c r="B131" s="3">
-        <v>1190942</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>44406</v>
+        <v>44413</v>
       </c>
       <c r="B132" s="3">
-        <v>1156321</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>44405</v>
+        <v>44412</v>
       </c>
       <c r="B133" s="3">
-        <v>1108405</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>44404</v>
+        <v>44411</v>
       </c>
       <c r="B134" s="3">
-        <v>1071895</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>44403</v>
+        <v>44410</v>
       </c>
       <c r="B135" s="3">
-        <v>1045515</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>44402</v>
+        <v>44409</v>
       </c>
       <c r="B136" s="3">
-        <v>1034280</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>44401</v>
+        <v>44408</v>
       </c>
       <c r="B137" s="3">
-        <v>1012939</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>44400</v>
+        <v>44407</v>
       </c>
       <c r="B138" s="3">
-        <v>982170</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>44399</v>
+        <v>44406</v>
       </c>
       <c r="B139" s="3">
-        <v>948667</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>44398</v>
+        <v>44405</v>
       </c>
       <c r="B140" s="3">
-        <v>912940</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>44397</v>
+        <v>44404</v>
       </c>
       <c r="B141" s="3">
-        <v>882844</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>44396</v>
+        <v>44403</v>
       </c>
       <c r="B142" s="3">
-        <v>854625</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>44395</v>
+        <v>44402</v>
       </c>
       <c r="B143" s="3">
-        <v>846261</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>44394</v>
+        <v>44401</v>
       </c>
       <c r="B144" s="3">
-        <v>830856</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>44393</v>
+        <v>44400</v>
       </c>
       <c r="B145" s="3">
-        <v>801520</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
-        <v>44392</v>
+        <v>44399</v>
       </c>
       <c r="B146" s="3">
-        <v>769552</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>44391</v>
+        <v>44398</v>
       </c>
       <c r="B147" s="3">
-        <v>741075</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>44390</v>
+        <v>44397</v>
       </c>
       <c r="B148" s="3">
-        <v>710714</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>44389</v>
+        <v>44396</v>
       </c>
       <c r="B149" s="3">
-        <v>686408</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
-        <v>44388</v>
+        <v>44395</v>
       </c>
       <c r="B150" s="3">
-        <v>683667</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
-        <v>44387</v>
+        <v>44394</v>
       </c>
       <c r="B151" s="3">
-        <v>671858</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
-        <v>44386</v>
+        <v>44393</v>
       </c>
       <c r="B152" s="3">
-        <v>651446</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
-        <v>44385</v>
+        <v>44392</v>
       </c>
       <c r="B153" s="3">
-        <v>629961</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
-        <v>44384</v>
+        <v>44391</v>
       </c>
       <c r="B154" s="3">
-        <v>609108</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
-        <v>44383</v>
+        <v>44390</v>
       </c>
       <c r="B155" s="3">
-        <v>586674</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
-        <v>44382</v>
+        <v>44389</v>
       </c>
       <c r="B156" s="3">
-        <v>567316</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
-        <v>44381</v>
+        <v>44388</v>
       </c>
       <c r="B157" s="3">
-        <v>564930</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
-        <v>44380</v>
+        <v>44387</v>
       </c>
       <c r="B158" s="3">
-        <v>554057</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
-        <v>44379</v>
+        <v>44386</v>
       </c>
       <c r="B159" s="3">
-        <v>534493</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
-        <v>44378</v>
+        <v>44385</v>
       </c>
       <c r="B160" s="3">
-        <v>471176</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
-        <v>44377</v>
+        <v>44384</v>
       </c>
       <c r="B161" s="3">
-        <v>471176</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
-        <v>44376</v>
+        <v>44383</v>
       </c>
       <c r="B162" s="3">
-        <v>463624</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
-        <v>44375</v>
+        <v>44382</v>
       </c>
       <c r="B163" s="3">
-        <v>396652</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
-        <v>44374</v>
+        <v>44381</v>
       </c>
       <c r="B164" s="3">
-        <v>396246</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
-        <v>44373</v>
+        <v>44380</v>
       </c>
       <c r="B165" s="3">
-        <v>392527</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
-        <v>44372</v>
+        <v>44379</v>
       </c>
       <c r="B166" s="3">
-        <v>385092</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
-        <v>44371</v>
+        <v>44378</v>
       </c>
       <c r="B167" s="3">
-        <v>376276</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
-        <v>44370</v>
+        <v>44377</v>
       </c>
       <c r="B168" s="3">
-        <v>366660</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
-        <v>44369</v>
+        <v>44376</v>
       </c>
       <c r="B169" s="3">
-        <v>357767</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
-        <v>44368</v>
+        <v>44375</v>
       </c>
       <c r="B170" s="3">
-        <v>294981</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
-        <v>44367</v>
+        <v>44374</v>
       </c>
       <c r="B171" s="3">
-        <v>294965</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
-        <v>44366</v>
+        <v>44373</v>
       </c>
       <c r="B172" s="3">
-        <v>289941</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
-        <v>44365</v>
+        <v>44372</v>
       </c>
       <c r="B173" s="3">
-        <v>279418</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
-        <v>44364</v>
+        <v>44371</v>
       </c>
       <c r="B174" s="3">
-        <v>269824</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
-        <v>44363</v>
+        <v>44370</v>
       </c>
       <c r="B175" s="3">
-        <v>259437</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
-        <v>44362</v>
+        <v>44369</v>
       </c>
       <c r="B176" s="3">
-        <v>237250</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
-        <v>44361</v>
+        <v>44368</v>
       </c>
       <c r="B177" s="3">
-        <v>237250</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
-        <v>44360</v>
+        <v>44367</v>
       </c>
       <c r="B178" s="3">
-        <v>237250</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
-        <v>44359</v>
+        <v>44366</v>
       </c>
       <c r="B179" s="3">
-        <v>232335</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
-        <v>44358</v>
+        <v>44365</v>
       </c>
       <c r="B180" s="3">
-        <v>222807</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
-        <v>44357</v>
+        <v>44364</v>
       </c>
       <c r="B181" s="3">
-        <v>213686</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
-        <v>44356</v>
+        <v>44363</v>
       </c>
       <c r="B182" s="3">
-        <v>213686</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
-        <v>44355</v>
+        <v>44362</v>
       </c>
       <c r="B183" s="3">
-        <v>204595</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
-        <v>44354</v>
+        <v>44361</v>
       </c>
       <c r="B184" s="3">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
-        <v>44353</v>
+        <v>44360</v>
       </c>
       <c r="B185" s="3">
-        <v>180397</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
-        <v>44352</v>
+        <v>44359</v>
       </c>
       <c r="B186" s="3">
-        <v>179477</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
-        <v>44351</v>
+        <v>44358</v>
       </c>
       <c r="B187" s="3">
-        <v>175030</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
-        <v>44350</v>
+        <v>44357</v>
       </c>
       <c r="B188" s="3">
-        <v>170669</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
-        <v>44349</v>
+        <v>44356</v>
       </c>
       <c r="B189" s="3">
-        <v>167075</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
-        <v>44348</v>
+        <v>44355</v>
       </c>
       <c r="B190" s="3">
-        <v>156333</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
-        <v>44347</v>
+        <v>44354</v>
       </c>
       <c r="B191" s="3">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
-        <v>44346</v>
+        <v>44353</v>
       </c>
       <c r="B192" s="3">
-        <v>153886</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
-        <v>44345</v>
+        <v>44352</v>
       </c>
       <c r="B193" s="3">
-        <v>153886</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
-        <v>44344</v>
+        <v>44351</v>
       </c>
       <c r="B194" s="3">
-        <v>153886</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
-        <v>44343</v>
+        <v>44350</v>
       </c>
       <c r="B195" s="3">
-        <v>150552</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
-        <v>44342</v>
+        <v>44349</v>
       </c>
       <c r="B196" s="3">
-        <v>145341</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
-        <v>44341</v>
+        <v>44348</v>
       </c>
       <c r="B197" s="3">
-        <v>125810</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
-        <v>44340</v>
+        <v>44347</v>
       </c>
       <c r="B198" s="3">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
-        <v>44339</v>
+        <v>44346</v>
       </c>
       <c r="B199" s="3">
-        <v>96745</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
-        <v>44338</v>
+        <v>44345</v>
       </c>
       <c r="B200" s="3">
-        <v>96266</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
-        <v>44337</v>
+        <v>44344</v>
       </c>
       <c r="B201" s="3">
-        <v>93860</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
-        <v>44336</v>
+        <v>44343</v>
       </c>
       <c r="B202" s="3">
-        <v>91297</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
-        <v>44335</v>
+        <v>44342</v>
       </c>
       <c r="B203" s="3">
-        <v>89049</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
-        <v>44334</v>
+        <v>44341</v>
       </c>
       <c r="B204" s="3">
-        <v>87045</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
-        <v>44333</v>
+        <v>44340</v>
       </c>
       <c r="B205" s="3">
-        <v>84963</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
-        <v>44332</v>
+        <v>44339</v>
       </c>
       <c r="B206" s="3">
-        <v>84963</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
-        <v>44331</v>
+        <v>44338</v>
       </c>
       <c r="B207" s="3">
-        <v>84474</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
-        <v>44330</v>
+        <v>44337</v>
       </c>
       <c r="B208" s="3">
-        <v>82774</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
-        <v>44329</v>
+        <v>44336</v>
       </c>
       <c r="B209" s="3">
-        <v>81457</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
-        <v>44328</v>
+        <v>44335</v>
       </c>
       <c r="B210" s="3">
-        <v>80082</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
-        <v>44327</v>
+        <v>44334</v>
       </c>
       <c r="B211" s="3">
-        <v>78744</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
-        <v>44326</v>
+        <v>44333</v>
       </c>
       <c r="B212" s="3">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
-        <v>44325</v>
+        <v>44332</v>
       </c>
       <c r="B213" s="3">
-        <v>77392</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
-        <v>44324</v>
+        <v>44331</v>
       </c>
       <c r="B214" s="3">
-        <v>76908</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
-        <v>44323</v>
+        <v>44330</v>
       </c>
       <c r="B215" s="3">
-        <v>75187</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
-        <v>44322</v>
+        <v>44329</v>
       </c>
       <c r="B216" s="3">
-        <v>73270</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
-        <v>44321</v>
+        <v>44328</v>
       </c>
       <c r="B217" s="3">
-        <v>71767</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
-        <v>44320</v>
+        <v>44327</v>
       </c>
       <c r="B218" s="3">
-        <v>70039</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
-        <v>44319</v>
+        <v>44326</v>
       </c>
       <c r="B219" s="3">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
-        <v>44318</v>
+        <v>44325</v>
       </c>
       <c r="B220" s="3">
-        <v>68656</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
-        <v>44317</v>
+        <v>44324</v>
       </c>
       <c r="B221" s="3">
-        <v>68472</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
-        <v>44316</v>
+        <v>44323</v>
       </c>
       <c r="B222" s="3">
-        <v>67149</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
-        <v>44315</v>
+        <v>44322</v>
       </c>
       <c r="B223" s="3">
-        <v>65948</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
-        <v>44314</v>
+        <v>44321</v>
       </c>
       <c r="B224" s="3">
-        <v>64910</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
-        <v>44313</v>
+        <v>44320</v>
       </c>
       <c r="B225" s="3">
-        <v>63944</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
-        <v>44312</v>
+        <v>44319</v>
       </c>
       <c r="B226" s="3">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
-        <v>44311</v>
+        <v>44318</v>
       </c>
       <c r="B227" s="3">
-        <v>63537</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
-        <v>44310</v>
+        <v>44317</v>
       </c>
       <c r="B228" s="3">
-        <v>63317</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
-        <v>44309</v>
+        <v>44316</v>
       </c>
       <c r="B229" s="3">
-        <v>62491</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
-        <v>44308</v>
+        <v>44315</v>
       </c>
       <c r="B230" s="3">
-        <v>60582</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
-        <v>44307</v>
+        <v>44314</v>
       </c>
       <c r="B231" s="3">
-        <v>58662</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
-        <v>44306</v>
+        <v>44313</v>
       </c>
       <c r="B232" s="3">
-        <v>54736</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
-        <v>44305</v>
+        <v>44312</v>
       </c>
       <c r="B233" s="3">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
-        <v>44304</v>
+        <v>44311</v>
       </c>
       <c r="B234" s="3">
-        <v>54668</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
-        <v>44303</v>
+        <v>44310</v>
       </c>
       <c r="B235" s="3">
-        <v>54555</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
-        <v>44302</v>
+        <v>44309</v>
       </c>
       <c r="B236" s="3">
-        <v>52537</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
-        <v>44301</v>
+        <v>44308</v>
       </c>
       <c r="B237" s="3">
-        <v>50388</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
-        <v>44300</v>
+        <v>44307</v>
       </c>
       <c r="B238" s="3">
-        <v>48482</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
-        <v>44299</v>
+        <v>44306</v>
       </c>
       <c r="B239" s="3">
-        <v>46400</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
-        <v>44298</v>
+        <v>44305</v>
       </c>
       <c r="B240" s="3">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
-        <v>44297</v>
+        <v>44304</v>
       </c>
       <c r="B241" s="3">
-        <v>44208</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
-        <v>44296</v>
+        <v>44303</v>
       </c>
       <c r="B242" s="3">
-        <v>44016</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
-        <v>44295</v>
+        <v>44302</v>
       </c>
       <c r="B243" s="3">
-        <v>41376</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
-        <v>44294</v>
+        <v>44301</v>
       </c>
       <c r="B244" s="3">
-        <v>38445</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
-        <v>44293</v>
+        <v>44300</v>
       </c>
       <c r="B245" s="3">
-        <v>35475</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
-        <v>44292</v>
+        <v>44299</v>
       </c>
       <c r="B246" s="3">
-        <v>31795</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
-        <v>44291</v>
+        <v>44298</v>
       </c>
       <c r="B247" s="3">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
-        <v>44290</v>
+        <v>44297</v>
       </c>
       <c r="B248" s="3">
-        <v>31212</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
-        <v>44289</v>
+        <v>44296</v>
       </c>
       <c r="B249" s="3">
-        <v>30383</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
-        <v>44288</v>
+        <v>44295</v>
       </c>
       <c r="B250" s="3">
-        <v>29796</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B251" s="4"/>
+        <v>44294</v>
+      </c>
+      <c r="B251" s="3">
+        <v>38445</v>
+      </c>
     </row>
     <row r="252" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
-        <v>44286</v>
-      </c>
-      <c r="B252" s="4"/>
+        <v>44293</v>
+      </c>
+      <c r="B252" s="3">
+        <v>35475</v>
+      </c>
     </row>
     <row r="253" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
-        <v>44285</v>
-      </c>
-      <c r="B253" s="4"/>
+        <v>44292</v>
+      </c>
+      <c r="B253" s="3">
+        <v>31795</v>
+      </c>
     </row>
     <row r="254" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
-        <v>44284</v>
-      </c>
-      <c r="B254" s="4"/>
+        <v>44291</v>
+      </c>
+      <c r="B254" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="255" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
-        <v>44283</v>
-      </c>
-      <c r="B255" s="4"/>
+        <v>44290</v>
+      </c>
+      <c r="B255" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="256" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
-        <v>44282</v>
-      </c>
-      <c r="B256" s="4"/>
+        <v>44289</v>
+      </c>
+      <c r="B256" s="3">
+        <v>30383</v>
+      </c>
     </row>
     <row r="257" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
-        <v>44281</v>
-      </c>
-      <c r="B257" s="4"/>
+        <v>44288</v>
+      </c>
+      <c r="B257" s="3">
+        <v>29796</v>
+      </c>
     </row>
     <row r="258" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
-        <v>44280</v>
+        <v>44287</v>
       </c>
       <c r="B258" s="4"/>
     </row>
     <row r="259" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
-        <v>44279</v>
+        <v>44286</v>
       </c>
       <c r="B259" s="4"/>
     </row>
     <row r="260" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
+        <v>44285</v>
+      </c>
+      <c r="B260" s="4"/>
+    </row>
+    <row r="261" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A261" s="2">
+        <v>44284</v>
+      </c>
+      <c r="B261" s="4"/>
+    </row>
+    <row r="262" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A262" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B262" s="4"/>
+    </row>
+    <row r="263" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A263" s="2">
+        <v>44282</v>
+      </c>
+      <c r="B263" s="4"/>
+    </row>
+    <row r="264" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A264" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B264" s="4"/>
+    </row>
+    <row r="265" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A265" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B265" s="4"/>
+    </row>
+    <row r="266" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A266" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B266" s="4"/>
+    </row>
+    <row r="267" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A267" s="2">
         <v>44278</v>
       </c>
-      <c r="B260" s="4"/>
+      <c r="B267" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{91D4ACBB-8FF7-E24F-9942-0CA78BD7EE64}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{07D2E571-3882-CE4D-943E-FB5D21A4041C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
special update of NZ-AU comparison charts to 17 December
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B4F36-9055-9C4D-B4B3-ADF51E11E82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA73C90-709C-5F46-BD84-6392DB6D108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BAE720-0FFD-AC44-A3E0-A012DA41F8A8}">
-  <dimension ref="A1:B267"/>
+  <dimension ref="A1:B270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,1599 +447,1599 @@
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44543</v>
+        <v>44546</v>
       </c>
       <c r="B2" s="3">
-        <v>6419310</v>
+        <v>6429276</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44542</v>
+        <v>44545</v>
       </c>
       <c r="B3" s="3">
-        <v>6418911</v>
+        <v>6426296</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44541</v>
+        <v>44544</v>
       </c>
       <c r="B4" s="3">
-        <v>6417289</v>
+        <v>6422891</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44540</v>
+        <v>44543</v>
       </c>
       <c r="B5" s="3">
-        <v>6413287</v>
+        <v>6419310</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44539</v>
+        <v>44542</v>
       </c>
       <c r="B6" s="3">
-        <v>6409218</v>
+        <v>6418911</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44538</v>
+        <v>44541</v>
       </c>
       <c r="B7" s="3">
-        <v>6405004</v>
+        <v>6417289</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44537</v>
+        <v>44540</v>
       </c>
       <c r="B8" s="3">
-        <v>6400706</v>
+        <v>6413287</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44536</v>
+        <v>44539</v>
       </c>
       <c r="B9" s="3">
-        <v>6396368</v>
+        <v>6409218</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44535</v>
+        <v>44538</v>
       </c>
       <c r="B10" s="3">
-        <v>6395543</v>
+        <v>6405004</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44534</v>
+        <v>44537</v>
       </c>
       <c r="B11" s="3">
-        <v>6393476</v>
+        <v>6400706</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44533</v>
+        <v>44536</v>
       </c>
       <c r="B12" s="3">
-        <v>6387955</v>
+        <v>6396368</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44532</v>
+        <v>44535</v>
       </c>
       <c r="B13" s="3">
-        <v>6383068</v>
+        <v>6395543</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44531</v>
+        <v>44534</v>
       </c>
       <c r="B14" s="3">
-        <v>6378225</v>
+        <v>6393476</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44530</v>
+        <v>44533</v>
       </c>
       <c r="B15" s="3">
-        <v>6372197</v>
+        <v>6387955</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44529</v>
+        <v>44532</v>
       </c>
       <c r="B16" s="3">
-        <v>6366060</v>
+        <v>6383068</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44528</v>
+        <v>44531</v>
       </c>
       <c r="B17" s="3">
-        <v>6365073</v>
+        <v>6378225</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44527</v>
+        <v>44530</v>
       </c>
       <c r="B18" s="3">
-        <v>6362348</v>
+        <v>6372197</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44526</v>
+        <v>44529</v>
       </c>
       <c r="B19" s="3">
-        <v>6355156</v>
+        <v>6366060</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>44525</v>
+        <v>44528</v>
       </c>
       <c r="B20" s="3">
-        <v>6348980</v>
+        <v>6365073</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44524</v>
+        <v>44527</v>
       </c>
       <c r="B21" s="3">
-        <v>6341726</v>
+        <v>6362348</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44523</v>
+        <v>44526</v>
       </c>
       <c r="B22" s="3">
-        <v>6334061</v>
+        <v>6355156</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44522</v>
+        <v>44525</v>
       </c>
       <c r="B23" s="3">
-        <v>6325341</v>
+        <v>6348980</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44521</v>
+        <v>44524</v>
       </c>
       <c r="B24" s="3">
-        <v>6324333</v>
+        <v>6341726</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44520</v>
+        <v>44523</v>
       </c>
       <c r="B25" s="3">
-        <v>6320582</v>
+        <v>6334061</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44519</v>
+        <v>44522</v>
       </c>
       <c r="B26" s="3">
-        <v>6311361</v>
+        <v>6325341</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44518</v>
+        <v>44521</v>
       </c>
       <c r="B27" s="3">
-        <v>6301870</v>
+        <v>6324333</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44517</v>
+        <v>44520</v>
       </c>
       <c r="B28" s="3">
-        <v>6291057</v>
+        <v>6320582</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44516</v>
+        <v>44519</v>
       </c>
       <c r="B29" s="3">
-        <v>6279967</v>
+        <v>6311361</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44515</v>
+        <v>44518</v>
       </c>
       <c r="B30" s="3">
-        <v>6268391</v>
+        <v>6301870</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44514</v>
+        <v>44517</v>
       </c>
       <c r="B31" s="3">
-        <v>6265758</v>
+        <v>6291057</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44513</v>
+        <v>44516</v>
       </c>
       <c r="B32" s="3">
-        <v>6259089</v>
+        <v>6279967</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44512</v>
+        <v>44515</v>
       </c>
       <c r="B33" s="3">
-        <v>6243318</v>
+        <v>6268391</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44511</v>
+        <v>44514</v>
       </c>
       <c r="B34" s="3">
-        <v>6226830</v>
+        <v>6265758</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44510</v>
+        <v>44513</v>
       </c>
       <c r="B35" s="3">
-        <v>6210103</v>
+        <v>6259089</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44509</v>
+        <v>44512</v>
       </c>
       <c r="B36" s="3">
-        <v>6192099</v>
+        <v>6243318</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44508</v>
+        <v>44511</v>
       </c>
       <c r="B37" s="3">
-        <v>6172372</v>
+        <v>6226830</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44507</v>
+        <v>44510</v>
       </c>
       <c r="B38" s="3">
-        <v>6168060</v>
+        <v>6210103</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44506</v>
+        <v>44509</v>
       </c>
       <c r="B39" s="3">
-        <v>6156414</v>
+        <v>6192099</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44505</v>
+        <v>44508</v>
       </c>
       <c r="B40" s="3">
-        <v>6130474</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44504</v>
+        <v>44507</v>
       </c>
       <c r="B41" s="3">
-        <v>6105744</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44503</v>
+        <v>44506</v>
       </c>
       <c r="B42" s="3">
-        <v>6077355</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44502</v>
+        <v>44505</v>
       </c>
       <c r="B43" s="3">
-        <v>6046074</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44501</v>
+        <v>44504</v>
       </c>
       <c r="B44" s="3">
-        <v>6009574</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44500</v>
+        <v>44503</v>
       </c>
       <c r="B45" s="3">
-        <v>5999926</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44499</v>
+        <v>44502</v>
       </c>
       <c r="B46" s="3">
-        <v>5977973</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44498</v>
+        <v>44501</v>
       </c>
       <c r="B47" s="3">
-        <v>5938861</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44497</v>
+        <v>44500</v>
       </c>
       <c r="B48" s="3">
-        <v>5898147</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44496</v>
+        <v>44499</v>
       </c>
       <c r="B49" s="3">
-        <v>5858123</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44495</v>
+        <v>44498</v>
       </c>
       <c r="B50" s="3">
-        <v>5818705</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44494</v>
+        <v>44497</v>
       </c>
       <c r="B51" s="3">
-        <v>5780737</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>44493</v>
+        <v>44496</v>
       </c>
       <c r="B52" s="3">
-        <v>5766748</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44492</v>
+        <v>44495</v>
       </c>
       <c r="B53" s="3">
-        <v>5732872</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>44491</v>
+        <v>44494</v>
       </c>
       <c r="B54" s="3">
-        <v>5677232</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44490</v>
+        <v>44493</v>
       </c>
       <c r="B55" s="3">
-        <v>5621660</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44489</v>
+        <v>44492</v>
       </c>
       <c r="B56" s="3">
-        <v>5565441</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>44488</v>
+        <v>44491</v>
       </c>
       <c r="B57" s="3">
-        <v>5506563</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>44487</v>
+        <v>44490</v>
       </c>
       <c r="B58" s="3">
-        <v>5440365</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44486</v>
+        <v>44489</v>
       </c>
       <c r="B59" s="3">
-        <v>5405628</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>44485</v>
+        <v>44488</v>
       </c>
       <c r="B60" s="3">
-        <v>5364911</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44484</v>
+        <v>44487</v>
       </c>
       <c r="B61" s="3">
-        <v>5288225</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>44483</v>
+        <v>44486</v>
       </c>
       <c r="B62" s="3">
-        <v>5207377</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>44482</v>
+        <v>44485</v>
       </c>
       <c r="B63" s="3">
-        <v>5116994</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>44481</v>
+        <v>44484</v>
       </c>
       <c r="B64" s="3">
-        <v>5018535</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>44480</v>
+        <v>44483</v>
       </c>
       <c r="B65" s="3">
-        <v>4925635</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44479</v>
+        <v>44482</v>
       </c>
       <c r="B66" s="3">
-        <v>4890800</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>44478</v>
+        <v>44481</v>
       </c>
       <c r="B67" s="3">
-        <v>4831173</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>44477</v>
+        <v>44480</v>
       </c>
       <c r="B68" s="3">
-        <v>4738793</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>44476</v>
+        <v>44479</v>
       </c>
       <c r="B69" s="3">
-        <v>4653723</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>44475</v>
+        <v>44478</v>
       </c>
       <c r="B70" s="3">
-        <v>4567214</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>44474</v>
+        <v>44477</v>
       </c>
       <c r="B71" s="3">
-        <v>4465060</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>44473</v>
+        <v>44476</v>
       </c>
       <c r="B72" s="3">
-        <v>4449546</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>44472</v>
+        <v>44475</v>
       </c>
       <c r="B73" s="3">
-        <v>4428121</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>44471</v>
+        <v>44474</v>
       </c>
       <c r="B74" s="3">
-        <v>4384051</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>44470</v>
+        <v>44473</v>
       </c>
       <c r="B75" s="3">
-        <v>4297900</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>44469</v>
+        <v>44472</v>
       </c>
       <c r="B76" s="3">
-        <v>4218516</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>44468</v>
+        <v>44471</v>
       </c>
       <c r="B77" s="3">
-        <v>4145673</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>44467</v>
+        <v>44470</v>
       </c>
       <c r="B78" s="3">
-        <v>4060612</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>44466</v>
+        <v>44469</v>
       </c>
       <c r="B79" s="3">
-        <v>3979094</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>44465</v>
+        <v>44468</v>
       </c>
       <c r="B80" s="3">
-        <v>3953132</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>44464</v>
+        <v>44467</v>
       </c>
       <c r="B81" s="3">
-        <v>3898564</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>44463</v>
+        <v>44466</v>
       </c>
       <c r="B82" s="3">
-        <v>3804258</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>44462</v>
+        <v>44465</v>
       </c>
       <c r="B83" s="3">
-        <v>3724979</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>44461</v>
+        <v>44464</v>
       </c>
       <c r="B84" s="3">
-        <v>3646849</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B85" s="3">
-        <v>3563962</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>44459</v>
+        <v>44462</v>
       </c>
       <c r="B86" s="3">
-        <v>3487539</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>44458</v>
+        <v>44461</v>
       </c>
       <c r="B87" s="3">
-        <v>3461082</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>44457</v>
+        <v>44460</v>
       </c>
       <c r="B88" s="3">
-        <v>3412016</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>44456</v>
+        <v>44459</v>
       </c>
       <c r="B89" s="3">
-        <v>3323936</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>44455</v>
+        <v>44458</v>
       </c>
       <c r="B90" s="3">
-        <v>3259323</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>44454</v>
+        <v>44457</v>
       </c>
       <c r="B91" s="3">
-        <v>3189070</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>44453</v>
+        <v>44456</v>
       </c>
       <c r="B92" s="3">
-        <v>3123699</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>44452</v>
+        <v>44455</v>
       </c>
       <c r="B93" s="3">
-        <v>3051925</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>44451</v>
+        <v>44454</v>
       </c>
       <c r="B94" s="3">
-        <v>3031072</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>44450</v>
+        <v>44453</v>
       </c>
       <c r="B95" s="3">
-        <v>2992899</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>44449</v>
+        <v>44452</v>
       </c>
       <c r="B96" s="3">
-        <v>2924263</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>44448</v>
+        <v>44451</v>
       </c>
       <c r="B97" s="3">
-        <v>2860253</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>44447</v>
+        <v>44450</v>
       </c>
       <c r="B98" s="3">
-        <v>2802011</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>44446</v>
+        <v>44449</v>
       </c>
       <c r="B99" s="3">
-        <v>2743498</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>44445</v>
+        <v>44448</v>
       </c>
       <c r="B100" s="3">
-        <v>2692904</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>44444</v>
+        <v>44447</v>
       </c>
       <c r="B101" s="3">
-        <v>2678906</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>44443</v>
+        <v>44446</v>
       </c>
       <c r="B102" s="3">
-        <v>2644865</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>44442</v>
+        <v>44445</v>
       </c>
       <c r="B103" s="3">
-        <v>2590966</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>44441</v>
+        <v>44444</v>
       </c>
       <c r="B104" s="3">
-        <v>2539287</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>44440</v>
+        <v>44443</v>
       </c>
       <c r="B105" s="3">
-        <v>2484199</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>44439</v>
+        <v>44442</v>
       </c>
       <c r="B106" s="3">
-        <v>2433592</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>44438</v>
+        <v>44441</v>
       </c>
       <c r="B107" s="3">
-        <v>2372417</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>44437</v>
+        <v>44440</v>
       </c>
       <c r="B108" s="3">
-        <v>2353563</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>44436</v>
+        <v>44439</v>
       </c>
       <c r="B109" s="3">
-        <v>2326130</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>44435</v>
+        <v>44438</v>
       </c>
       <c r="B110" s="3">
-        <v>2273984</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>44434</v>
+        <v>44437</v>
       </c>
       <c r="B111" s="3">
-        <v>2218458</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>44433</v>
+        <v>44436</v>
       </c>
       <c r="B112" s="3">
-        <v>2163192</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>44432</v>
+        <v>44435</v>
       </c>
       <c r="B113" s="3">
-        <v>2112611</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>44431</v>
+        <v>44434</v>
       </c>
       <c r="B114" s="3">
-        <v>2066915</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>44430</v>
+        <v>44433</v>
       </c>
       <c r="B115" s="3">
-        <v>2052364</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>44429</v>
+        <v>44432</v>
       </c>
       <c r="B116" s="3">
-        <v>2022928</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>44428</v>
+        <v>44431</v>
       </c>
       <c r="B117" s="3">
-        <v>1973224</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>44427</v>
+        <v>44430</v>
       </c>
       <c r="B118" s="3">
-        <v>1924839</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>44426</v>
+        <v>44429</v>
       </c>
       <c r="B119" s="3">
-        <v>1871458</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>44425</v>
+        <v>44428</v>
       </c>
       <c r="B120" s="3">
-        <v>1826165</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>44424</v>
+        <v>44427</v>
       </c>
       <c r="B121" s="3">
-        <v>1781578</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>44423</v>
+        <v>44426</v>
       </c>
       <c r="B122" s="3">
-        <v>1767176</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>44422</v>
+        <v>44425</v>
       </c>
       <c r="B123" s="3">
-        <v>1742669</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>44421</v>
+        <v>44424</v>
       </c>
       <c r="B124" s="3">
-        <v>1693577</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>44420</v>
+        <v>44423</v>
       </c>
       <c r="B125" s="3">
-        <v>1645077</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>44419</v>
+        <v>44422</v>
       </c>
       <c r="B126" s="3">
-        <v>1599438</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>44418</v>
+        <v>44421</v>
       </c>
       <c r="B127" s="3">
-        <v>1548545</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>44417</v>
+        <v>44420</v>
       </c>
       <c r="B128" s="3">
-        <v>1510648</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>44416</v>
+        <v>44419</v>
       </c>
       <c r="B129" s="3">
-        <v>1501249</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>44415</v>
+        <v>44418</v>
       </c>
       <c r="B130" s="3">
-        <v>1463495</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="B131" s="3">
-        <v>1423185</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>44413</v>
+        <v>44416</v>
       </c>
       <c r="B132" s="3">
-        <v>1381481</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>44412</v>
+        <v>44415</v>
       </c>
       <c r="B133" s="3">
-        <v>1342211</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>44411</v>
+        <v>44414</v>
       </c>
       <c r="B134" s="3">
-        <v>1300394</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>44410</v>
+        <v>44413</v>
       </c>
       <c r="B135" s="3">
-        <v>1265839</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>44409</v>
+        <v>44412</v>
       </c>
       <c r="B136" s="3">
-        <v>1252304</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>44408</v>
+        <v>44411</v>
       </c>
       <c r="B137" s="3">
-        <v>1228845</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>44407</v>
+        <v>44410</v>
       </c>
       <c r="B138" s="3">
-        <v>1190942</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>44406</v>
+        <v>44409</v>
       </c>
       <c r="B139" s="3">
-        <v>1156321</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>44405</v>
+        <v>44408</v>
       </c>
       <c r="B140" s="3">
-        <v>1108405</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>44404</v>
+        <v>44407</v>
       </c>
       <c r="B141" s="3">
-        <v>1071895</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>44403</v>
+        <v>44406</v>
       </c>
       <c r="B142" s="3">
-        <v>1045515</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>44402</v>
+        <v>44405</v>
       </c>
       <c r="B143" s="3">
-        <v>1034280</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>44401</v>
+        <v>44404</v>
       </c>
       <c r="B144" s="3">
-        <v>1012939</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>44400</v>
+        <v>44403</v>
       </c>
       <c r="B145" s="3">
-        <v>982170</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
-        <v>44399</v>
+        <v>44402</v>
       </c>
       <c r="B146" s="3">
-        <v>948667</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>44398</v>
+        <v>44401</v>
       </c>
       <c r="B147" s="3">
-        <v>912940</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>44397</v>
+        <v>44400</v>
       </c>
       <c r="B148" s="3">
-        <v>882844</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>44396</v>
+        <v>44399</v>
       </c>
       <c r="B149" s="3">
-        <v>854625</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
-        <v>44395</v>
+        <v>44398</v>
       </c>
       <c r="B150" s="3">
-        <v>846261</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
-        <v>44394</v>
+        <v>44397</v>
       </c>
       <c r="B151" s="3">
-        <v>830856</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
-        <v>44393</v>
+        <v>44396</v>
       </c>
       <c r="B152" s="3">
-        <v>801520</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
-        <v>44392</v>
+        <v>44395</v>
       </c>
       <c r="B153" s="3">
-        <v>769552</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
-        <v>44391</v>
+        <v>44394</v>
       </c>
       <c r="B154" s="3">
-        <v>741075</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
-        <v>44390</v>
+        <v>44393</v>
       </c>
       <c r="B155" s="3">
-        <v>710714</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
-        <v>44389</v>
+        <v>44392</v>
       </c>
       <c r="B156" s="3">
-        <v>686408</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
-        <v>44388</v>
+        <v>44391</v>
       </c>
       <c r="B157" s="3">
-        <v>683667</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
-        <v>44387</v>
+        <v>44390</v>
       </c>
       <c r="B158" s="3">
-        <v>671858</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
-        <v>44386</v>
+        <v>44389</v>
       </c>
       <c r="B159" s="3">
-        <v>651446</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
-        <v>44385</v>
+        <v>44388</v>
       </c>
       <c r="B160" s="3">
-        <v>629961</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
-        <v>44384</v>
+        <v>44387</v>
       </c>
       <c r="B161" s="3">
-        <v>609108</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
-        <v>44383</v>
+        <v>44386</v>
       </c>
       <c r="B162" s="3">
-        <v>586674</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
-        <v>44382</v>
+        <v>44385</v>
       </c>
       <c r="B163" s="3">
-        <v>567316</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
-        <v>44381</v>
+        <v>44384</v>
       </c>
       <c r="B164" s="3">
-        <v>564930</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
-        <v>44380</v>
+        <v>44383</v>
       </c>
       <c r="B165" s="3">
-        <v>554057</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
-        <v>44379</v>
+        <v>44382</v>
       </c>
       <c r="B166" s="3">
-        <v>534493</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
-        <v>44378</v>
+        <v>44381</v>
       </c>
       <c r="B167" s="3">
-        <v>471176</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
-        <v>44377</v>
+        <v>44380</v>
       </c>
       <c r="B168" s="3">
-        <v>471176</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
-        <v>44376</v>
+        <v>44379</v>
       </c>
       <c r="B169" s="3">
-        <v>463624</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
-        <v>44375</v>
+        <v>44378</v>
       </c>
       <c r="B170" s="3">
-        <v>396652</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
-        <v>44374</v>
+        <v>44377</v>
       </c>
       <c r="B171" s="3">
-        <v>396246</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
-        <v>44373</v>
+        <v>44376</v>
       </c>
       <c r="B172" s="3">
-        <v>392527</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
-        <v>44372</v>
+        <v>44375</v>
       </c>
       <c r="B173" s="3">
-        <v>385092</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
-        <v>44371</v>
+        <v>44374</v>
       </c>
       <c r="B174" s="3">
-        <v>376276</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
-        <v>44370</v>
+        <v>44373</v>
       </c>
       <c r="B175" s="3">
-        <v>366660</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
-        <v>44369</v>
+        <v>44372</v>
       </c>
       <c r="B176" s="3">
-        <v>357767</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
-        <v>44368</v>
+        <v>44371</v>
       </c>
       <c r="B177" s="3">
-        <v>294981</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
-        <v>44367</v>
+        <v>44370</v>
       </c>
       <c r="B178" s="3">
-        <v>294965</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
-        <v>44366</v>
+        <v>44369</v>
       </c>
       <c r="B179" s="3">
-        <v>289941</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
-        <v>44365</v>
+        <v>44368</v>
       </c>
       <c r="B180" s="3">
-        <v>279418</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
-        <v>44364</v>
+        <v>44367</v>
       </c>
       <c r="B181" s="3">
-        <v>269824</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
-        <v>44363</v>
+        <v>44366</v>
       </c>
       <c r="B182" s="3">
-        <v>259437</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
-        <v>44362</v>
+        <v>44365</v>
       </c>
       <c r="B183" s="3">
-        <v>237250</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
-        <v>44361</v>
+        <v>44364</v>
       </c>
       <c r="B184" s="3">
-        <v>237250</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
-        <v>44360</v>
+        <v>44363</v>
       </c>
       <c r="B185" s="3">
-        <v>237250</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
-        <v>44359</v>
+        <v>44362</v>
       </c>
       <c r="B186" s="3">
-        <v>232335</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
-        <v>44358</v>
+        <v>44361</v>
       </c>
       <c r="B187" s="3">
-        <v>222807</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
-        <v>44357</v>
+        <v>44360</v>
       </c>
       <c r="B188" s="3">
-        <v>213686</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
-        <v>44356</v>
+        <v>44359</v>
       </c>
       <c r="B189" s="3">
-        <v>213686</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
-        <v>44355</v>
+        <v>44358</v>
       </c>
       <c r="B190" s="3">
-        <v>204595</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
-        <v>44354</v>
+        <v>44357</v>
       </c>
       <c r="B191" s="3">
-        <v>180397</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
-        <v>44353</v>
+        <v>44356</v>
       </c>
       <c r="B192" s="3">
-        <v>180397</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
-        <v>44352</v>
+        <v>44355</v>
       </c>
       <c r="B193" s="3">
-        <v>179477</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
-        <v>44351</v>
+        <v>44354</v>
       </c>
       <c r="B194" s="3">
-        <v>175030</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
-        <v>44350</v>
+        <v>44353</v>
       </c>
       <c r="B195" s="3">
-        <v>170669</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
-        <v>44349</v>
+        <v>44352</v>
       </c>
       <c r="B196" s="3">
-        <v>167075</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
-        <v>44348</v>
+        <v>44351</v>
       </c>
       <c r="B197" s="3">
-        <v>156333</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
-        <v>44347</v>
+        <v>44350</v>
       </c>
       <c r="B198" s="3">
-        <v>153886</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
-        <v>44346</v>
+        <v>44349</v>
       </c>
       <c r="B199" s="3">
-        <v>153886</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
-        <v>44345</v>
+        <v>44348</v>
       </c>
       <c r="B200" s="3">
-        <v>153886</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
-        <v>44344</v>
+        <v>44347</v>
       </c>
       <c r="B201" s="3">
         <v>153886</v>
@@ -2047,515 +2047,539 @@
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
-        <v>44343</v>
+        <v>44346</v>
       </c>
       <c r="B202" s="3">
-        <v>150552</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
-        <v>44342</v>
+        <v>44345</v>
       </c>
       <c r="B203" s="3">
-        <v>145341</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
-        <v>44341</v>
+        <v>44344</v>
       </c>
       <c r="B204" s="3">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
-        <v>44340</v>
+        <v>44343</v>
       </c>
       <c r="B205" s="3">
-        <v>125810</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
-        <v>44339</v>
+        <v>44342</v>
       </c>
       <c r="B206" s="3">
-        <v>96745</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
-        <v>44338</v>
+        <v>44341</v>
       </c>
       <c r="B207" s="3">
-        <v>96266</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
-        <v>44337</v>
+        <v>44340</v>
       </c>
       <c r="B208" s="3">
-        <v>93860</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
-        <v>44336</v>
+        <v>44339</v>
       </c>
       <c r="B209" s="3">
-        <v>91297</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
-        <v>44335</v>
+        <v>44338</v>
       </c>
       <c r="B210" s="3">
-        <v>89049</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
-        <v>44334</v>
+        <v>44337</v>
       </c>
       <c r="B211" s="3">
-        <v>87045</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
-        <v>44333</v>
+        <v>44336</v>
       </c>
       <c r="B212" s="3">
-        <v>84963</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
-        <v>44332</v>
+        <v>44335</v>
       </c>
       <c r="B213" s="3">
-        <v>84963</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
-        <v>44331</v>
+        <v>44334</v>
       </c>
       <c r="B214" s="3">
-        <v>84474</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
-        <v>44330</v>
+        <v>44333</v>
       </c>
       <c r="B215" s="3">
-        <v>82774</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
-        <v>44329</v>
+        <v>44332</v>
       </c>
       <c r="B216" s="3">
-        <v>81457</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
-        <v>44328</v>
+        <v>44331</v>
       </c>
       <c r="B217" s="3">
-        <v>80082</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
-        <v>44327</v>
+        <v>44330</v>
       </c>
       <c r="B218" s="3">
-        <v>78744</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
-        <v>44326</v>
+        <v>44329</v>
       </c>
       <c r="B219" s="3">
-        <v>77392</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
-        <v>44325</v>
+        <v>44328</v>
       </c>
       <c r="B220" s="3">
-        <v>77392</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
-        <v>44324</v>
+        <v>44327</v>
       </c>
       <c r="B221" s="3">
-        <v>76908</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
-        <v>44323</v>
+        <v>44326</v>
       </c>
       <c r="B222" s="3">
-        <v>75187</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
-        <v>44322</v>
+        <v>44325</v>
       </c>
       <c r="B223" s="3">
-        <v>73270</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
-        <v>44321</v>
+        <v>44324</v>
       </c>
       <c r="B224" s="3">
-        <v>71767</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
-        <v>44320</v>
+        <v>44323</v>
       </c>
       <c r="B225" s="3">
-        <v>70039</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
-        <v>44319</v>
+        <v>44322</v>
       </c>
       <c r="B226" s="3">
-        <v>68656</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
-        <v>44318</v>
+        <v>44321</v>
       </c>
       <c r="B227" s="3">
-        <v>68656</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
-        <v>44317</v>
+        <v>44320</v>
       </c>
       <c r="B228" s="3">
-        <v>68472</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
-        <v>44316</v>
+        <v>44319</v>
       </c>
       <c r="B229" s="3">
-        <v>67149</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
-        <v>44315</v>
+        <v>44318</v>
       </c>
       <c r="B230" s="3">
-        <v>65948</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
-        <v>44314</v>
+        <v>44317</v>
       </c>
       <c r="B231" s="3">
-        <v>64910</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
-        <v>44313</v>
+        <v>44316</v>
       </c>
       <c r="B232" s="3">
-        <v>63944</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
-        <v>44312</v>
+        <v>44315</v>
       </c>
       <c r="B233" s="3">
-        <v>63537</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
-        <v>44311</v>
+        <v>44314</v>
       </c>
       <c r="B234" s="3">
-        <v>63537</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
-        <v>44310</v>
+        <v>44313</v>
       </c>
       <c r="B235" s="3">
-        <v>63317</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
-        <v>44309</v>
+        <v>44312</v>
       </c>
       <c r="B236" s="3">
-        <v>62491</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
-        <v>44308</v>
+        <v>44311</v>
       </c>
       <c r="B237" s="3">
-        <v>60582</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
-        <v>44307</v>
+        <v>44310</v>
       </c>
       <c r="B238" s="3">
-        <v>58662</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
-        <v>44306</v>
+        <v>44309</v>
       </c>
       <c r="B239" s="3">
-        <v>54736</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
-        <v>44305</v>
+        <v>44308</v>
       </c>
       <c r="B240" s="3">
-        <v>54668</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
-        <v>44304</v>
+        <v>44307</v>
       </c>
       <c r="B241" s="3">
-        <v>54668</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
-        <v>44303</v>
+        <v>44306</v>
       </c>
       <c r="B242" s="3">
-        <v>54555</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
-        <v>44302</v>
+        <v>44305</v>
       </c>
       <c r="B243" s="3">
-        <v>52537</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
-        <v>44301</v>
+        <v>44304</v>
       </c>
       <c r="B244" s="3">
-        <v>50388</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
-        <v>44300</v>
+        <v>44303</v>
       </c>
       <c r="B245" s="3">
-        <v>48482</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
-        <v>44299</v>
+        <v>44302</v>
       </c>
       <c r="B246" s="3">
-        <v>46400</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
-        <v>44298</v>
+        <v>44301</v>
       </c>
       <c r="B247" s="3">
-        <v>44208</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
-        <v>44297</v>
+        <v>44300</v>
       </c>
       <c r="B248" s="3">
-        <v>44208</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
-        <v>44296</v>
+        <v>44299</v>
       </c>
       <c r="B249" s="3">
-        <v>44016</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
-        <v>44295</v>
+        <v>44298</v>
       </c>
       <c r="B250" s="3">
-        <v>41376</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
-        <v>44294</v>
+        <v>44297</v>
       </c>
       <c r="B251" s="3">
-        <v>38445</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
-        <v>44293</v>
+        <v>44296</v>
       </c>
       <c r="B252" s="3">
-        <v>35475</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
-        <v>44292</v>
+        <v>44295</v>
       </c>
       <c r="B253" s="3">
-        <v>31795</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
-        <v>44291</v>
+        <v>44294</v>
       </c>
       <c r="B254" s="3">
-        <v>31212</v>
+        <v>38445</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
-        <v>44290</v>
+        <v>44293</v>
       </c>
       <c r="B255" s="3">
-        <v>31212</v>
+        <v>35475</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
-        <v>44289</v>
+        <v>44292</v>
       </c>
       <c r="B256" s="3">
-        <v>30383</v>
+        <v>31795</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
-        <v>44288</v>
+        <v>44291</v>
       </c>
       <c r="B257" s="3">
-        <v>29796</v>
+        <v>31212</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B258" s="4"/>
+        <v>44290</v>
+      </c>
+      <c r="B258" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="259" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
-        <v>44286</v>
-      </c>
-      <c r="B259" s="4"/>
+        <v>44289</v>
+      </c>
+      <c r="B259" s="3">
+        <v>30383</v>
+      </c>
     </row>
     <row r="260" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
-        <v>44285</v>
-      </c>
-      <c r="B260" s="4"/>
+        <v>44288</v>
+      </c>
+      <c r="B260" s="3">
+        <v>29796</v>
+      </c>
     </row>
     <row r="261" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A261" s="2">
-        <v>44284</v>
+        <v>44287</v>
       </c>
       <c r="B261" s="4"/>
     </row>
     <row r="262" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
-        <v>44283</v>
+        <v>44286</v>
       </c>
       <c r="B262" s="4"/>
     </row>
     <row r="263" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A263" s="2">
-        <v>44282</v>
+        <v>44285</v>
       </c>
       <c r="B263" s="4"/>
     </row>
     <row r="264" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
-        <v>44281</v>
+        <v>44284</v>
       </c>
       <c r="B264" s="4"/>
     </row>
     <row r="265" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A265" s="2">
-        <v>44280</v>
+        <v>44283</v>
       </c>
       <c r="B265" s="4"/>
     </row>
     <row r="266" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
-        <v>44279</v>
+        <v>44282</v>
       </c>
       <c r="B266" s="4"/>
     </row>
     <row r="267" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A267" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B267" s="4"/>
+    </row>
+    <row r="268" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A268" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B268" s="4"/>
+    </row>
+    <row r="269" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A269" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B269" s="4"/>
+    </row>
+    <row r="270" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A270" s="2">
         <v>44278</v>
       </c>
-      <c r="B267" s="4"/>
+      <c r="B270" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{07D2E571-3882-CE4D-943E-FB5D21A4041C}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{49D6E36B-F0E2-6C42-B0C2-231D46C40C46}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated NZ-AU comparisons to 21 December
</commit_message>
<xml_diff>
--- a/data/nsw_second_doses.xlsx
+++ b/data/nsw_second_doses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Library/Mobile Documents/com~apple~CloudDocs/Work - iCloud/Workshop/nz-covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA73C90-709C-5F46-BD84-6392DB6D108A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6B7D5D-E33A-0746-88B2-14F50CBC7477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{FCB09FBB-56FF-1C46-98C1-A9F540B75259}"/>
   </bookViews>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BAE720-0FFD-AC44-A3E0-A012DA41F8A8}">
-  <dimension ref="A1:B270"/>
+  <dimension ref="A1:B274"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,2139 +447,2171 @@
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>44546</v>
+        <v>44550</v>
       </c>
       <c r="B2" s="3">
-        <v>6429276</v>
+        <v>6437227</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44545</v>
+        <v>44549</v>
       </c>
       <c r="B3" s="3">
-        <v>6426296</v>
+        <v>6436676</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>44544</v>
+        <v>44548</v>
       </c>
       <c r="B4" s="3">
-        <v>6422891</v>
+        <v>6435466</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>44543</v>
+        <v>44547</v>
       </c>
       <c r="B5" s="3">
-        <v>6419310</v>
+        <v>6432466</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>44542</v>
+        <v>44546</v>
       </c>
       <c r="B6" s="3">
-        <v>6418911</v>
+        <v>6429276</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>44541</v>
+        <v>44545</v>
       </c>
       <c r="B7" s="3">
-        <v>6417289</v>
+        <v>6426296</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>44540</v>
+        <v>44544</v>
       </c>
       <c r="B8" s="3">
-        <v>6413287</v>
+        <v>6422891</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>44539</v>
+        <v>44543</v>
       </c>
       <c r="B9" s="3">
-        <v>6409218</v>
+        <v>6419310</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>44538</v>
+        <v>44542</v>
       </c>
       <c r="B10" s="3">
-        <v>6405004</v>
+        <v>6418911</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>44537</v>
+        <v>44541</v>
       </c>
       <c r="B11" s="3">
-        <v>6400706</v>
+        <v>6417289</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>44536</v>
+        <v>44540</v>
       </c>
       <c r="B12" s="3">
-        <v>6396368</v>
+        <v>6413287</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>44535</v>
+        <v>44539</v>
       </c>
       <c r="B13" s="3">
-        <v>6395543</v>
+        <v>6409218</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>44534</v>
+        <v>44538</v>
       </c>
       <c r="B14" s="3">
-        <v>6393476</v>
+        <v>6405004</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>44533</v>
+        <v>44537</v>
       </c>
       <c r="B15" s="3">
-        <v>6387955</v>
+        <v>6400706</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>44532</v>
+        <v>44536</v>
       </c>
       <c r="B16" s="3">
-        <v>6383068</v>
+        <v>6396368</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>44531</v>
+        <v>44535</v>
       </c>
       <c r="B17" s="3">
-        <v>6378225</v>
+        <v>6395543</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>44530</v>
+        <v>44534</v>
       </c>
       <c r="B18" s="3">
-        <v>6372197</v>
+        <v>6393476</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>44529</v>
+        <v>44533</v>
       </c>
       <c r="B19" s="3">
-        <v>6366060</v>
+        <v>6387955</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>44528</v>
+        <v>44532</v>
       </c>
       <c r="B20" s="3">
-        <v>6365073</v>
+        <v>6383068</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>44527</v>
+        <v>44531</v>
       </c>
       <c r="B21" s="3">
-        <v>6362348</v>
+        <v>6378225</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>44526</v>
+        <v>44530</v>
       </c>
       <c r="B22" s="3">
-        <v>6355156</v>
+        <v>6372197</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>44525</v>
+        <v>44529</v>
       </c>
       <c r="B23" s="3">
-        <v>6348980</v>
+        <v>6366060</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>44524</v>
+        <v>44528</v>
       </c>
       <c r="B24" s="3">
-        <v>6341726</v>
+        <v>6365073</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>44523</v>
+        <v>44527</v>
       </c>
       <c r="B25" s="3">
-        <v>6334061</v>
+        <v>6362348</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>44522</v>
+        <v>44526</v>
       </c>
       <c r="B26" s="3">
-        <v>6325341</v>
+        <v>6355156</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>44521</v>
+        <v>44525</v>
       </c>
       <c r="B27" s="3">
-        <v>6324333</v>
+        <v>6348980</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>44520</v>
+        <v>44524</v>
       </c>
       <c r="B28" s="3">
-        <v>6320582</v>
+        <v>6341726</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>44519</v>
+        <v>44523</v>
       </c>
       <c r="B29" s="3">
-        <v>6311361</v>
+        <v>6334061</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>44518</v>
+        <v>44522</v>
       </c>
       <c r="B30" s="3">
-        <v>6301870</v>
+        <v>6325341</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>44517</v>
+        <v>44521</v>
       </c>
       <c r="B31" s="3">
-        <v>6291057</v>
+        <v>6324333</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>44516</v>
+        <v>44520</v>
       </c>
       <c r="B32" s="3">
-        <v>6279967</v>
+        <v>6320582</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>44515</v>
+        <v>44519</v>
       </c>
       <c r="B33" s="3">
-        <v>6268391</v>
+        <v>6311361</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>44514</v>
+        <v>44518</v>
       </c>
       <c r="B34" s="3">
-        <v>6265758</v>
+        <v>6301870</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>44513</v>
+        <v>44517</v>
       </c>
       <c r="B35" s="3">
-        <v>6259089</v>
+        <v>6291057</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>44512</v>
+        <v>44516</v>
       </c>
       <c r="B36" s="3">
-        <v>6243318</v>
+        <v>6279967</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>44511</v>
+        <v>44515</v>
       </c>
       <c r="B37" s="3">
-        <v>6226830</v>
+        <v>6268391</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>44510</v>
+        <v>44514</v>
       </c>
       <c r="B38" s="3">
-        <v>6210103</v>
+        <v>6265758</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>44509</v>
+        <v>44513</v>
       </c>
       <c r="B39" s="3">
-        <v>6192099</v>
+        <v>6259089</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>44508</v>
+        <v>44512</v>
       </c>
       <c r="B40" s="3">
-        <v>6172372</v>
+        <v>6243318</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>44507</v>
+        <v>44511</v>
       </c>
       <c r="B41" s="3">
-        <v>6168060</v>
+        <v>6226830</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>44506</v>
+        <v>44510</v>
       </c>
       <c r="B42" s="3">
-        <v>6156414</v>
+        <v>6210103</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>44505</v>
+        <v>44509</v>
       </c>
       <c r="B43" s="3">
-        <v>6130474</v>
+        <v>6192099</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>44504</v>
+        <v>44508</v>
       </c>
       <c r="B44" s="3">
-        <v>6105744</v>
+        <v>6172372</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44503</v>
+        <v>44507</v>
       </c>
       <c r="B45" s="3">
-        <v>6077355</v>
+        <v>6168060</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>44502</v>
+        <v>44506</v>
       </c>
       <c r="B46" s="3">
-        <v>6046074</v>
+        <v>6156414</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>44501</v>
+        <v>44505</v>
       </c>
       <c r="B47" s="3">
-        <v>6009574</v>
+        <v>6130474</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>44500</v>
+        <v>44504</v>
       </c>
       <c r="B48" s="3">
-        <v>5999926</v>
+        <v>6105744</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>44499</v>
+        <v>44503</v>
       </c>
       <c r="B49" s="3">
-        <v>5977973</v>
+        <v>6077355</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>44498</v>
+        <v>44502</v>
       </c>
       <c r="B50" s="3">
-        <v>5938861</v>
+        <v>6046074</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>44497</v>
+        <v>44501</v>
       </c>
       <c r="B51" s="3">
-        <v>5898147</v>
+        <v>6009574</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>44496</v>
+        <v>44500</v>
       </c>
       <c r="B52" s="3">
-        <v>5858123</v>
+        <v>5999926</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>44495</v>
+        <v>44499</v>
       </c>
       <c r="B53" s="3">
-        <v>5818705</v>
+        <v>5977973</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>44494</v>
+        <v>44498</v>
       </c>
       <c r="B54" s="3">
-        <v>5780737</v>
+        <v>5938861</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>44493</v>
+        <v>44497</v>
       </c>
       <c r="B55" s="3">
-        <v>5766748</v>
+        <v>5898147</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>44492</v>
+        <v>44496</v>
       </c>
       <c r="B56" s="3">
-        <v>5732872</v>
+        <v>5858123</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>44491</v>
+        <v>44495</v>
       </c>
       <c r="B57" s="3">
-        <v>5677232</v>
+        <v>5818705</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>44490</v>
+        <v>44494</v>
       </c>
       <c r="B58" s="3">
-        <v>5621660</v>
+        <v>5780737</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>44489</v>
+        <v>44493</v>
       </c>
       <c r="B59" s="3">
-        <v>5565441</v>
+        <v>5766748</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>44488</v>
+        <v>44492</v>
       </c>
       <c r="B60" s="3">
-        <v>5506563</v>
+        <v>5732872</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>44487</v>
+        <v>44491</v>
       </c>
       <c r="B61" s="3">
-        <v>5440365</v>
+        <v>5677232</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>44486</v>
+        <v>44490</v>
       </c>
       <c r="B62" s="3">
-        <v>5405628</v>
+        <v>5621660</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>44485</v>
+        <v>44489</v>
       </c>
       <c r="B63" s="3">
-        <v>5364911</v>
+        <v>5565441</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>44484</v>
+        <v>44488</v>
       </c>
       <c r="B64" s="3">
-        <v>5288225</v>
+        <v>5506563</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>44483</v>
+        <v>44487</v>
       </c>
       <c r="B65" s="3">
-        <v>5207377</v>
+        <v>5440365</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>44482</v>
+        <v>44486</v>
       </c>
       <c r="B66" s="3">
-        <v>5116994</v>
+        <v>5405628</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>44481</v>
+        <v>44485</v>
       </c>
       <c r="B67" s="3">
-        <v>5018535</v>
+        <v>5364911</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>44480</v>
+        <v>44484</v>
       </c>
       <c r="B68" s="3">
-        <v>4925635</v>
+        <v>5288225</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>44479</v>
+        <v>44483</v>
       </c>
       <c r="B69" s="3">
-        <v>4890800</v>
+        <v>5207377</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>44478</v>
+        <v>44482</v>
       </c>
       <c r="B70" s="3">
-        <v>4831173</v>
+        <v>5116994</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>44477</v>
+        <v>44481</v>
       </c>
       <c r="B71" s="3">
-        <v>4738793</v>
+        <v>5018535</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>44476</v>
+        <v>44480</v>
       </c>
       <c r="B72" s="3">
-        <v>4653723</v>
+        <v>4925635</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>44475</v>
+        <v>44479</v>
       </c>
       <c r="B73" s="3">
-        <v>4567214</v>
+        <v>4890800</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>44474</v>
+        <v>44478</v>
       </c>
       <c r="B74" s="3">
-        <v>4465060</v>
+        <v>4831173</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>44473</v>
+        <v>44477</v>
       </c>
       <c r="B75" s="3">
-        <v>4449546</v>
+        <v>4738793</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>44472</v>
+        <v>44476</v>
       </c>
       <c r="B76" s="3">
-        <v>4428121</v>
+        <v>4653723</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>44471</v>
+        <v>44475</v>
       </c>
       <c r="B77" s="3">
-        <v>4384051</v>
+        <v>4567214</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>44470</v>
+        <v>44474</v>
       </c>
       <c r="B78" s="3">
-        <v>4297900</v>
+        <v>4465060</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>44469</v>
+        <v>44473</v>
       </c>
       <c r="B79" s="3">
-        <v>4218516</v>
+        <v>4449546</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>44468</v>
+        <v>44472</v>
       </c>
       <c r="B80" s="3">
-        <v>4145673</v>
+        <v>4428121</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>44467</v>
+        <v>44471</v>
       </c>
       <c r="B81" s="3">
-        <v>4060612</v>
+        <v>4384051</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>44466</v>
+        <v>44470</v>
       </c>
       <c r="B82" s="3">
-        <v>3979094</v>
+        <v>4297900</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>44465</v>
+        <v>44469</v>
       </c>
       <c r="B83" s="3">
-        <v>3953132</v>
+        <v>4218516</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>44464</v>
+        <v>44468</v>
       </c>
       <c r="B84" s="3">
-        <v>3898564</v>
+        <v>4145673</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>44463</v>
+        <v>44467</v>
       </c>
       <c r="B85" s="3">
-        <v>3804258</v>
+        <v>4060612</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>44462</v>
+        <v>44466</v>
       </c>
       <c r="B86" s="3">
-        <v>3724979</v>
+        <v>3979094</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>44461</v>
+        <v>44465</v>
       </c>
       <c r="B87" s="3">
-        <v>3646849</v>
+        <v>3953132</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>44460</v>
+        <v>44464</v>
       </c>
       <c r="B88" s="3">
-        <v>3563962</v>
+        <v>3898564</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>44459</v>
+        <v>44463</v>
       </c>
       <c r="B89" s="3">
-        <v>3487539</v>
+        <v>3804258</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>44458</v>
+        <v>44462</v>
       </c>
       <c r="B90" s="3">
-        <v>3461082</v>
+        <v>3724979</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>44457</v>
+        <v>44461</v>
       </c>
       <c r="B91" s="3">
-        <v>3412016</v>
+        <v>3646849</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>44456</v>
+        <v>44460</v>
       </c>
       <c r="B92" s="3">
-        <v>3323936</v>
+        <v>3563962</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>44455</v>
+        <v>44459</v>
       </c>
       <c r="B93" s="3">
-        <v>3259323</v>
+        <v>3487539</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>44454</v>
+        <v>44458</v>
       </c>
       <c r="B94" s="3">
-        <v>3189070</v>
+        <v>3461082</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>44453</v>
+        <v>44457</v>
       </c>
       <c r="B95" s="3">
-        <v>3123699</v>
+        <v>3412016</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>44452</v>
+        <v>44456</v>
       </c>
       <c r="B96" s="3">
-        <v>3051925</v>
+        <v>3323936</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>44451</v>
+        <v>44455</v>
       </c>
       <c r="B97" s="3">
-        <v>3031072</v>
+        <v>3259323</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>44450</v>
+        <v>44454</v>
       </c>
       <c r="B98" s="3">
-        <v>2992899</v>
+        <v>3189070</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>44449</v>
+        <v>44453</v>
       </c>
       <c r="B99" s="3">
-        <v>2924263</v>
+        <v>3123699</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>44448</v>
+        <v>44452</v>
       </c>
       <c r="B100" s="3">
-        <v>2860253</v>
+        <v>3051925</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>44447</v>
+        <v>44451</v>
       </c>
       <c r="B101" s="3">
-        <v>2802011</v>
+        <v>3031072</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>44446</v>
+        <v>44450</v>
       </c>
       <c r="B102" s="3">
-        <v>2743498</v>
+        <v>2992899</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>44445</v>
+        <v>44449</v>
       </c>
       <c r="B103" s="3">
-        <v>2692904</v>
+        <v>2924263</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>44444</v>
+        <v>44448</v>
       </c>
       <c r="B104" s="3">
-        <v>2678906</v>
+        <v>2860253</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>44443</v>
+        <v>44447</v>
       </c>
       <c r="B105" s="3">
-        <v>2644865</v>
+        <v>2802011</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>44442</v>
+        <v>44446</v>
       </c>
       <c r="B106" s="3">
-        <v>2590966</v>
+        <v>2743498</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>44441</v>
+        <v>44445</v>
       </c>
       <c r="B107" s="3">
-        <v>2539287</v>
+        <v>2692904</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>44440</v>
+        <v>44444</v>
       </c>
       <c r="B108" s="3">
-        <v>2484199</v>
+        <v>2678906</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>44439</v>
+        <v>44443</v>
       </c>
       <c r="B109" s="3">
-        <v>2433592</v>
+        <v>2644865</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>44438</v>
+        <v>44442</v>
       </c>
       <c r="B110" s="3">
-        <v>2372417</v>
+        <v>2590966</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>44437</v>
+        <v>44441</v>
       </c>
       <c r="B111" s="3">
-        <v>2353563</v>
+        <v>2539287</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>44436</v>
+        <v>44440</v>
       </c>
       <c r="B112" s="3">
-        <v>2326130</v>
+        <v>2484199</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>44435</v>
+        <v>44439</v>
       </c>
       <c r="B113" s="3">
-        <v>2273984</v>
+        <v>2433592</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>44434</v>
+        <v>44438</v>
       </c>
       <c r="B114" s="3">
-        <v>2218458</v>
+        <v>2372417</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>44433</v>
+        <v>44437</v>
       </c>
       <c r="B115" s="3">
-        <v>2163192</v>
+        <v>2353563</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>44432</v>
+        <v>44436</v>
       </c>
       <c r="B116" s="3">
-        <v>2112611</v>
+        <v>2326130</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>44431</v>
+        <v>44435</v>
       </c>
       <c r="B117" s="3">
-        <v>2066915</v>
+        <v>2273984</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>44430</v>
+        <v>44434</v>
       </c>
       <c r="B118" s="3">
-        <v>2052364</v>
+        <v>2218458</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>44429</v>
+        <v>44433</v>
       </c>
       <c r="B119" s="3">
-        <v>2022928</v>
+        <v>2163192</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>44428</v>
+        <v>44432</v>
       </c>
       <c r="B120" s="3">
-        <v>1973224</v>
+        <v>2112611</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>44427</v>
+        <v>44431</v>
       </c>
       <c r="B121" s="3">
-        <v>1924839</v>
+        <v>2066915</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>44426</v>
+        <v>44430</v>
       </c>
       <c r="B122" s="3">
-        <v>1871458</v>
+        <v>2052364</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>44425</v>
+        <v>44429</v>
       </c>
       <c r="B123" s="3">
-        <v>1826165</v>
+        <v>2022928</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>44424</v>
+        <v>44428</v>
       </c>
       <c r="B124" s="3">
-        <v>1781578</v>
+        <v>1973224</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>44423</v>
+        <v>44427</v>
       </c>
       <c r="B125" s="3">
-        <v>1767176</v>
+        <v>1924839</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>44422</v>
+        <v>44426</v>
       </c>
       <c r="B126" s="3">
-        <v>1742669</v>
+        <v>1871458</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>44421</v>
+        <v>44425</v>
       </c>
       <c r="B127" s="3">
-        <v>1693577</v>
+        <v>1826165</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>44420</v>
+        <v>44424</v>
       </c>
       <c r="B128" s="3">
-        <v>1645077</v>
+        <v>1781578</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>44419</v>
+        <v>44423</v>
       </c>
       <c r="B129" s="3">
-        <v>1599438</v>
+        <v>1767176</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>44418</v>
+        <v>44422</v>
       </c>
       <c r="B130" s="3">
-        <v>1548545</v>
+        <v>1742669</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>44417</v>
+        <v>44421</v>
       </c>
       <c r="B131" s="3">
-        <v>1510648</v>
+        <v>1693577</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>44416</v>
+        <v>44420</v>
       </c>
       <c r="B132" s="3">
-        <v>1501249</v>
+        <v>1645077</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>44415</v>
+        <v>44419</v>
       </c>
       <c r="B133" s="3">
-        <v>1463495</v>
+        <v>1599438</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>44414</v>
+        <v>44418</v>
       </c>
       <c r="B134" s="3">
-        <v>1423185</v>
+        <v>1548545</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>44413</v>
+        <v>44417</v>
       </c>
       <c r="B135" s="3">
-        <v>1381481</v>
+        <v>1510648</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>44412</v>
+        <v>44416</v>
       </c>
       <c r="B136" s="3">
-        <v>1342211</v>
+        <v>1501249</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>44411</v>
+        <v>44415</v>
       </c>
       <c r="B137" s="3">
-        <v>1300394</v>
+        <v>1463495</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>44410</v>
+        <v>44414</v>
       </c>
       <c r="B138" s="3">
-        <v>1265839</v>
+        <v>1423185</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>44409</v>
+        <v>44413</v>
       </c>
       <c r="B139" s="3">
-        <v>1252304</v>
+        <v>1381481</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>44408</v>
+        <v>44412</v>
       </c>
       <c r="B140" s="3">
-        <v>1228845</v>
+        <v>1342211</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>44407</v>
+        <v>44411</v>
       </c>
       <c r="B141" s="3">
-        <v>1190942</v>
+        <v>1300394</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>44406</v>
+        <v>44410</v>
       </c>
       <c r="B142" s="3">
-        <v>1156321</v>
+        <v>1265839</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>44405</v>
+        <v>44409</v>
       </c>
       <c r="B143" s="3">
-        <v>1108405</v>
+        <v>1252304</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>44404</v>
+        <v>44408</v>
       </c>
       <c r="B144" s="3">
-        <v>1071895</v>
+        <v>1228845</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>44403</v>
+        <v>44407</v>
       </c>
       <c r="B145" s="3">
-        <v>1045515</v>
+        <v>1190942</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
-        <v>44402</v>
+        <v>44406</v>
       </c>
       <c r="B146" s="3">
-        <v>1034280</v>
+        <v>1156321</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>44401</v>
+        <v>44405</v>
       </c>
       <c r="B147" s="3">
-        <v>1012939</v>
+        <v>1108405</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>44400</v>
+        <v>44404</v>
       </c>
       <c r="B148" s="3">
-        <v>982170</v>
+        <v>1071895</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>44399</v>
+        <v>44403</v>
       </c>
       <c r="B149" s="3">
-        <v>948667</v>
+        <v>1045515</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
-        <v>44398</v>
+        <v>44402</v>
       </c>
       <c r="B150" s="3">
-        <v>912940</v>
+        <v>1034280</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
-        <v>44397</v>
+        <v>44401</v>
       </c>
       <c r="B151" s="3">
-        <v>882844</v>
+        <v>1012939</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
-        <v>44396</v>
+        <v>44400</v>
       </c>
       <c r="B152" s="3">
-        <v>854625</v>
+        <v>982170</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
-        <v>44395</v>
+        <v>44399</v>
       </c>
       <c r="B153" s="3">
-        <v>846261</v>
+        <v>948667</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A154" s="2">
-        <v>44394</v>
+        <v>44398</v>
       </c>
       <c r="B154" s="3">
-        <v>830856</v>
+        <v>912940</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
-        <v>44393</v>
+        <v>44397</v>
       </c>
       <c r="B155" s="3">
-        <v>801520</v>
+        <v>882844</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A156" s="2">
-        <v>44392</v>
+        <v>44396</v>
       </c>
       <c r="B156" s="3">
-        <v>769552</v>
+        <v>854625</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
-        <v>44391</v>
+        <v>44395</v>
       </c>
       <c r="B157" s="3">
-        <v>741075</v>
+        <v>846261</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
-        <v>44390</v>
+        <v>44394</v>
       </c>
       <c r="B158" s="3">
-        <v>710714</v>
+        <v>830856</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
-        <v>44389</v>
+        <v>44393</v>
       </c>
       <c r="B159" s="3">
-        <v>686408</v>
+        <v>801520</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
-        <v>44388</v>
+        <v>44392</v>
       </c>
       <c r="B160" s="3">
-        <v>683667</v>
+        <v>769552</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A161" s="2">
-        <v>44387</v>
+        <v>44391</v>
       </c>
       <c r="B161" s="3">
-        <v>671858</v>
+        <v>741075</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
-        <v>44386</v>
+        <v>44390</v>
       </c>
       <c r="B162" s="3">
-        <v>651446</v>
+        <v>710714</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A163" s="2">
-        <v>44385</v>
+        <v>44389</v>
       </c>
       <c r="B163" s="3">
-        <v>629961</v>
+        <v>686408</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
-        <v>44384</v>
+        <v>44388</v>
       </c>
       <c r="B164" s="3">
-        <v>609108</v>
+        <v>683667</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
-        <v>44383</v>
+        <v>44387</v>
       </c>
       <c r="B165" s="3">
-        <v>586674</v>
+        <v>671858</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A166" s="2">
-        <v>44382</v>
+        <v>44386</v>
       </c>
       <c r="B166" s="3">
-        <v>567316</v>
+        <v>651446</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
-        <v>44381</v>
+        <v>44385</v>
       </c>
       <c r="B167" s="3">
-        <v>564930</v>
+        <v>629961</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A168" s="2">
-        <v>44380</v>
+        <v>44384</v>
       </c>
       <c r="B168" s="3">
-        <v>554057</v>
+        <v>609108</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
-        <v>44379</v>
+        <v>44383</v>
       </c>
       <c r="B169" s="3">
-        <v>534493</v>
+        <v>586674</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
-        <v>44378</v>
+        <v>44382</v>
       </c>
       <c r="B170" s="3">
-        <v>471176</v>
+        <v>567316</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A171" s="2">
-        <v>44377</v>
+        <v>44381</v>
       </c>
       <c r="B171" s="3">
-        <v>471176</v>
+        <v>564930</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
-        <v>44376</v>
+        <v>44380</v>
       </c>
       <c r="B172" s="3">
-        <v>463624</v>
+        <v>554057</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A173" s="2">
-        <v>44375</v>
+        <v>44379</v>
       </c>
       <c r="B173" s="3">
-        <v>396652</v>
+        <v>534493</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
-        <v>44374</v>
+        <v>44378</v>
       </c>
       <c r="B174" s="3">
-        <v>396246</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A175" s="2">
-        <v>44373</v>
+        <v>44377</v>
       </c>
       <c r="B175" s="3">
-        <v>392527</v>
+        <v>471176</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
-        <v>44372</v>
+        <v>44376</v>
       </c>
       <c r="B176" s="3">
-        <v>385092</v>
+        <v>463624</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
-        <v>44371</v>
+        <v>44375</v>
       </c>
       <c r="B177" s="3">
-        <v>376276</v>
+        <v>396652</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A178" s="2">
-        <v>44370</v>
+        <v>44374</v>
       </c>
       <c r="B178" s="3">
-        <v>366660</v>
+        <v>396246</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
-        <v>44369</v>
+        <v>44373</v>
       </c>
       <c r="B179" s="3">
-        <v>357767</v>
+        <v>392527</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A180" s="2">
-        <v>44368</v>
+        <v>44372</v>
       </c>
       <c r="B180" s="3">
-        <v>294981</v>
+        <v>385092</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
-        <v>44367</v>
+        <v>44371</v>
       </c>
       <c r="B181" s="3">
-        <v>294965</v>
+        <v>376276</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
-        <v>44366</v>
+        <v>44370</v>
       </c>
       <c r="B182" s="3">
-        <v>289941</v>
+        <v>366660</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A183" s="2">
-        <v>44365</v>
+        <v>44369</v>
       </c>
       <c r="B183" s="3">
-        <v>279418</v>
+        <v>357767</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
-        <v>44364</v>
+        <v>44368</v>
       </c>
       <c r="B184" s="3">
-        <v>269824</v>
+        <v>294981</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A185" s="2">
-        <v>44363</v>
+        <v>44367</v>
       </c>
       <c r="B185" s="3">
-        <v>259437</v>
+        <v>294965</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
-        <v>44362</v>
+        <v>44366</v>
       </c>
       <c r="B186" s="3">
-        <v>237250</v>
+        <v>289941</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A187" s="2">
-        <v>44361</v>
+        <v>44365</v>
       </c>
       <c r="B187" s="3">
-        <v>237250</v>
+        <v>279418</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
-        <v>44360</v>
+        <v>44364</v>
       </c>
       <c r="B188" s="3">
-        <v>237250</v>
+        <v>269824</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
-        <v>44359</v>
+        <v>44363</v>
       </c>
       <c r="B189" s="3">
-        <v>232335</v>
+        <v>259437</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A190" s="2">
-        <v>44358</v>
+        <v>44362</v>
       </c>
       <c r="B190" s="3">
-        <v>222807</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
-        <v>44357</v>
+        <v>44361</v>
       </c>
       <c r="B191" s="3">
-        <v>213686</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A192" s="2">
-        <v>44356</v>
+        <v>44360</v>
       </c>
       <c r="B192" s="3">
-        <v>213686</v>
+        <v>237250</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
-        <v>44355</v>
+        <v>44359</v>
       </c>
       <c r="B193" s="3">
-        <v>204595</v>
+        <v>232335</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
-        <v>44354</v>
+        <v>44358</v>
       </c>
       <c r="B194" s="3">
-        <v>180397</v>
+        <v>222807</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A195" s="2">
-        <v>44353</v>
+        <v>44357</v>
       </c>
       <c r="B195" s="3">
-        <v>180397</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
-        <v>44352</v>
+        <v>44356</v>
       </c>
       <c r="B196" s="3">
-        <v>179477</v>
+        <v>213686</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A197" s="2">
-        <v>44351</v>
+        <v>44355</v>
       </c>
       <c r="B197" s="3">
-        <v>175030</v>
+        <v>204595</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
-        <v>44350</v>
+        <v>44354</v>
       </c>
       <c r="B198" s="3">
-        <v>170669</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A199" s="2">
-        <v>44349</v>
+        <v>44353</v>
       </c>
       <c r="B199" s="3">
-        <v>167075</v>
+        <v>180397</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
-        <v>44348</v>
+        <v>44352</v>
       </c>
       <c r="B200" s="3">
-        <v>156333</v>
+        <v>179477</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A201" s="2">
-        <v>44347</v>
+        <v>44351</v>
       </c>
       <c r="B201" s="3">
-        <v>153886</v>
+        <v>175030</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A202" s="2">
-        <v>44346</v>
+        <v>44350</v>
       </c>
       <c r="B202" s="3">
-        <v>153886</v>
+        <v>170669</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A203" s="2">
-        <v>44345</v>
+        <v>44349</v>
       </c>
       <c r="B203" s="3">
-        <v>153886</v>
+        <v>167075</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A204" s="2">
-        <v>44344</v>
+        <v>44348</v>
       </c>
       <c r="B204" s="3">
-        <v>153886</v>
+        <v>156333</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
-        <v>44343</v>
+        <v>44347</v>
       </c>
       <c r="B205" s="3">
-        <v>150552</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A206" s="2">
-        <v>44342</v>
+        <v>44346</v>
       </c>
       <c r="B206" s="3">
-        <v>145341</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A207" s="2">
-        <v>44341</v>
+        <v>44345</v>
       </c>
       <c r="B207" s="3">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A208" s="2">
-        <v>44340</v>
+        <v>44344</v>
       </c>
       <c r="B208" s="3">
-        <v>125810</v>
+        <v>153886</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A209" s="2">
-        <v>44339</v>
+        <v>44343</v>
       </c>
       <c r="B209" s="3">
-        <v>96745</v>
+        <v>150552</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A210" s="2">
-        <v>44338</v>
+        <v>44342</v>
       </c>
       <c r="B210" s="3">
-        <v>96266</v>
+        <v>145341</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A211" s="2">
-        <v>44337</v>
+        <v>44341</v>
       </c>
       <c r="B211" s="3">
-        <v>93860</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A212" s="2">
-        <v>44336</v>
+        <v>44340</v>
       </c>
       <c r="B212" s="3">
-        <v>91297</v>
+        <v>125810</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A213" s="2">
-        <v>44335</v>
+        <v>44339</v>
       </c>
       <c r="B213" s="3">
-        <v>89049</v>
+        <v>96745</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A214" s="2">
-        <v>44334</v>
+        <v>44338</v>
       </c>
       <c r="B214" s="3">
-        <v>87045</v>
+        <v>96266</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A215" s="2">
-        <v>44333</v>
+        <v>44337</v>
       </c>
       <c r="B215" s="3">
-        <v>84963</v>
+        <v>93860</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A216" s="2">
-        <v>44332</v>
+        <v>44336</v>
       </c>
       <c r="B216" s="3">
-        <v>84963</v>
+        <v>91297</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A217" s="2">
-        <v>44331</v>
+        <v>44335</v>
       </c>
       <c r="B217" s="3">
-        <v>84474</v>
+        <v>89049</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A218" s="2">
-        <v>44330</v>
+        <v>44334</v>
       </c>
       <c r="B218" s="3">
-        <v>82774</v>
+        <v>87045</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A219" s="2">
-        <v>44329</v>
+        <v>44333</v>
       </c>
       <c r="B219" s="3">
-        <v>81457</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A220" s="2">
-        <v>44328</v>
+        <v>44332</v>
       </c>
       <c r="B220" s="3">
-        <v>80082</v>
+        <v>84963</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A221" s="2">
-        <v>44327</v>
+        <v>44331</v>
       </c>
       <c r="B221" s="3">
-        <v>78744</v>
+        <v>84474</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A222" s="2">
-        <v>44326</v>
+        <v>44330</v>
       </c>
       <c r="B222" s="3">
-        <v>77392</v>
+        <v>82774</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A223" s="2">
-        <v>44325</v>
+        <v>44329</v>
       </c>
       <c r="B223" s="3">
-        <v>77392</v>
+        <v>81457</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A224" s="2">
-        <v>44324</v>
+        <v>44328</v>
       </c>
       <c r="B224" s="3">
-        <v>76908</v>
+        <v>80082</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A225" s="2">
-        <v>44323</v>
+        <v>44327</v>
       </c>
       <c r="B225" s="3">
-        <v>75187</v>
+        <v>78744</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A226" s="2">
-        <v>44322</v>
+        <v>44326</v>
       </c>
       <c r="B226" s="3">
-        <v>73270</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A227" s="2">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B227" s="3">
-        <v>71767</v>
+        <v>77392</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A228" s="2">
-        <v>44320</v>
+        <v>44324</v>
       </c>
       <c r="B228" s="3">
-        <v>70039</v>
+        <v>76908</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A229" s="2">
-        <v>44319</v>
+        <v>44323</v>
       </c>
       <c r="B229" s="3">
-        <v>68656</v>
+        <v>75187</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A230" s="2">
-        <v>44318</v>
+        <v>44322</v>
       </c>
       <c r="B230" s="3">
-        <v>68656</v>
+        <v>73270</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A231" s="2">
-        <v>44317</v>
+        <v>44321</v>
       </c>
       <c r="B231" s="3">
-        <v>68472</v>
+        <v>71767</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A232" s="2">
-        <v>44316</v>
+        <v>44320</v>
       </c>
       <c r="B232" s="3">
-        <v>67149</v>
+        <v>70039</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A233" s="2">
-        <v>44315</v>
+        <v>44319</v>
       </c>
       <c r="B233" s="3">
-        <v>65948</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A234" s="2">
-        <v>44314</v>
+        <v>44318</v>
       </c>
       <c r="B234" s="3">
-        <v>64910</v>
+        <v>68656</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A235" s="2">
-        <v>44313</v>
+        <v>44317</v>
       </c>
       <c r="B235" s="3">
-        <v>63944</v>
+        <v>68472</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A236" s="2">
-        <v>44312</v>
+        <v>44316</v>
       </c>
       <c r="B236" s="3">
-        <v>63537</v>
+        <v>67149</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A237" s="2">
-        <v>44311</v>
+        <v>44315</v>
       </c>
       <c r="B237" s="3">
-        <v>63537</v>
+        <v>65948</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A238" s="2">
-        <v>44310</v>
+        <v>44314</v>
       </c>
       <c r="B238" s="3">
-        <v>63317</v>
+        <v>64910</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A239" s="2">
-        <v>44309</v>
+        <v>44313</v>
       </c>
       <c r="B239" s="3">
-        <v>62491</v>
+        <v>63944</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A240" s="2">
-        <v>44308</v>
+        <v>44312</v>
       </c>
       <c r="B240" s="3">
-        <v>60582</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A241" s="2">
-        <v>44307</v>
+        <v>44311</v>
       </c>
       <c r="B241" s="3">
-        <v>58662</v>
+        <v>63537</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A242" s="2">
-        <v>44306</v>
+        <v>44310</v>
       </c>
       <c r="B242" s="3">
-        <v>54736</v>
+        <v>63317</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A243" s="2">
-        <v>44305</v>
+        <v>44309</v>
       </c>
       <c r="B243" s="3">
-        <v>54668</v>
+        <v>62491</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A244" s="2">
-        <v>44304</v>
+        <v>44308</v>
       </c>
       <c r="B244" s="3">
-        <v>54668</v>
+        <v>60582</v>
       </c>
     </row>
     <row r="245" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A245" s="2">
-        <v>44303</v>
+        <v>44307</v>
       </c>
       <c r="B245" s="3">
-        <v>54555</v>
+        <v>58662</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A246" s="2">
-        <v>44302</v>
+        <v>44306</v>
       </c>
       <c r="B246" s="3">
-        <v>52537</v>
+        <v>54736</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A247" s="2">
-        <v>44301</v>
+        <v>44305</v>
       </c>
       <c r="B247" s="3">
-        <v>50388</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A248" s="2">
-        <v>44300</v>
+        <v>44304</v>
       </c>
       <c r="B248" s="3">
-        <v>48482</v>
+        <v>54668</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A249" s="2">
-        <v>44299</v>
+        <v>44303</v>
       </c>
       <c r="B249" s="3">
-        <v>46400</v>
+        <v>54555</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A250" s="2">
-        <v>44298</v>
+        <v>44302</v>
       </c>
       <c r="B250" s="3">
-        <v>44208</v>
+        <v>52537</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A251" s="2">
-        <v>44297</v>
+        <v>44301</v>
       </c>
       <c r="B251" s="3">
-        <v>44208</v>
+        <v>50388</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A252" s="2">
-        <v>44296</v>
+        <v>44300</v>
       </c>
       <c r="B252" s="3">
-        <v>44016</v>
+        <v>48482</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A253" s="2">
-        <v>44295</v>
+        <v>44299</v>
       </c>
       <c r="B253" s="3">
-        <v>41376</v>
+        <v>46400</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A254" s="2">
-        <v>44294</v>
+        <v>44298</v>
       </c>
       <c r="B254" s="3">
-        <v>38445</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A255" s="2">
-        <v>44293</v>
+        <v>44297</v>
       </c>
       <c r="B255" s="3">
-        <v>35475</v>
+        <v>44208</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A256" s="2">
-        <v>44292</v>
+        <v>44296</v>
       </c>
       <c r="B256" s="3">
-        <v>31795</v>
+        <v>44016</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A257" s="2">
-        <v>44291</v>
+        <v>44295</v>
       </c>
       <c r="B257" s="3">
-        <v>31212</v>
+        <v>41376</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A258" s="2">
-        <v>44290</v>
+        <v>44294</v>
       </c>
       <c r="B258" s="3">
-        <v>31212</v>
+        <v>38445</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A259" s="2">
-        <v>44289</v>
+        <v>44293</v>
       </c>
       <c r="B259" s="3">
-        <v>30383</v>
+        <v>35475</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A260" s="2">
-        <v>44288</v>
+        <v>44292</v>
       </c>
       <c r="B260" s="3">
-        <v>29796</v>
+        <v>31795</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A261" s="2">
-        <v>44287</v>
-      </c>
-      <c r="B261" s="4"/>
+        <v>44291</v>
+      </c>
+      <c r="B261" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="262" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A262" s="2">
-        <v>44286</v>
-      </c>
-      <c r="B262" s="4"/>
+        <v>44290</v>
+      </c>
+      <c r="B262" s="3">
+        <v>31212</v>
+      </c>
     </row>
     <row r="263" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A263" s="2">
-        <v>44285</v>
-      </c>
-      <c r="B263" s="4"/>
+        <v>44289</v>
+      </c>
+      <c r="B263" s="3">
+        <v>30383</v>
+      </c>
     </row>
     <row r="264" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A264" s="2">
-        <v>44284</v>
-      </c>
-      <c r="B264" s="4"/>
+        <v>44288</v>
+      </c>
+      <c r="B264" s="3">
+        <v>29796</v>
+      </c>
     </row>
     <row r="265" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A265" s="2">
-        <v>44283</v>
+        <v>44287</v>
       </c>
       <c r="B265" s="4"/>
     </row>
     <row r="266" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A266" s="2">
-        <v>44282</v>
+        <v>44286</v>
       </c>
       <c r="B266" s="4"/>
     </row>
     <row r="267" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A267" s="2">
-        <v>44281</v>
+        <v>44285</v>
       </c>
       <c r="B267" s="4"/>
     </row>
     <row r="268" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A268" s="2">
-        <v>44280</v>
+        <v>44284</v>
       </c>
       <c r="B268" s="4"/>
     </row>
     <row r="269" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A269" s="2">
-        <v>44279</v>
+        <v>44283</v>
       </c>
       <c r="B269" s="4"/>
     </row>
     <row r="270" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A270" s="2">
+        <v>44282</v>
+      </c>
+      <c r="B270" s="4"/>
+    </row>
+    <row r="271" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A271" s="2">
+        <v>44281</v>
+      </c>
+      <c r="B271" s="4"/>
+    </row>
+    <row r="272" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A272" s="2">
+        <v>44280</v>
+      </c>
+      <c r="B272" s="4"/>
+    </row>
+    <row r="273" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A273" s="2">
+        <v>44279</v>
+      </c>
+      <c r="B273" s="4"/>
+    </row>
+    <row r="274" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A274" s="2">
         <v>44278</v>
       </c>
-      <c r="B270" s="4"/>
+      <c r="B274" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{49D6E36B-F0E2-6C42-B0C2-231D46C40C46}"/>
+    <hyperlink ref="A1" r:id="rId1" display="https://covidlive.com.au/report/daily-vaccinations-people/nsw?sort=date" xr:uid="{8DAF23E4-9EFB-FF4C-8BA1-970594C6AF28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>